<commit_message>
Help pages, zero variance handling, refactoring, more input formats
</commit_message>
<xml_diff>
--- a/translations/source.xlsx
+++ b/translations/source.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22325"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/e6c7874704bc5dfb/Documents/R Studio/DataSuite/translations/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="110" documentId="8_{D77EC384-F39F-4BA6-8963-4B8AF986F7DE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{A19794B1-9D64-43F3-A115-D2E7D24B473D}"/>
+  <xr:revisionPtr revIDLastSave="201" documentId="8_{D77EC384-F39F-4BA6-8963-4B8AF986F7DE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{67AB39D3-0ABE-46DA-9125-C78F304DE3F9}"/>
   <bookViews>
-    <workbookView xWindow="5542" yWindow="960" windowWidth="18623" windowHeight="15240" xr2:uid="{BD840C99-A56D-4EBC-B1B7-A6018ADC22A6}"/>
+    <workbookView xWindow="1837" yWindow="960" windowWidth="18623" windowHeight="15240" xr2:uid="{BD840C99-A56D-4EBC-B1B7-A6018ADC22A6}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="711" uniqueCount="464">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="777" uniqueCount="508">
   <si>
     <t>base</t>
   </si>
@@ -219,12 +219,6 @@
     <t>Dunn's secondary index</t>
   </si>
   <si>
-    <t>Выбирать оптимальную модель</t>
-  </si>
-  <si>
-    <t>Optimal model</t>
-  </si>
-  <si>
     <t>Выбор переменных для анализа</t>
   </si>
   <si>
@@ -255,24 +249,12 @@
     <t>psycho::n_factors conclusions:</t>
   </si>
   <si>
-    <t>Выводы:</t>
-  </si>
-  <si>
-    <t>Conclusions:</t>
-  </si>
-  <si>
     <t>График нагрузок</t>
   </si>
   <si>
     <t>Loadings plot</t>
   </si>
   <si>
-    <t>График осыпи</t>
-  </si>
-  <si>
-    <t>Scree plot</t>
-  </si>
-  <si>
     <t>График осыпи кластеров (по методу К-средних)</t>
   </si>
   <si>
@@ -408,12 +390,6 @@
     <t>Dunn index</t>
   </si>
   <si>
-    <t>Индекс Такера-Льюиса:</t>
-  </si>
-  <si>
-    <t>Tucker-Lewis Index:</t>
-  </si>
-  <si>
     <t>Индексы качества кластеризации</t>
   </si>
   <si>
@@ -528,18 +504,6 @@
     <t>Components</t>
   </si>
   <si>
-    <t>Корень квадратов остатков:</t>
-  </si>
-  <si>
-    <t>RMS:</t>
-  </si>
-  <si>
-    <t>Корень среднего квадрата ошибки аппроксимации:</t>
-  </si>
-  <si>
-    <t>RMSEA:</t>
-  </si>
-  <si>
     <t>Корреляционный анализ</t>
   </si>
   <si>
@@ -1426,6 +1390,174 @@
   </si>
   <si>
     <t>Reversed items</t>
+  </si>
+  <si>
+    <t>Автовыбор</t>
+  </si>
+  <si>
+    <t>Auto</t>
+  </si>
+  <si>
+    <t>Значимый p-уровень</t>
+  </si>
+  <si>
+    <t>Significant p-level</t>
+  </si>
+  <si>
+    <t>Настройки</t>
+  </si>
+  <si>
+    <t>Settings</t>
+  </si>
+  <si>
+    <t>Индекс Такера-Льюиса</t>
+  </si>
+  <si>
+    <t>Корень квадратов остатков</t>
+  </si>
+  <si>
+    <t>Корень среднего квадрата ошибки аппроксимации</t>
+  </si>
+  <si>
+    <t>RMSEA</t>
+  </si>
+  <si>
+    <t>RMS</t>
+  </si>
+  <si>
+    <t>Tucker-Lewis Index</t>
+  </si>
+  <si>
+    <t>Подбор количества факторов</t>
+  </si>
+  <si>
+    <t>Factor number selection</t>
+  </si>
+  <si>
+    <t>Отсекать нагрузки</t>
+  </si>
+  <si>
+    <t>Выделять нагрузки</t>
+  </si>
+  <si>
+    <t>Cut-off loadings</t>
+  </si>
+  <si>
+    <t>Highlight loadings</t>
+  </si>
+  <si>
+    <t>Общее</t>
+  </si>
+  <si>
+    <t>Альфа</t>
+  </si>
+  <si>
+    <t>Стандартизированная Альфа</t>
+  </si>
+  <si>
+    <t>Лямбда-6</t>
+  </si>
+  <si>
+    <t>Средняя корреляция</t>
+  </si>
+  <si>
+    <t>Сигнал/Шум</t>
+  </si>
+  <si>
+    <t>Стандартная ошибка Альфы</t>
+  </si>
+  <si>
+    <t>Медианная корреляция</t>
+  </si>
+  <si>
+    <t>Корреляция с общим</t>
+  </si>
+  <si>
+    <t>Корреляция с общим стандартизированная</t>
+  </si>
+  <si>
+    <t>Скорректированная корреляция с общим</t>
+  </si>
+  <si>
+    <t>Корреляция при отбросе</t>
+  </si>
+  <si>
+    <t>TOTAL</t>
+  </si>
+  <si>
+    <t>Alpha</t>
+  </si>
+  <si>
+    <t>G6</t>
+  </si>
+  <si>
+    <t>Mean correlation</t>
+  </si>
+  <si>
+    <t>Signal/Noise</t>
+  </si>
+  <si>
+    <t>Alpha Standard Error</t>
+  </si>
+  <si>
+    <t>Standardized Alpha</t>
+  </si>
+  <si>
+    <t>Median correlation</t>
+  </si>
+  <si>
+    <t>Correlation with total</t>
+  </si>
+  <si>
+    <t>Standardized correlation with total</t>
+  </si>
+  <si>
+    <t>Corrected correlation with total</t>
+  </si>
+  <si>
+    <t>Correlation if dropped</t>
+  </si>
+  <si>
+    <t>Статистика элементов</t>
+  </si>
+  <si>
+    <t>Item statistics</t>
+  </si>
+  <si>
+    <t>Оптимальные модели</t>
+  </si>
+  <si>
+    <t>Optimal models</t>
+  </si>
+  <si>
+    <t>Непараметрическая описательная статистика</t>
+  </si>
+  <si>
+    <t>Nonparametric descriptive statistics</t>
+  </si>
+  <si>
+    <t>Зависимые переменные</t>
+  </si>
+  <si>
+    <t>Dependent variables</t>
+  </si>
+  <si>
+    <t>Не выбраны зависимые переменные!</t>
+  </si>
+  <si>
+    <t>Dependent variables are not selected!</t>
+  </si>
+  <si>
+    <t>Следующие столбцы имели единственное значение и были устранены из анализа:</t>
+  </si>
+  <si>
+    <t>Following columns were removed from the analysis due to having no variance</t>
+  </si>
+  <si>
+    <t>В таблице данных нет столбцов с ненулевым разбросом значений</t>
+  </si>
+  <si>
+    <t>There are no non-zero-variance variables in data</t>
   </si>
 </sst>
 </file>
@@ -1783,17 +1915,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C853ECA4-158B-4D85-A448-9ECE56776B5F}">
-  <dimension ref="A1:C237"/>
+  <dimension ref="A1:C259"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A206" workbookViewId="0">
-      <selection activeCell="A237" sqref="A237"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="148.59765625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="116.1328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="16384" width="9.06640625" style="1"/>
+    <col min="1" max="1" width="85.59765625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="87.1328125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="145.9296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="9.06640625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.45">
@@ -1853,13 +1986,13 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A6" s="1" t="s">
-        <v>457</v>
+        <v>445</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>17</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>457</v>
+        <v>445</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.45">
@@ -1875,13 +2008,13 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A8" s="1" t="s">
-        <v>456</v>
+        <v>444</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>19</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>456</v>
+        <v>444</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.45">
@@ -1897,35 +2030,35 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A10" s="2" t="s">
-        <v>394</v>
+        <v>382</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>395</v>
+        <v>383</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>394</v>
+        <v>382</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A11" s="2" t="s">
-        <v>396</v>
+        <v>384</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>397</v>
+        <v>385</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>396</v>
+        <v>384</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A12" s="2" t="s">
-        <v>447</v>
+        <v>435</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>447</v>
+        <v>435</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.45">
@@ -2040,2372 +2173,2614 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A23" s="2" t="s">
-        <v>370</v>
+        <v>452</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>371</v>
+        <v>453</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>370</v>
+        <v>452</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A24" s="2" t="s">
-        <v>38</v>
+      <c r="A24" s="1" t="s">
+        <v>471</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="C24" s="3" t="s">
-        <v>38</v>
+        <v>483</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>471</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A25" s="2" t="s">
-        <v>7</v>
+        <v>358</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>8</v>
+        <v>359</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>7</v>
+        <v>358</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A26" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>448</v>
+        <v>39</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A27" s="2" t="s">
-        <v>41</v>
+        <v>7</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>42</v>
+        <v>8</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>41</v>
+        <v>7</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A28" s="2" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>44</v>
+        <v>436</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A29" s="2" t="s">
-        <v>398</v>
+        <v>41</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>399</v>
-      </c>
-      <c r="C29" s="2" t="s">
-        <v>398</v>
+        <v>42</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A30" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A31" s="2" t="s">
-        <v>47</v>
+        <v>386</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="C31" s="3" t="s">
-        <v>47</v>
+        <v>387</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>386</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A32" s="2" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A33" s="2" t="s">
-        <v>374</v>
+        <v>506</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>375</v>
+        <v>507</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>374</v>
+        <v>506</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A34" s="2" t="s">
-        <v>382</v>
+        <v>47</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>383</v>
-      </c>
-      <c r="C34" s="2" t="s">
-        <v>382</v>
+        <v>48</v>
+      </c>
+      <c r="C34" s="3" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A35" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A36" s="2" t="s">
-        <v>404</v>
+        <v>362</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>407</v>
+        <v>363</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>404</v>
+        <v>362</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A37" s="1" t="s">
-        <v>425</v>
+      <c r="A37" s="2" t="s">
+        <v>370</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>436</v>
-      </c>
-      <c r="C37" s="1" t="s">
-        <v>425</v>
+        <v>371</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>370</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A38" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A39" s="2" t="s">
-        <v>358</v>
+        <v>392</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>359</v>
-      </c>
-      <c r="C39" s="3" t="s">
-        <v>358</v>
+        <v>395</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>392</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A40" s="2" t="s">
-        <v>55</v>
+      <c r="A40" s="1" t="s">
+        <v>413</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="C40" s="3" t="s">
-        <v>55</v>
+        <v>424</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>413</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A41" s="1" t="s">
-        <v>420</v>
-      </c>
-      <c r="B41" s="1" t="s">
-        <v>438</v>
-      </c>
-      <c r="C41" s="1" t="s">
-        <v>420</v>
+      <c r="A41" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="C41" s="3" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A42" s="2" t="s">
-        <v>57</v>
+        <v>346</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>58</v>
+        <v>347</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>57</v>
+        <v>346</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A43" s="2" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A44" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="B44" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="C44" s="3" t="s">
-        <v>61</v>
+      <c r="A44" s="1" t="s">
+        <v>408</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>426</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>408</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A45" s="2" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A46" s="2" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="C46" s="2" t="s">
-        <v>65</v>
+        <v>60</v>
+      </c>
+      <c r="C46" s="3" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A47" s="2" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="C47" s="2" t="s">
-        <v>67</v>
+        <v>62</v>
+      </c>
+      <c r="C47" s="3" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A48" s="2" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="C48" s="3" t="s">
-        <v>69</v>
+        <v>64</v>
+      </c>
+      <c r="C48" s="2" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A49" s="2" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="C49" s="3" t="s">
-        <v>71</v>
+        <v>66</v>
+      </c>
+      <c r="C49" s="2" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A50" s="2" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="C50" s="2" t="s">
-        <v>73</v>
+        <v>68</v>
+      </c>
+      <c r="C50" s="3" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A51" s="2" t="s">
-        <v>350</v>
+        <v>69</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>351</v>
+        <v>70</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>350</v>
+        <v>69</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A52" s="2" t="s">
-        <v>362</v>
+        <v>467</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>363</v>
+        <v>469</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>362</v>
+        <v>467</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A53" s="1" t="s">
-        <v>450</v>
-      </c>
-      <c r="B53" s="1" t="s">
-        <v>451</v>
-      </c>
-      <c r="C53" s="1" t="s">
-        <v>450</v>
+      <c r="A53" s="2" t="s">
+        <v>338</v>
+      </c>
+      <c r="B53" s="2" t="s">
+        <v>339</v>
+      </c>
+      <c r="C53" s="3" t="s">
+        <v>338</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A54" s="2" t="s">
-        <v>75</v>
+        <v>350</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="C54" s="3" t="s">
-        <v>75</v>
+        <v>351</v>
+      </c>
+      <c r="C54" s="2" t="s">
+        <v>350</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A55" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="B55" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="C55" s="2" t="s">
-        <v>77</v>
+      <c r="A55" s="1" t="s">
+        <v>438</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>439</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>438</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A56" s="2" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="C56" s="3" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A57" s="2" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="C57" s="3" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A58" s="2" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="C58" s="3" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A59" s="2" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="C59" s="3" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A60" s="2" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
       <c r="C60" s="3" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A61" s="2" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="C61" s="2" t="s">
-        <v>89</v>
+        <v>82</v>
+      </c>
+      <c r="C61" s="3" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A62" s="2" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="C62" s="3" t="s">
-        <v>91</v>
+        <v>84</v>
+      </c>
+      <c r="C62" s="2" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A63" s="2" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="C63" s="3" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A64" s="2" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>96</v>
+        <v>88</v>
       </c>
       <c r="C64" s="3" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A65" s="1" t="s">
-        <v>419</v>
+      <c r="A65" s="2" t="s">
+        <v>89</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>430</v>
-      </c>
-      <c r="C65" s="1" t="s">
-        <v>419</v>
+        <v>90</v>
+      </c>
+      <c r="C65" s="3" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A66" s="1" t="s">
+        <v>407</v>
+      </c>
+      <c r="B66" s="2" t="s">
         <v>418</v>
       </c>
-      <c r="B66" s="2" t="s">
-        <v>429</v>
-      </c>
       <c r="C66" s="1" t="s">
-        <v>418</v>
+        <v>407</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A67" s="2" t="s">
-        <v>97</v>
+      <c r="A67" s="1" t="s">
+        <v>406</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="C67" s="2" t="s">
-        <v>97</v>
+        <v>417</v>
+      </c>
+      <c r="C67" s="1" t="s">
+        <v>406</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A68" s="2" t="s">
-        <v>386</v>
+        <v>91</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>387</v>
+        <v>92</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>386</v>
+        <v>91</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A69" s="2" t="s">
-        <v>99</v>
+        <v>374</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="C69" s="3" t="s">
-        <v>99</v>
+        <v>375</v>
+      </c>
+      <c r="C69" s="2" t="s">
+        <v>374</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A70" s="2" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>449</v>
+        <v>94</v>
       </c>
       <c r="C70" s="3" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A71" s="2" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>103</v>
+        <v>437</v>
       </c>
       <c r="C71" s="3" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A72" s="2" t="s">
-        <v>104</v>
+        <v>96</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>105</v>
+        <v>97</v>
       </c>
       <c r="C72" s="3" t="s">
-        <v>104</v>
+        <v>96</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A73" s="2" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="C73" s="3" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A74" s="2" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="C74" s="3" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A75" s="2" t="s">
-        <v>110</v>
+        <v>102</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="C75" s="3" t="s">
-        <v>110</v>
+        <v>102</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A76" s="2" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
       <c r="C76" s="3" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A77" s="2" t="s">
-        <v>114</v>
+        <v>106</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="C77" s="3" t="s">
-        <v>114</v>
+        <v>106</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A78" s="2" t="s">
-        <v>116</v>
+        <v>500</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>117</v>
+        <v>501</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>116</v>
+        <v>500</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A79" s="2" t="s">
-        <v>118</v>
+        <v>108</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="C79" s="2" t="s">
-        <v>118</v>
+        <v>109</v>
+      </c>
+      <c r="C79" s="3" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A80" s="2" t="s">
-        <v>120</v>
+        <v>110</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>121</v>
+        <v>111</v>
       </c>
       <c r="C80" s="2" t="s">
-        <v>120</v>
+        <v>110</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A81" s="2" t="s">
-        <v>122</v>
+        <v>112</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>123</v>
+        <v>113</v>
       </c>
       <c r="C81" s="2" t="s">
-        <v>122</v>
+        <v>112</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A82" s="2" t="s">
-        <v>124</v>
+        <v>114</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="C82" s="3" t="s">
-        <v>124</v>
+        <v>115</v>
+      </c>
+      <c r="C82" s="2" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A83" s="2" t="s">
-        <v>126</v>
+      <c r="A83" s="1" t="s">
+        <v>454</v>
       </c>
       <c r="B83" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="C83" s="3" t="s">
-        <v>126</v>
+        <v>455</v>
+      </c>
+      <c r="C83" s="1" t="s">
+        <v>454</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A84" s="2" t="s">
-        <v>128</v>
+        <v>116</v>
       </c>
       <c r="B84" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="C84" s="3" t="s">
-        <v>128</v>
+        <v>117</v>
+      </c>
+      <c r="C84" s="2" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A85" s="2" t="s">
-        <v>130</v>
+        <v>458</v>
       </c>
       <c r="B85" s="2" t="s">
-        <v>131</v>
+        <v>463</v>
       </c>
       <c r="C85" s="3" t="s">
-        <v>130</v>
+        <v>458</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A86" s="2" t="s">
-        <v>132</v>
+        <v>118</v>
       </c>
       <c r="B86" s="2" t="s">
-        <v>133</v>
+        <v>119</v>
       </c>
       <c r="C86" s="3" t="s">
-        <v>132</v>
+        <v>118</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A87" s="2" t="s">
-        <v>134</v>
+        <v>120</v>
       </c>
       <c r="B87" s="2" t="s">
-        <v>135</v>
-      </c>
-      <c r="C87" s="2" t="s">
-        <v>134</v>
+        <v>121</v>
+      </c>
+      <c r="C87" s="3" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A88" s="2" t="s">
-        <v>376</v>
+        <v>122</v>
       </c>
       <c r="B88" s="2" t="s">
-        <v>377</v>
-      </c>
-      <c r="C88" s="2" t="s">
-        <v>376</v>
+        <v>123</v>
+      </c>
+      <c r="C88" s="3" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A89" s="2" t="s">
-        <v>136</v>
+        <v>124</v>
       </c>
       <c r="B89" s="2" t="s">
-        <v>137</v>
-      </c>
-      <c r="C89" s="2" t="s">
-        <v>136</v>
+        <v>125</v>
+      </c>
+      <c r="C89" s="3" t="s">
+        <v>124</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A90" s="2" t="s">
-        <v>400</v>
+        <v>126</v>
       </c>
       <c r="B90" s="2" t="s">
-        <v>137</v>
+        <v>127</v>
       </c>
       <c r="C90" s="2" t="s">
-        <v>400</v>
+        <v>126</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A91" s="2" t="s">
-        <v>138</v>
+        <v>364</v>
       </c>
       <c r="B91" s="2" t="s">
-        <v>139</v>
-      </c>
-      <c r="C91" s="3" t="s">
-        <v>138</v>
+        <v>365</v>
+      </c>
+      <c r="C91" s="2" t="s">
+        <v>364</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A92" s="2" t="s">
-        <v>140</v>
+        <v>128</v>
       </c>
       <c r="B92" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="C92" s="3" t="s">
-        <v>140</v>
+        <v>129</v>
+      </c>
+      <c r="C92" s="2" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A93" s="2" t="s">
-        <v>142</v>
+        <v>388</v>
       </c>
       <c r="B93" s="2" t="s">
-        <v>143</v>
+        <v>129</v>
       </c>
       <c r="C93" s="2" t="s">
-        <v>142</v>
+        <v>388</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A94" s="2" t="s">
-        <v>144</v>
+        <v>130</v>
       </c>
       <c r="B94" s="2" t="s">
-        <v>145</v>
+        <v>131</v>
       </c>
       <c r="C94" s="3" t="s">
-        <v>144</v>
+        <v>130</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A95" s="1" t="s">
-        <v>421</v>
+      <c r="A95" s="2" t="s">
+        <v>132</v>
       </c>
       <c r="B95" s="2" t="s">
-        <v>431</v>
-      </c>
-      <c r="C95" s="1" t="s">
-        <v>421</v>
+        <v>133</v>
+      </c>
+      <c r="C95" s="3" t="s">
+        <v>132</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A96" s="2" t="s">
-        <v>146</v>
+        <v>134</v>
       </c>
       <c r="B96" s="2" t="s">
-        <v>147</v>
-      </c>
-      <c r="C96" s="3" t="s">
-        <v>146</v>
+        <v>135</v>
+      </c>
+      <c r="C96" s="2" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A97" s="2" t="s">
-        <v>148</v>
+        <v>136</v>
       </c>
       <c r="B97" s="2" t="s">
-        <v>149</v>
+        <v>137</v>
       </c>
       <c r="C97" s="3" t="s">
-        <v>148</v>
+        <v>136</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A98" s="2" t="s">
-        <v>150</v>
+      <c r="A98" s="1" t="s">
+        <v>409</v>
       </c>
       <c r="B98" s="2" t="s">
-        <v>151</v>
-      </c>
-      <c r="C98" s="3" t="s">
-        <v>150</v>
+        <v>419</v>
+      </c>
+      <c r="C98" s="1" t="s">
+        <v>409</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A99" s="2" t="s">
-        <v>152</v>
+        <v>138</v>
       </c>
       <c r="B99" s="2" t="s">
-        <v>153</v>
+        <v>139</v>
       </c>
       <c r="C99" s="3" t="s">
-        <v>152</v>
+        <v>138</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A100" s="2" t="s">
-        <v>154</v>
+        <v>140</v>
       </c>
       <c r="B100" s="2" t="s">
-        <v>155</v>
+        <v>141</v>
       </c>
       <c r="C100" s="3" t="s">
-        <v>154</v>
+        <v>140</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A101" s="2" t="s">
-        <v>156</v>
+        <v>142</v>
       </c>
       <c r="B101" s="2" t="s">
-        <v>157</v>
+        <v>143</v>
       </c>
       <c r="C101" s="3" t="s">
-        <v>156</v>
+        <v>142</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A102" s="2" t="s">
-        <v>158</v>
+        <v>144</v>
       </c>
       <c r="B102" s="2" t="s">
-        <v>159</v>
+        <v>145</v>
       </c>
       <c r="C102" s="3" t="s">
-        <v>158</v>
+        <v>144</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A103" s="2" t="s">
-        <v>160</v>
+        <v>146</v>
       </c>
       <c r="B103" s="2" t="s">
-        <v>161</v>
-      </c>
-      <c r="C103" s="2" t="s">
-        <v>160</v>
+        <v>147</v>
+      </c>
+      <c r="C103" s="3" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A104" s="2" t="s">
-        <v>440</v>
+        <v>148</v>
       </c>
       <c r="B104" s="2" t="s">
-        <v>441</v>
-      </c>
-      <c r="C104" s="2" t="s">
-        <v>440</v>
+        <v>149</v>
+      </c>
+      <c r="C104" s="3" t="s">
+        <v>148</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A105" s="2" t="s">
-        <v>162</v>
+        <v>150</v>
       </c>
       <c r="B105" s="2" t="s">
-        <v>163</v>
-      </c>
-      <c r="C105" s="2" t="s">
-        <v>162</v>
+        <v>151</v>
+      </c>
+      <c r="C105" s="3" t="s">
+        <v>150</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A106" s="2" t="s">
-        <v>164</v>
+        <v>152</v>
       </c>
       <c r="B106" s="2" t="s">
-        <v>165</v>
-      </c>
-      <c r="C106" s="3" t="s">
-        <v>164</v>
+        <v>153</v>
+      </c>
+      <c r="C106" s="2" t="s">
+        <v>152</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A107" s="2" t="s">
-        <v>166</v>
+        <v>428</v>
       </c>
       <c r="B107" s="2" t="s">
-        <v>167</v>
-      </c>
-      <c r="C107" s="3" t="s">
-        <v>166</v>
+        <v>429</v>
+      </c>
+      <c r="C107" s="2" t="s">
+        <v>428</v>
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A108" s="1" t="s">
-        <v>426</v>
-      </c>
-      <c r="B108" s="1" t="s">
-        <v>433</v>
-      </c>
-      <c r="C108" s="1" t="s">
-        <v>426</v>
+      <c r="A108" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="B108" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="C108" s="2" t="s">
+        <v>154</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A109" s="2" t="s">
-        <v>168</v>
+        <v>459</v>
       </c>
       <c r="B109" s="2" t="s">
-        <v>169</v>
+        <v>462</v>
       </c>
       <c r="C109" s="3" t="s">
-        <v>168</v>
+        <v>459</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A110" s="2" t="s">
-        <v>170</v>
+        <v>460</v>
       </c>
       <c r="B110" s="2" t="s">
-        <v>171</v>
-      </c>
-      <c r="C110" s="2" t="s">
-        <v>170</v>
+        <v>461</v>
+      </c>
+      <c r="C110" s="3" t="s">
+        <v>460</v>
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A111" s="2" t="s">
-        <v>172</v>
-      </c>
-      <c r="B111" s="2" t="s">
-        <v>401</v>
-      </c>
-      <c r="C111" s="3" t="s">
-        <v>172</v>
+      <c r="A111" s="1" t="s">
+        <v>414</v>
+      </c>
+      <c r="B111" s="1" t="s">
+        <v>421</v>
+      </c>
+      <c r="C111" s="1" t="s">
+        <v>414</v>
       </c>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A112" s="2" t="s">
-        <v>173</v>
+        <v>156</v>
       </c>
       <c r="B112" s="2" t="s">
-        <v>174</v>
+        <v>157</v>
       </c>
       <c r="C112" s="3" t="s">
-        <v>173</v>
+        <v>156</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A113" s="2" t="s">
-        <v>175</v>
+      <c r="A113" s="1" t="s">
+        <v>481</v>
       </c>
       <c r="B113" s="2" t="s">
-        <v>176</v>
-      </c>
-      <c r="C113" s="3" t="s">
-        <v>175</v>
+        <v>493</v>
+      </c>
+      <c r="C113" s="1" t="s">
+        <v>481</v>
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A114" s="2" t="s">
-        <v>177</v>
+      <c r="A114" s="1" t="s">
+        <v>478</v>
       </c>
       <c r="B114" s="2" t="s">
-        <v>178</v>
-      </c>
-      <c r="C114" s="3" t="s">
-        <v>177</v>
+        <v>490</v>
+      </c>
+      <c r="C114" s="1" t="s">
+        <v>478</v>
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A115" s="2" t="s">
-        <v>179</v>
+      <c r="A115" s="1" t="s">
+        <v>479</v>
       </c>
       <c r="B115" s="2" t="s">
-        <v>180</v>
-      </c>
-      <c r="C115" s="3" t="s">
-        <v>179</v>
+        <v>491</v>
+      </c>
+      <c r="C115" s="1" t="s">
+        <v>479</v>
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A116" s="2" t="s">
-        <v>181</v>
+        <v>158</v>
       </c>
       <c r="B116" s="2" t="s">
-        <v>182</v>
-      </c>
-      <c r="C116" s="3" t="s">
-        <v>181</v>
+        <v>159</v>
+      </c>
+      <c r="C116" s="2" t="s">
+        <v>158</v>
       </c>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A117" s="2" t="s">
-        <v>183</v>
+        <v>160</v>
       </c>
       <c r="B117" s="2" t="s">
-        <v>184</v>
+        <v>389</v>
       </c>
       <c r="C117" s="3" t="s">
-        <v>183</v>
+        <v>160</v>
       </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A118" s="2" t="s">
-        <v>185</v>
+        <v>161</v>
       </c>
       <c r="B118" s="2" t="s">
-        <v>174</v>
+        <v>162</v>
       </c>
       <c r="C118" s="3" t="s">
-        <v>185</v>
+        <v>161</v>
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A119" s="2" t="s">
-        <v>186</v>
+        <v>163</v>
       </c>
       <c r="B119" s="2" t="s">
-        <v>187</v>
+        <v>164</v>
       </c>
       <c r="C119" s="3" t="s">
-        <v>186</v>
+        <v>163</v>
       </c>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A120" s="2" t="s">
-        <v>188</v>
+        <v>165</v>
       </c>
       <c r="B120" s="2" t="s">
-        <v>189</v>
+        <v>166</v>
       </c>
       <c r="C120" s="3" t="s">
-        <v>188</v>
+        <v>165</v>
       </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A121" s="1" t="s">
-        <v>410</v>
+      <c r="A121" s="2" t="s">
+        <v>167</v>
       </c>
       <c r="B121" s="2" t="s">
-        <v>411</v>
-      </c>
-      <c r="C121" s="1" t="s">
-        <v>410</v>
+        <v>168</v>
+      </c>
+      <c r="C121" s="3" t="s">
+        <v>167</v>
       </c>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A122" s="2" t="s">
-        <v>364</v>
+        <v>169</v>
       </c>
       <c r="B122" s="2" t="s">
-        <v>365</v>
+        <v>170</v>
       </c>
       <c r="C122" s="3" t="s">
-        <v>364</v>
+        <v>169</v>
       </c>
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A123" s="2" t="s">
-        <v>190</v>
+        <v>171</v>
       </c>
       <c r="B123" s="2" t="s">
-        <v>191</v>
-      </c>
-      <c r="C123" s="2" t="s">
-        <v>190</v>
+        <v>172</v>
+      </c>
+      <c r="C123" s="3" t="s">
+        <v>171</v>
       </c>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A124" s="2" t="s">
-        <v>402</v>
+        <v>173</v>
       </c>
       <c r="B124" s="2" t="s">
-        <v>405</v>
-      </c>
-      <c r="C124" s="2" t="s">
-        <v>402</v>
+        <v>162</v>
+      </c>
+      <c r="C124" s="3" t="s">
+        <v>173</v>
       </c>
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A125" s="2" t="s">
-        <v>192</v>
+        <v>174</v>
       </c>
       <c r="B125" s="2" t="s">
-        <v>193</v>
+        <v>175</v>
       </c>
       <c r="C125" s="3" t="s">
-        <v>192</v>
+        <v>174</v>
       </c>
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A126" s="2" t="s">
-        <v>194</v>
+      <c r="A126" s="1" t="s">
+        <v>473</v>
       </c>
       <c r="B126" s="2" t="s">
-        <v>195</v>
-      </c>
-      <c r="C126" s="3" t="s">
-        <v>194</v>
+        <v>484</v>
+      </c>
+      <c r="C126" s="1" t="s">
+        <v>473</v>
       </c>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A127" s="2" t="s">
-        <v>196</v>
+        <v>176</v>
       </c>
       <c r="B127" s="2" t="s">
-        <v>197</v>
+        <v>177</v>
       </c>
       <c r="C127" s="3" t="s">
-        <v>196</v>
+        <v>176</v>
       </c>
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A128" s="2" t="s">
-        <v>352</v>
+      <c r="A128" s="1" t="s">
+        <v>398</v>
       </c>
       <c r="B128" s="2" t="s">
-        <v>353</v>
-      </c>
-      <c r="C128" s="3" t="s">
-        <v>352</v>
+        <v>399</v>
+      </c>
+      <c r="C128" s="1" t="s">
+        <v>398</v>
       </c>
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A129" s="2" t="s">
-        <v>368</v>
+        <v>352</v>
       </c>
       <c r="B129" s="2" t="s">
-        <v>369</v>
+        <v>353</v>
       </c>
       <c r="C129" s="3" t="s">
-        <v>368</v>
+        <v>352</v>
       </c>
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A130" s="2" t="s">
-        <v>366</v>
+        <v>178</v>
       </c>
       <c r="B130" s="2" t="s">
-        <v>367</v>
-      </c>
-      <c r="C130" s="3" t="s">
-        <v>366</v>
+        <v>179</v>
+      </c>
+      <c r="C130" s="2" t="s">
+        <v>178</v>
       </c>
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A131" s="2" t="s">
-        <v>198</v>
+        <v>390</v>
       </c>
       <c r="B131" s="2" t="s">
-        <v>199</v>
+        <v>393</v>
       </c>
       <c r="C131" s="2" t="s">
-        <v>198</v>
+        <v>390</v>
       </c>
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A132" s="2" t="s">
-        <v>200</v>
+      <c r="A132" s="1" t="s">
+        <v>477</v>
       </c>
       <c r="B132" s="2" t="s">
-        <v>201</v>
-      </c>
-      <c r="C132" s="3" t="s">
-        <v>200</v>
+        <v>489</v>
+      </c>
+      <c r="C132" s="1" t="s">
+        <v>477</v>
       </c>
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A133" s="2" t="s">
-        <v>202</v>
+        <v>180</v>
       </c>
       <c r="B133" s="2" t="s">
-        <v>203</v>
+        <v>181</v>
       </c>
       <c r="C133" s="3" t="s">
-        <v>202</v>
+        <v>180</v>
       </c>
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A134" s="1" t="s">
-        <v>445</v>
-      </c>
-      <c r="B134" s="1" t="s">
-        <v>446</v>
-      </c>
-      <c r="C134" s="1" t="s">
-        <v>445</v>
+      <c r="A134" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="B134" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="C134" s="3" t="s">
+        <v>182</v>
       </c>
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A135" s="2" t="s">
-        <v>204</v>
+        <v>184</v>
       </c>
       <c r="B135" s="2" t="s">
-        <v>205</v>
+        <v>185</v>
       </c>
       <c r="C135" s="3" t="s">
-        <v>204</v>
+        <v>184</v>
       </c>
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A136" s="2" t="s">
-        <v>354</v>
+        <v>340</v>
       </c>
       <c r="B136" s="2" t="s">
-        <v>355</v>
+        <v>341</v>
       </c>
       <c r="C136" s="3" t="s">
-        <v>354</v>
+        <v>340</v>
       </c>
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A137" s="2" t="s">
-        <v>206</v>
+        <v>356</v>
       </c>
       <c r="B137" s="2" t="s">
-        <v>207</v>
+        <v>357</v>
       </c>
       <c r="C137" s="3" t="s">
-        <v>206</v>
+        <v>356</v>
       </c>
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A138" s="2" t="s">
-        <v>208</v>
+        <v>354</v>
       </c>
       <c r="B138" s="2" t="s">
-        <v>209</v>
+        <v>355</v>
       </c>
       <c r="C138" s="3" t="s">
-        <v>208</v>
+        <v>354</v>
       </c>
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A139" s="2" t="s">
-        <v>210</v>
+        <v>186</v>
       </c>
       <c r="B139" s="2" t="s">
-        <v>211</v>
-      </c>
-      <c r="C139" s="3" t="s">
-        <v>210</v>
+        <v>187</v>
+      </c>
+      <c r="C139" s="2" t="s">
+        <v>186</v>
       </c>
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A140" s="2" t="s">
-        <v>212</v>
+        <v>188</v>
       </c>
       <c r="B140" s="2" t="s">
-        <v>213</v>
+        <v>189</v>
       </c>
       <c r="C140" s="3" t="s">
-        <v>212</v>
+        <v>188</v>
       </c>
     </row>
     <row r="141" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A141" s="2" t="s">
-        <v>214</v>
+        <v>190</v>
       </c>
       <c r="B141" s="2" t="s">
-        <v>215</v>
+        <v>191</v>
       </c>
       <c r="C141" s="3" t="s">
-        <v>214</v>
+        <v>190</v>
       </c>
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A142" s="2" t="s">
-        <v>216</v>
-      </c>
-      <c r="B142" s="2" t="s">
-        <v>217</v>
-      </c>
-      <c r="C142" s="3" t="s">
-        <v>216</v>
+      <c r="A142" s="1" t="s">
+        <v>433</v>
+      </c>
+      <c r="B142" s="1" t="s">
+        <v>434</v>
+      </c>
+      <c r="C142" s="1" t="s">
+        <v>433</v>
       </c>
     </row>
     <row r="143" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A143" s="2" t="s">
-        <v>218</v>
+        <v>192</v>
       </c>
       <c r="B143" s="2" t="s">
-        <v>219</v>
+        <v>193</v>
       </c>
       <c r="C143" s="3" t="s">
-        <v>218</v>
+        <v>192</v>
       </c>
     </row>
     <row r="144" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A144" s="2" t="s">
-        <v>220</v>
+        <v>342</v>
       </c>
       <c r="B144" s="2" t="s">
-        <v>221</v>
+        <v>343</v>
       </c>
       <c r="C144" s="3" t="s">
-        <v>220</v>
+        <v>342</v>
       </c>
     </row>
     <row r="145" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A145" s="2" t="s">
-        <v>222</v>
+        <v>456</v>
       </c>
       <c r="B145" s="2" t="s">
-        <v>223</v>
+        <v>457</v>
       </c>
       <c r="C145" s="3" t="s">
-        <v>222</v>
+        <v>456</v>
       </c>
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A146" s="2" t="s">
-        <v>372</v>
+        <v>194</v>
       </c>
       <c r="B146" s="2" t="s">
-        <v>373</v>
-      </c>
-      <c r="C146" s="2" t="s">
-        <v>372</v>
+        <v>195</v>
+      </c>
+      <c r="C146" s="3" t="s">
+        <v>194</v>
       </c>
     </row>
     <row r="147" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A147" s="2" t="s">
-        <v>224</v>
+        <v>196</v>
       </c>
       <c r="B147" s="2" t="s">
-        <v>225</v>
+        <v>197</v>
       </c>
       <c r="C147" s="3" t="s">
-        <v>224</v>
+        <v>196</v>
       </c>
     </row>
     <row r="148" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A148" s="2" t="s">
-        <v>226</v>
+      <c r="A148" s="1" t="s">
+        <v>502</v>
       </c>
       <c r="B148" s="2" t="s">
-        <v>227</v>
-      </c>
-      <c r="C148" s="3" t="s">
-        <v>226</v>
+        <v>503</v>
+      </c>
+      <c r="C148" s="1" t="s">
+        <v>502</v>
       </c>
     </row>
     <row r="149" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A149" s="2" t="s">
-        <v>403</v>
+        <v>198</v>
       </c>
       <c r="B149" s="2" t="s">
-        <v>406</v>
-      </c>
-      <c r="C149" s="2" t="s">
-        <v>403</v>
+        <v>199</v>
+      </c>
+      <c r="C149" s="3" t="s">
+        <v>198</v>
       </c>
     </row>
     <row r="150" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A150" s="1" t="s">
-        <v>424</v>
-      </c>
-      <c r="B150" s="1" t="s">
-        <v>435</v>
-      </c>
-      <c r="C150" s="1" t="s">
-        <v>424</v>
+      <c r="A150" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="B150" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="C150" s="3" t="s">
+        <v>200</v>
       </c>
     </row>
     <row r="151" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A151" s="2" t="s">
-        <v>228</v>
+        <v>202</v>
       </c>
       <c r="B151" s="2" t="s">
-        <v>229</v>
+        <v>203</v>
       </c>
       <c r="C151" s="3" t="s">
-        <v>228</v>
+        <v>202</v>
       </c>
     </row>
     <row r="152" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A152" s="2" t="s">
-        <v>230</v>
+        <v>204</v>
       </c>
       <c r="B152" s="2" t="s">
-        <v>231</v>
+        <v>205</v>
       </c>
       <c r="C152" s="3" t="s">
-        <v>230</v>
+        <v>204</v>
       </c>
     </row>
     <row r="153" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A153" s="2" t="s">
-        <v>232</v>
+        <v>206</v>
       </c>
       <c r="B153" s="2" t="s">
-        <v>233</v>
+        <v>207</v>
       </c>
       <c r="C153" s="3" t="s">
-        <v>232</v>
+        <v>206</v>
       </c>
     </row>
     <row r="154" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A154" s="2" t="s">
-        <v>234</v>
+        <v>208</v>
       </c>
       <c r="B154" s="2" t="s">
-        <v>235</v>
-      </c>
-      <c r="C154" s="2" t="s">
-        <v>234</v>
+        <v>209</v>
+      </c>
+      <c r="C154" s="3" t="s">
+        <v>208</v>
       </c>
     </row>
     <row r="155" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A155" s="1" t="s">
-        <v>458</v>
-      </c>
-      <c r="B155" s="1" t="s">
-        <v>460</v>
+        <v>498</v>
+      </c>
+      <c r="B155" s="2" t="s">
+        <v>499</v>
       </c>
       <c r="C155" s="1" t="s">
-        <v>458</v>
+        <v>498</v>
       </c>
     </row>
     <row r="156" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A156" s="2" t="s">
-        <v>390</v>
+        <v>210</v>
       </c>
       <c r="B156" s="2" t="s">
-        <v>391</v>
-      </c>
-      <c r="C156" s="2" t="s">
-        <v>390</v>
+        <v>211</v>
+      </c>
+      <c r="C156" s="3" t="s">
+        <v>210</v>
       </c>
     </row>
     <row r="157" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A157" s="2" t="s">
-        <v>236</v>
+        <v>360</v>
       </c>
       <c r="B157" s="2" t="s">
-        <v>237</v>
-      </c>
-      <c r="C157" s="3" t="s">
-        <v>236</v>
+        <v>361</v>
+      </c>
+      <c r="C157" s="2" t="s">
+        <v>360</v>
       </c>
     </row>
     <row r="158" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A158" s="2" t="s">
-        <v>360</v>
+        <v>212</v>
       </c>
       <c r="B158" s="2" t="s">
-        <v>361</v>
+        <v>213</v>
       </c>
       <c r="C158" s="3" t="s">
-        <v>360</v>
+        <v>212</v>
       </c>
     </row>
     <row r="159" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A159" s="1" t="s">
-        <v>462</v>
+      <c r="A159" s="2" t="s">
+        <v>214</v>
       </c>
       <c r="B159" s="2" t="s">
-        <v>463</v>
-      </c>
-      <c r="C159" s="1" t="s">
-        <v>462</v>
+        <v>215</v>
+      </c>
+      <c r="C159" s="3" t="s">
+        <v>214</v>
       </c>
     </row>
     <row r="160" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A160" s="2" t="s">
-        <v>238</v>
+        <v>391</v>
       </c>
       <c r="B160" s="2" t="s">
-        <v>239</v>
+        <v>394</v>
       </c>
       <c r="C160" s="2" t="s">
-        <v>238</v>
+        <v>391</v>
       </c>
     </row>
     <row r="161" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A161" s="2" t="s">
-        <v>240</v>
-      </c>
-      <c r="B161" s="2" t="s">
-        <v>241</v>
-      </c>
-      <c r="C161" s="2" t="s">
-        <v>240</v>
+      <c r="A161" s="1" t="s">
+        <v>412</v>
+      </c>
+      <c r="B161" s="1" t="s">
+        <v>423</v>
+      </c>
+      <c r="C161" s="1" t="s">
+        <v>412</v>
       </c>
     </row>
     <row r="162" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A162" s="2" t="s">
-        <v>242</v>
+        <v>216</v>
       </c>
       <c r="B162" s="2" t="s">
-        <v>243</v>
+        <v>217</v>
       </c>
       <c r="C162" s="3" t="s">
-        <v>242</v>
+        <v>216</v>
       </c>
     </row>
     <row r="163" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A163" s="2" t="s">
-        <v>244</v>
+        <v>218</v>
       </c>
       <c r="B163" s="2" t="s">
-        <v>245</v>
-      </c>
-      <c r="C163" s="2" t="s">
-        <v>244</v>
+        <v>219</v>
+      </c>
+      <c r="C163" s="3" t="s">
+        <v>218</v>
       </c>
     </row>
     <row r="164" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A164" s="2" t="s">
-        <v>246</v>
+        <v>220</v>
       </c>
       <c r="B164" s="2" t="s">
-        <v>247</v>
+        <v>221</v>
       </c>
       <c r="C164" s="3" t="s">
-        <v>246</v>
+        <v>220</v>
       </c>
     </row>
     <row r="165" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A165" s="2" t="s">
-        <v>248</v>
+        <v>222</v>
       </c>
       <c r="B165" s="2" t="s">
-        <v>249</v>
-      </c>
-      <c r="C165" s="3" t="s">
-        <v>248</v>
+        <v>223</v>
+      </c>
+      <c r="C165" s="2" t="s">
+        <v>222</v>
       </c>
     </row>
     <row r="166" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A166" s="2" t="s">
-        <v>250</v>
-      </c>
-      <c r="B166" s="2" t="s">
-        <v>251</v>
-      </c>
-      <c r="C166" s="3" t="s">
-        <v>250</v>
+      <c r="A166" s="1" t="s">
+        <v>446</v>
+      </c>
+      <c r="B166" s="1" t="s">
+        <v>448</v>
+      </c>
+      <c r="C166" s="1" t="s">
+        <v>446</v>
       </c>
     </row>
     <row r="167" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A167" s="2" t="s">
-        <v>252</v>
+        <v>378</v>
       </c>
       <c r="B167" s="2" t="s">
-        <v>416</v>
+        <v>379</v>
       </c>
       <c r="C167" s="2" t="s">
-        <v>252</v>
+        <v>378</v>
       </c>
     </row>
     <row r="168" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A168" s="2" t="s">
-        <v>408</v>
+        <v>224</v>
       </c>
       <c r="B168" s="2" t="s">
-        <v>409</v>
-      </c>
-      <c r="C168" s="2" t="s">
-        <v>408</v>
+        <v>225</v>
+      </c>
+      <c r="C168" s="3" t="s">
+        <v>224</v>
       </c>
     </row>
     <row r="169" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A169" s="2" t="s">
-        <v>253</v>
+        <v>348</v>
       </c>
       <c r="B169" s="2" t="s">
-        <v>412</v>
-      </c>
-      <c r="C169" s="2" t="s">
-        <v>253</v>
+        <v>349</v>
+      </c>
+      <c r="C169" s="3" t="s">
+        <v>348</v>
       </c>
     </row>
     <row r="170" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A170" s="2" t="s">
-        <v>254</v>
+      <c r="A170" s="1" t="s">
+        <v>450</v>
       </c>
       <c r="B170" s="2" t="s">
-        <v>255</v>
-      </c>
-      <c r="C170" s="2" t="s">
-        <v>254</v>
+        <v>451</v>
+      </c>
+      <c r="C170" s="1" t="s">
+        <v>450</v>
       </c>
     </row>
     <row r="171" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A171" s="2" t="s">
-        <v>256</v>
+        <v>226</v>
       </c>
       <c r="B171" s="2" t="s">
-        <v>257</v>
-      </c>
-      <c r="C171" s="3" t="s">
-        <v>256</v>
+        <v>227</v>
+      </c>
+      <c r="C171" s="2" t="s">
+        <v>226</v>
       </c>
     </row>
     <row r="172" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A172" s="2" t="s">
-        <v>258</v>
+      <c r="A172" s="1" t="s">
+        <v>470</v>
       </c>
       <c r="B172" s="2" t="s">
-        <v>259</v>
-      </c>
-      <c r="C172" s="3" t="s">
-        <v>258</v>
+        <v>482</v>
+      </c>
+      <c r="C172" s="1" t="s">
+        <v>470</v>
       </c>
     </row>
     <row r="173" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A173" s="2" t="s">
-        <v>260</v>
+        <v>228</v>
       </c>
       <c r="B173" s="2" t="s">
-        <v>261</v>
+        <v>229</v>
       </c>
       <c r="C173" s="2" t="s">
-        <v>260</v>
+        <v>228</v>
       </c>
     </row>
     <row r="174" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A174" s="2" t="s">
-        <v>262</v>
+        <v>230</v>
       </c>
       <c r="B174" s="2" t="s">
-        <v>443</v>
+        <v>231</v>
       </c>
       <c r="C174" s="3" t="s">
-        <v>262</v>
+        <v>230</v>
       </c>
     </row>
     <row r="175" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A175" s="2" t="s">
-        <v>263</v>
+        <v>232</v>
       </c>
       <c r="B175" s="2" t="s">
-        <v>444</v>
-      </c>
-      <c r="C175" s="3" t="s">
-        <v>263</v>
+        <v>233</v>
+      </c>
+      <c r="C175" s="2" t="s">
+        <v>232</v>
       </c>
     </row>
     <row r="176" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A176" s="2" t="s">
-        <v>264</v>
+        <v>234</v>
       </c>
       <c r="B176" s="2" t="s">
-        <v>265</v>
-      </c>
-      <c r="C176" s="2" t="s">
-        <v>264</v>
+        <v>235</v>
+      </c>
+      <c r="C176" s="3" t="s">
+        <v>234</v>
       </c>
     </row>
     <row r="177" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A177" s="2" t="s">
-        <v>266</v>
+        <v>236</v>
       </c>
       <c r="B177" s="2" t="s">
-        <v>267</v>
+        <v>237</v>
       </c>
       <c r="C177" s="3" t="s">
-        <v>266</v>
+        <v>236</v>
       </c>
     </row>
     <row r="178" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A178" s="2" t="s">
-        <v>268</v>
+        <v>496</v>
       </c>
       <c r="B178" s="2" t="s">
-        <v>269</v>
-      </c>
-      <c r="C178" s="3" t="s">
-        <v>268</v>
+        <v>497</v>
+      </c>
+      <c r="C178" s="2" t="s">
+        <v>496</v>
       </c>
     </row>
     <row r="179" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A179" s="2" t="s">
-        <v>270</v>
+        <v>238</v>
       </c>
       <c r="B179" s="2" t="s">
-        <v>271</v>
-      </c>
-      <c r="C179" s="2" t="s">
-        <v>270</v>
+        <v>239</v>
+      </c>
+      <c r="C179" s="3" t="s">
+        <v>238</v>
       </c>
     </row>
     <row r="180" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A180" s="2" t="s">
-        <v>272</v>
+        <v>240</v>
       </c>
       <c r="B180" s="2" t="s">
-        <v>273</v>
-      </c>
-      <c r="C180" s="3" t="s">
-        <v>272</v>
+        <v>404</v>
+      </c>
+      <c r="C180" s="2" t="s">
+        <v>240</v>
       </c>
     </row>
     <row r="181" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A181" s="2" t="s">
-        <v>274</v>
+        <v>396</v>
       </c>
       <c r="B181" s="2" t="s">
-        <v>275</v>
-      </c>
-      <c r="C181" s="3" t="s">
-        <v>274</v>
+        <v>397</v>
+      </c>
+      <c r="C181" s="2" t="s">
+        <v>396</v>
       </c>
     </row>
     <row r="182" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A182" s="1" t="s">
-        <v>452</v>
-      </c>
-      <c r="B182" s="1" t="s">
-        <v>454</v>
-      </c>
-      <c r="C182" s="1" t="s">
-        <v>452</v>
+      <c r="A182" s="2" t="s">
+        <v>466</v>
+      </c>
+      <c r="B182" s="2" t="s">
+        <v>468</v>
+      </c>
+      <c r="C182" s="2" t="s">
+        <v>466</v>
       </c>
     </row>
     <row r="183" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A183" s="1" t="s">
-        <v>453</v>
-      </c>
-      <c r="B183" s="1" t="s">
-        <v>455</v>
-      </c>
-      <c r="C183" s="1" t="s">
-        <v>453</v>
+      <c r="A183" s="2" t="s">
+        <v>241</v>
+      </c>
+      <c r="B183" s="2" t="s">
+        <v>400</v>
+      </c>
+      <c r="C183" s="2" t="s">
+        <v>241</v>
       </c>
     </row>
     <row r="184" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A184" s="2" t="s">
-        <v>276</v>
+        <v>242</v>
       </c>
       <c r="B184" s="2" t="s">
-        <v>277</v>
-      </c>
-      <c r="C184" s="3" t="s">
-        <v>276</v>
+        <v>243</v>
+      </c>
+      <c r="C184" s="2" t="s">
+        <v>242</v>
       </c>
     </row>
     <row r="185" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A185" s="2" t="s">
-        <v>414</v>
+        <v>244</v>
       </c>
       <c r="B185" s="2" t="s">
-        <v>415</v>
-      </c>
-      <c r="C185" s="2" t="s">
-        <v>414</v>
+        <v>245</v>
+      </c>
+      <c r="C185" s="3" t="s">
+        <v>244</v>
       </c>
     </row>
     <row r="186" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A186" s="2" t="s">
-        <v>388</v>
+        <v>246</v>
       </c>
       <c r="B186" s="2" t="s">
-        <v>389</v>
-      </c>
-      <c r="C186" s="2" t="s">
-        <v>388</v>
+        <v>247</v>
+      </c>
+      <c r="C186" s="3" t="s">
+        <v>246</v>
       </c>
     </row>
     <row r="187" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A187" s="2" t="s">
-        <v>278</v>
+        <v>248</v>
       </c>
       <c r="B187" s="2" t="s">
-        <v>413</v>
+        <v>249</v>
       </c>
       <c r="C187" s="2" t="s">
-        <v>278</v>
+        <v>248</v>
       </c>
     </row>
     <row r="188" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A188" s="2" t="s">
-        <v>279</v>
+        <v>250</v>
       </c>
       <c r="B188" s="2" t="s">
-        <v>280</v>
+        <v>431</v>
       </c>
       <c r="C188" s="3" t="s">
-        <v>279</v>
+        <v>250</v>
       </c>
     </row>
     <row r="189" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A189" s="2" t="s">
-        <v>281</v>
+        <v>251</v>
       </c>
       <c r="B189" s="2" t="s">
-        <v>282</v>
-      </c>
-      <c r="C189" s="2" t="s">
-        <v>281</v>
+        <v>432</v>
+      </c>
+      <c r="C189" s="3" t="s">
+        <v>251</v>
       </c>
     </row>
     <row r="190" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A190" s="1" t="s">
-        <v>417</v>
+      <c r="A190" s="2" t="s">
+        <v>464</v>
       </c>
       <c r="B190" s="2" t="s">
-        <v>428</v>
-      </c>
-      <c r="C190" s="1" t="s">
-        <v>417</v>
+        <v>465</v>
+      </c>
+      <c r="C190" s="2" t="s">
+        <v>464</v>
       </c>
     </row>
     <row r="191" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A191" s="2" t="s">
-        <v>283</v>
+        <v>252</v>
       </c>
       <c r="B191" s="2" t="s">
-        <v>284</v>
-      </c>
-      <c r="C191" s="3" t="s">
-        <v>283</v>
+        <v>253</v>
+      </c>
+      <c r="C191" s="2" t="s">
+        <v>252</v>
       </c>
     </row>
     <row r="192" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A192" s="2" t="s">
-        <v>285</v>
+        <v>254</v>
       </c>
       <c r="B192" s="2" t="s">
-        <v>286</v>
-      </c>
-      <c r="C192" s="2" t="s">
-        <v>285</v>
+        <v>255</v>
+      </c>
+      <c r="C192" s="3" t="s">
+        <v>254</v>
       </c>
     </row>
     <row r="193" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A193" s="2" t="s">
-        <v>287</v>
+        <v>256</v>
       </c>
       <c r="B193" s="2" t="s">
-        <v>288</v>
+        <v>257</v>
       </c>
       <c r="C193" s="3" t="s">
-        <v>287</v>
+        <v>256</v>
       </c>
     </row>
     <row r="194" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A194" s="2" t="s">
-        <v>9</v>
+        <v>258</v>
       </c>
       <c r="B194" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C194" s="3" t="s">
-        <v>9</v>
+        <v>259</v>
+      </c>
+      <c r="C194" s="2" t="s">
+        <v>258</v>
       </c>
     </row>
     <row r="195" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A195" s="2" t="s">
-        <v>289</v>
+        <v>260</v>
       </c>
       <c r="B195" s="2" t="s">
-        <v>290</v>
+        <v>261</v>
       </c>
       <c r="C195" s="3" t="s">
-        <v>289</v>
+        <v>260</v>
       </c>
     </row>
     <row r="196" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A196" s="2" t="s">
-        <v>392</v>
+        <v>262</v>
       </c>
       <c r="B196" s="2" t="s">
-        <v>393</v>
-      </c>
-      <c r="C196" s="2" t="s">
-        <v>392</v>
+        <v>263</v>
+      </c>
+      <c r="C196" s="3" t="s">
+        <v>262</v>
       </c>
     </row>
     <row r="197" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A197" s="2" t="s">
-        <v>291</v>
-      </c>
-      <c r="B197" s="2" t="s">
-        <v>292</v>
-      </c>
-      <c r="C197" s="3" t="s">
-        <v>291</v>
+      <c r="A197" s="1" t="s">
+        <v>440</v>
+      </c>
+      <c r="B197" s="1" t="s">
+        <v>442</v>
+      </c>
+      <c r="C197" s="1" t="s">
+        <v>440</v>
       </c>
     </row>
     <row r="198" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A198" s="2" t="s">
-        <v>293</v>
-      </c>
-      <c r="B198" s="2" t="s">
-        <v>294</v>
-      </c>
-      <c r="C198" s="3" t="s">
-        <v>293</v>
+      <c r="A198" s="1" t="s">
+        <v>441</v>
+      </c>
+      <c r="B198" s="1" t="s">
+        <v>443</v>
+      </c>
+      <c r="C198" s="1" t="s">
+        <v>441</v>
       </c>
     </row>
     <row r="199" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A199" s="2" t="s">
-        <v>5</v>
+        <v>264</v>
       </c>
       <c r="B199" s="2" t="s">
-        <v>6</v>
+        <v>265</v>
       </c>
       <c r="C199" s="3" t="s">
-        <v>5</v>
+        <v>264</v>
       </c>
     </row>
     <row r="200" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A200" s="2" t="s">
-        <v>295</v>
+        <v>402</v>
       </c>
       <c r="B200" s="2" t="s">
-        <v>296</v>
+        <v>403</v>
       </c>
       <c r="C200" s="2" t="s">
-        <v>295</v>
+        <v>402</v>
       </c>
     </row>
     <row r="201" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A201" s="2" t="s">
-        <v>297</v>
+        <v>376</v>
       </c>
       <c r="B201" s="2" t="s">
-        <v>298</v>
-      </c>
-      <c r="C201" s="3" t="s">
-        <v>297</v>
+        <v>377</v>
+      </c>
+      <c r="C201" s="2" t="s">
+        <v>376</v>
       </c>
     </row>
     <row r="202" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A202" s="2" t="s">
-        <v>299</v>
+        <v>266</v>
       </c>
       <c r="B202" s="2" t="s">
-        <v>298</v>
-      </c>
-      <c r="C202" s="3" t="s">
-        <v>299</v>
+        <v>401</v>
+      </c>
+      <c r="C202" s="2" t="s">
+        <v>266</v>
       </c>
     </row>
     <row r="203" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A203" s="2" t="s">
-        <v>300</v>
+        <v>267</v>
       </c>
       <c r="B203" s="2" t="s">
-        <v>301</v>
+        <v>268</v>
       </c>
       <c r="C203" s="3" t="s">
-        <v>300</v>
+        <v>267</v>
       </c>
     </row>
     <row r="204" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A204" s="2" t="s">
-        <v>302</v>
+        <v>269</v>
       </c>
       <c r="B204" s="2" t="s">
-        <v>303</v>
-      </c>
-      <c r="C204" s="3" t="s">
-        <v>302</v>
+        <v>270</v>
+      </c>
+      <c r="C204" s="2" t="s">
+        <v>269</v>
       </c>
     </row>
     <row r="205" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A205" s="2" t="s">
-        <v>304</v>
+      <c r="A205" s="1" t="s">
+        <v>405</v>
       </c>
       <c r="B205" s="2" t="s">
-        <v>305</v>
-      </c>
-      <c r="C205" s="3" t="s">
-        <v>304</v>
+        <v>416</v>
+      </c>
+      <c r="C205" s="1" t="s">
+        <v>405</v>
       </c>
     </row>
     <row r="206" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A206" s="2" t="s">
-        <v>306</v>
+        <v>271</v>
       </c>
       <c r="B206" s="2" t="s">
-        <v>307</v>
+        <v>272</v>
       </c>
       <c r="C206" s="3" t="s">
-        <v>306</v>
+        <v>271</v>
       </c>
     </row>
     <row r="207" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A207" s="2" t="s">
-        <v>308</v>
+        <v>273</v>
       </c>
       <c r="B207" s="2" t="s">
-        <v>309</v>
-      </c>
-      <c r="C207" s="3" t="s">
-        <v>308</v>
+        <v>274</v>
+      </c>
+      <c r="C207" s="2" t="s">
+        <v>273</v>
       </c>
     </row>
     <row r="208" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A208" s="2" t="s">
-        <v>310</v>
+        <v>275</v>
       </c>
       <c r="B208" s="2" t="s">
-        <v>311</v>
+        <v>276</v>
       </c>
       <c r="C208" s="3" t="s">
-        <v>310</v>
+        <v>275</v>
       </c>
     </row>
     <row r="209" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A209" s="2" t="s">
-        <v>312</v>
+        <v>9</v>
       </c>
       <c r="B209" s="2" t="s">
-        <v>313</v>
-      </c>
-      <c r="C209" s="2" t="s">
-        <v>312</v>
+        <v>10</v>
+      </c>
+      <c r="C209" s="3" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="210" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A210" s="1" t="s">
-        <v>423</v>
+      <c r="A210" s="2" t="s">
+        <v>277</v>
       </c>
       <c r="B210" s="2" t="s">
-        <v>432</v>
-      </c>
-      <c r="C210" s="1" t="s">
-        <v>423</v>
+        <v>278</v>
+      </c>
+      <c r="C210" s="3" t="s">
+        <v>277</v>
       </c>
     </row>
     <row r="211" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A211" s="2" t="s">
-        <v>314</v>
+      <c r="A211" s="1" t="s">
+        <v>475</v>
       </c>
       <c r="B211" s="2" t="s">
-        <v>315</v>
-      </c>
-      <c r="C211" s="3" t="s">
-        <v>314</v>
+        <v>486</v>
+      </c>
+      <c r="C211" s="1" t="s">
+        <v>475</v>
       </c>
     </row>
     <row r="212" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A212" s="2" t="s">
-        <v>316</v>
+        <v>380</v>
       </c>
       <c r="B212" s="2" t="s">
-        <v>317</v>
-      </c>
-      <c r="C212" s="3" t="s">
-        <v>316</v>
+        <v>381</v>
+      </c>
+      <c r="C212" s="2" t="s">
+        <v>380</v>
       </c>
     </row>
     <row r="213" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A213" s="1" t="s">
-        <v>427</v>
-      </c>
-      <c r="B213" s="1" t="s">
-        <v>434</v>
-      </c>
-      <c r="C213" s="1" t="s">
-        <v>427</v>
+      <c r="A213" s="2" t="s">
+        <v>279</v>
+      </c>
+      <c r="B213" s="2" t="s">
+        <v>280</v>
+      </c>
+      <c r="C213" s="3" t="s">
+        <v>279</v>
       </c>
     </row>
     <row r="214" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A214" s="2" t="s">
-        <v>318</v>
+      <c r="A214" s="1" t="s">
+        <v>480</v>
       </c>
       <c r="B214" s="2" t="s">
-        <v>319</v>
-      </c>
-      <c r="C214" s="3" t="s">
-        <v>318</v>
+        <v>492</v>
+      </c>
+      <c r="C214" s="1" t="s">
+        <v>480</v>
       </c>
     </row>
     <row r="215" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A215" s="2" t="s">
-        <v>320</v>
+      <c r="A215" s="1" t="s">
+        <v>504</v>
       </c>
       <c r="B215" s="2" t="s">
-        <v>321</v>
-      </c>
-      <c r="C215" s="3" t="s">
-        <v>320</v>
+        <v>505</v>
+      </c>
+      <c r="C215" s="1" t="s">
+        <v>504</v>
       </c>
     </row>
     <row r="216" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A216" s="2" t="s">
-        <v>322</v>
+        <v>281</v>
       </c>
       <c r="B216" s="2" t="s">
-        <v>323</v>
+        <v>282</v>
       </c>
       <c r="C216" s="3" t="s">
-        <v>322</v>
+        <v>281</v>
       </c>
     </row>
     <row r="217" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A217" s="2" t="s">
-        <v>324</v>
+        <v>5</v>
       </c>
       <c r="B217" s="2" t="s">
-        <v>325</v>
+        <v>6</v>
       </c>
       <c r="C217" s="3" t="s">
-        <v>324</v>
+        <v>5</v>
       </c>
     </row>
     <row r="218" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A218" s="1" t="s">
-        <v>422</v>
+      <c r="A218" s="2" t="s">
+        <v>283</v>
       </c>
       <c r="B218" s="2" t="s">
-        <v>437</v>
-      </c>
-      <c r="C218" s="1" t="s">
-        <v>422</v>
+        <v>284</v>
+      </c>
+      <c r="C218" s="2" t="s">
+        <v>283</v>
       </c>
     </row>
     <row r="219" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A219" s="2" t="s">
-        <v>378</v>
+        <v>285</v>
       </c>
       <c r="B219" s="2" t="s">
-        <v>379</v>
-      </c>
-      <c r="C219" s="2" t="s">
-        <v>378</v>
+        <v>286</v>
+      </c>
+      <c r="C219" s="3" t="s">
+        <v>285</v>
       </c>
     </row>
     <row r="220" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A220" s="2" t="s">
-        <v>384</v>
+        <v>287</v>
       </c>
       <c r="B220" s="2" t="s">
-        <v>385</v>
-      </c>
-      <c r="C220" s="2" t="s">
-        <v>384</v>
+        <v>286</v>
+      </c>
+      <c r="C220" s="3" t="s">
+        <v>287</v>
       </c>
     </row>
     <row r="221" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A221" s="2" t="s">
-        <v>326</v>
+        <v>288</v>
       </c>
       <c r="B221" s="2" t="s">
-        <v>327</v>
+        <v>289</v>
       </c>
       <c r="C221" s="3" t="s">
-        <v>326</v>
+        <v>288</v>
       </c>
     </row>
     <row r="222" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A222" s="2" t="s">
-        <v>11</v>
+        <v>290</v>
       </c>
       <c r="B222" s="2" t="s">
-        <v>12</v>
+        <v>291</v>
       </c>
       <c r="C222" s="3" t="s">
-        <v>11</v>
+        <v>290</v>
       </c>
     </row>
     <row r="223" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A223" s="2" t="s">
-        <v>328</v>
+        <v>292</v>
       </c>
       <c r="B223" s="2" t="s">
-        <v>329</v>
-      </c>
-      <c r="C223" s="2" t="s">
-        <v>328</v>
+        <v>293</v>
+      </c>
+      <c r="C223" s="3" t="s">
+        <v>292</v>
       </c>
     </row>
     <row r="224" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A224" s="2" t="s">
-        <v>330</v>
+        <v>294</v>
       </c>
       <c r="B224" s="2" t="s">
-        <v>331</v>
+        <v>295</v>
       </c>
       <c r="C224" s="3" t="s">
-        <v>330</v>
+        <v>294</v>
       </c>
     </row>
     <row r="225" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A225" s="2" t="s">
-        <v>332</v>
+        <v>296</v>
       </c>
       <c r="B225" s="2" t="s">
-        <v>333</v>
+        <v>297</v>
       </c>
       <c r="C225" s="3" t="s">
-        <v>332</v>
+        <v>296</v>
       </c>
     </row>
     <row r="226" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A226" s="2" t="s">
-        <v>334</v>
+        <v>298</v>
       </c>
       <c r="B226" s="2" t="s">
-        <v>335</v>
-      </c>
-      <c r="C226" s="2" t="s">
-        <v>334</v>
+        <v>299</v>
+      </c>
+      <c r="C226" s="3" t="s">
+        <v>298</v>
       </c>
     </row>
     <row r="227" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A227" s="1" t="s">
-        <v>459</v>
-      </c>
-      <c r="B227" s="1" t="s">
-        <v>461</v>
-      </c>
-      <c r="C227" s="1" t="s">
-        <v>459</v>
+      <c r="A227" s="2" t="s">
+        <v>300</v>
+      </c>
+      <c r="B227" s="2" t="s">
+        <v>301</v>
+      </c>
+      <c r="C227" s="2" t="s">
+        <v>300</v>
       </c>
     </row>
     <row r="228" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A228" s="2" t="s">
-        <v>336</v>
+      <c r="A228" s="1" t="s">
+        <v>411</v>
       </c>
       <c r="B228" s="2" t="s">
-        <v>337</v>
-      </c>
-      <c r="C228" s="3" t="s">
-        <v>336</v>
+        <v>420</v>
+      </c>
+      <c r="C228" s="1" t="s">
+        <v>411</v>
       </c>
     </row>
     <row r="229" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A229" s="2" t="s">
-        <v>338</v>
+        <v>302</v>
       </c>
       <c r="B229" s="2" t="s">
-        <v>339</v>
-      </c>
-      <c r="C229" s="2" t="s">
-        <v>338</v>
+        <v>303</v>
+      </c>
+      <c r="C229" s="3" t="s">
+        <v>302</v>
       </c>
     </row>
     <row r="230" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A230" s="2" t="s">
-        <v>340</v>
+      <c r="A230" s="1" t="s">
+        <v>474</v>
       </c>
       <c r="B230" s="2" t="s">
-        <v>341</v>
-      </c>
-      <c r="C230" s="2" t="s">
-        <v>340</v>
+        <v>485</v>
+      </c>
+      <c r="C230" s="1" t="s">
+        <v>474</v>
       </c>
     </row>
     <row r="231" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A231" s="2" t="s">
-        <v>342</v>
+        <v>304</v>
       </c>
       <c r="B231" s="2" t="s">
-        <v>343</v>
+        <v>305</v>
       </c>
       <c r="C231" s="3" t="s">
-        <v>342</v>
+        <v>304</v>
       </c>
     </row>
     <row r="232" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A232" s="2" t="s">
-        <v>439</v>
+      <c r="A232" s="1" t="s">
+        <v>472</v>
       </c>
       <c r="B232" s="2" t="s">
-        <v>442</v>
-      </c>
-      <c r="C232" s="2" t="s">
-        <v>439</v>
+        <v>488</v>
+      </c>
+      <c r="C232" s="1" t="s">
+        <v>472</v>
       </c>
     </row>
     <row r="233" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A233" s="2" t="s">
-        <v>344</v>
-      </c>
-      <c r="B233" s="2" t="s">
-        <v>345</v>
-      </c>
-      <c r="C233" s="2" t="s">
-        <v>344</v>
+      <c r="A233" s="1" t="s">
+        <v>415</v>
+      </c>
+      <c r="B233" s="1" t="s">
+        <v>422</v>
+      </c>
+      <c r="C233" s="1" t="s">
+        <v>415</v>
       </c>
     </row>
     <row r="234" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A234" s="2" t="s">
-        <v>346</v>
+      <c r="A234" s="1" t="s">
+        <v>476</v>
       </c>
       <c r="B234" s="2" t="s">
-        <v>347</v>
-      </c>
-      <c r="C234" s="3" t="s">
-        <v>346</v>
+        <v>487</v>
+      </c>
+      <c r="C234" s="1" t="s">
+        <v>476</v>
       </c>
     </row>
     <row r="235" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A235" s="2" t="s">
-        <v>348</v>
+        <v>306</v>
       </c>
       <c r="B235" s="2" t="s">
-        <v>349</v>
+        <v>307</v>
       </c>
       <c r="C235" s="3" t="s">
-        <v>348</v>
+        <v>306</v>
       </c>
     </row>
     <row r="236" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A236" s="2" t="s">
-        <v>380</v>
+      <c r="A236" s="1" t="s">
+        <v>494</v>
       </c>
       <c r="B236" s="2" t="s">
-        <v>381</v>
-      </c>
-      <c r="C236" s="2" t="s">
-        <v>380</v>
+        <v>495</v>
+      </c>
+      <c r="C236" s="1" t="s">
+        <v>494</v>
       </c>
     </row>
     <row r="237" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A237" s="2" t="s">
-        <v>356</v>
+        <v>308</v>
       </c>
       <c r="B237" s="2" t="s">
-        <v>357</v>
+        <v>309</v>
       </c>
       <c r="C237" s="3" t="s">
-        <v>356</v>
+        <v>308</v>
+      </c>
+    </row>
+    <row r="238" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A238" s="2" t="s">
+        <v>310</v>
+      </c>
+      <c r="B238" s="2" t="s">
+        <v>311</v>
+      </c>
+      <c r="C238" s="3" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="239" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A239" s="2" t="s">
+        <v>312</v>
+      </c>
+      <c r="B239" s="2" t="s">
+        <v>313</v>
+      </c>
+      <c r="C239" s="3" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="240" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A240" s="1" t="s">
+        <v>410</v>
+      </c>
+      <c r="B240" s="2" t="s">
+        <v>425</v>
+      </c>
+      <c r="C240" s="1" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="241" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A241" s="2" t="s">
+        <v>366</v>
+      </c>
+      <c r="B241" s="2" t="s">
+        <v>367</v>
+      </c>
+      <c r="C241" s="2" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="242" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A242" s="2" t="s">
+        <v>372</v>
+      </c>
+      <c r="B242" s="2" t="s">
+        <v>373</v>
+      </c>
+      <c r="C242" s="2" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="243" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A243" s="2" t="s">
+        <v>314</v>
+      </c>
+      <c r="B243" s="2" t="s">
+        <v>315</v>
+      </c>
+      <c r="C243" s="3" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="244" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A244" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B244" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C244" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="245" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A245" s="2" t="s">
+        <v>316</v>
+      </c>
+      <c r="B245" s="2" t="s">
+        <v>317</v>
+      </c>
+      <c r="C245" s="2" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="246" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A246" s="2" t="s">
+        <v>318</v>
+      </c>
+      <c r="B246" s="2" t="s">
+        <v>319</v>
+      </c>
+      <c r="C246" s="3" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="247" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A247" s="2" t="s">
+        <v>320</v>
+      </c>
+      <c r="B247" s="2" t="s">
+        <v>321</v>
+      </c>
+      <c r="C247" s="3" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="248" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A248" s="2" t="s">
+        <v>322</v>
+      </c>
+      <c r="B248" s="2" t="s">
+        <v>323</v>
+      </c>
+      <c r="C248" s="2" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="249" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A249" s="1" t="s">
+        <v>447</v>
+      </c>
+      <c r="B249" s="1" t="s">
+        <v>449</v>
+      </c>
+      <c r="C249" s="1" t="s">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="250" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A250" s="2" t="s">
+        <v>324</v>
+      </c>
+      <c r="B250" s="2" t="s">
+        <v>325</v>
+      </c>
+      <c r="C250" s="3" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="251" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A251" s="2" t="s">
+        <v>326</v>
+      </c>
+      <c r="B251" s="2" t="s">
+        <v>327</v>
+      </c>
+      <c r="C251" s="2" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="252" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A252" s="2" t="s">
+        <v>328</v>
+      </c>
+      <c r="B252" s="2" t="s">
+        <v>329</v>
+      </c>
+      <c r="C252" s="2" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="253" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A253" s="2" t="s">
+        <v>330</v>
+      </c>
+      <c r="B253" s="2" t="s">
+        <v>331</v>
+      </c>
+      <c r="C253" s="3" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="254" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A254" s="2" t="s">
+        <v>427</v>
+      </c>
+      <c r="B254" s="2" t="s">
+        <v>430</v>
+      </c>
+      <c r="C254" s="2" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="255" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A255" s="2" t="s">
+        <v>332</v>
+      </c>
+      <c r="B255" s="2" t="s">
+        <v>333</v>
+      </c>
+      <c r="C255" s="2" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="256" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A256" s="2" t="s">
+        <v>334</v>
+      </c>
+      <c r="B256" s="2" t="s">
+        <v>335</v>
+      </c>
+      <c r="C256" s="3" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="257" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A257" s="2" t="s">
+        <v>336</v>
+      </c>
+      <c r="B257" s="2" t="s">
+        <v>337</v>
+      </c>
+      <c r="C257" s="3" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="258" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A258" s="2" t="s">
+        <v>368</v>
+      </c>
+      <c r="B258" s="2" t="s">
+        <v>369</v>
+      </c>
+      <c r="C258" s="2" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="259" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A259" s="2" t="s">
+        <v>344</v>
+      </c>
+      <c r="B259" s="2" t="s">
+        <v>345</v>
+      </c>
+      <c r="C259" s="3" t="s">
+        <v>344</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:C1" xr:uid="{56EE5BC3-7B0A-4577-92C7-56F73F7DDC8B}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C237">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C259">
       <sortCondition ref="A1"/>
     </sortState>
   </autoFilter>

</xml_diff>

<commit_message>
Couple of tests for normality of distribution
</commit_message>
<xml_diff>
--- a/translations/source.xlsx
+++ b/translations/source.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/e6c7874704bc5dfb/Documents/R Studio/DataSuite/translations/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="220" documentId="8_{D77EC384-F39F-4BA6-8963-4B8AF986F7DE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{CFD1DA65-D5D8-4C11-9E3E-2CA4D226B7C5}"/>
+  <xr:revisionPtr revIDLastSave="237" documentId="8_{D77EC384-F39F-4BA6-8963-4B8AF986F7DE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{74E0BBAB-F522-43AB-A081-5DE5C0F0188C}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="16395" xr2:uid="{BD840C99-A56D-4EBC-B1B7-A6018ADC22A6}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="804" uniqueCount="525">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="810" uniqueCount="529">
   <si>
     <t>base</t>
   </si>
@@ -531,12 +531,6 @@
     <t>Shapiro-Wilk's test</t>
   </si>
   <si>
-    <t>Критерий Шапиро-Уилка для проверки нормальности распределения</t>
-  </si>
-  <si>
-    <t>Shapiro-Wilk's test for normality of distribution</t>
-  </si>
-  <si>
     <t>критерию Кендалла</t>
   </si>
   <si>
@@ -1609,6 +1603,24 @@
   </si>
   <si>
     <t>Adjustment for multiple testing</t>
+  </si>
+  <si>
+    <t>Критерий Лиллиефорса</t>
+  </si>
+  <si>
+    <t>Lilliefors</t>
+  </si>
+  <si>
+    <t>Критерий Колмогорова-Смирнова</t>
+  </si>
+  <si>
+    <t>Kolmogorov-Smirnov's test</t>
+  </si>
+  <si>
+    <t>{method_title} для проверки нормальности распределения</t>
+  </si>
+  <si>
+    <t>{method_title} for normality of distribution</t>
   </si>
 </sst>
 </file>
@@ -1966,10 +1978,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C853ECA4-158B-4D85-A448-9ECE56776B5F}">
-  <dimension ref="A1:C268"/>
+  <dimension ref="A1:C270"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B269" sqref="B269"/>
+    <sheetView tabSelected="1" topLeftCell="A100" workbookViewId="0">
+      <selection activeCell="B107" sqref="B107"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -2037,13 +2049,13 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A6" s="1" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>17</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.45">
@@ -2059,13 +2071,13 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A8" s="1" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>19</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.45">
@@ -2081,35 +2093,35 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A10" s="2" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A11" s="2" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A12" s="2" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.45">
@@ -2224,35 +2236,35 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A23" s="2" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A24" s="1" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A25" s="2" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.45">
@@ -2282,7 +2294,7 @@
         <v>40</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="C28" s="3" t="s">
         <v>40</v>
@@ -2312,46 +2324,46 @@
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A31" s="1" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A32" s="1" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>523</v>
+        <v>521</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A33" s="2" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A34" s="1" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>521</v>
+        <v>519</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.45">
@@ -2367,13 +2379,13 @@
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A36" s="2" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.45">
@@ -2400,24 +2412,24 @@
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A39" s="2" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A40" s="2" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.45">
@@ -2433,24 +2445,24 @@
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A42" s="2" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A43" s="1" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.45">
@@ -2466,13 +2478,13 @@
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A45" s="2" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.45">
@@ -2488,13 +2500,13 @@
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A47" s="1" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.45">
@@ -2543,13 +2555,13 @@
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A52" s="1" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.45">
@@ -2587,46 +2599,46 @@
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A56" s="2" t="s">
+        <v>465</v>
+      </c>
+      <c r="B56" s="2" t="s">
         <v>467</v>
       </c>
-      <c r="B56" s="2" t="s">
-        <v>469</v>
-      </c>
       <c r="C56" s="2" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A57" s="2" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="C57" s="3" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A58" s="2" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A59" s="1" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.45">
@@ -2741,24 +2753,24 @@
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A70" s="1" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A71" s="1" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.45">
@@ -2774,13 +2786,13 @@
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A73" s="2" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.45">
@@ -2799,7 +2811,7 @@
         <v>95</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="C75" s="3" t="s">
         <v>95</v>
@@ -2873,13 +2885,13 @@
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A82" s="2" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="C82" s="2" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.45">
@@ -2928,13 +2940,13 @@
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A87" s="1" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="B87" s="2" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.45">
@@ -2950,13 +2962,13 @@
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A89" s="2" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="B89" s="2" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="C89" s="3" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.45">
@@ -3016,13 +3028,13 @@
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A95" s="2" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="B95" s="2" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="C95" s="2" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.45">
@@ -3038,13 +3050,13 @@
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A97" s="2" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="B97" s="2" t="s">
         <v>129</v>
       </c>
       <c r="C97" s="2" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.45">
@@ -3093,13 +3105,13 @@
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A102" s="1" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="B102" s="2" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="C102" s="1" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.45">
@@ -3192,13 +3204,13 @@
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A111" s="2" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="B111" s="2" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="C111" s="2" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.45">
@@ -3214,35 +3226,35 @@
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A113" s="2" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="B113" s="2" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
       <c r="C113" s="3" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A114" s="2" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
       <c r="B114" s="2" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
       <c r="C114" s="3" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A115" s="1" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="B115" s="1" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="C115" s="1" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.45">
@@ -3258,35 +3270,35 @@
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A117" s="1" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
       <c r="B117" s="2" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
       <c r="C117" s="1" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A118" s="1" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
       <c r="B118" s="2" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
       <c r="C118" s="1" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A119" s="1" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="B119" s="2" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
       <c r="C119" s="1" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.45">
@@ -3305,7 +3317,7 @@
         <v>160</v>
       </c>
       <c r="B121" s="2" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="C121" s="3" t="s">
         <v>160</v>
@@ -3324,1267 +3336,1267 @@
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A123" s="2" t="s">
-        <v>163</v>
+        <v>525</v>
       </c>
       <c r="B123" s="2" t="s">
-        <v>164</v>
-      </c>
-      <c r="C123" s="3" t="s">
-        <v>163</v>
+        <v>526</v>
+      </c>
+      <c r="C123" s="2" t="s">
+        <v>525</v>
       </c>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A124" s="2" t="s">
-        <v>165</v>
+        <v>523</v>
       </c>
       <c r="B124" s="2" t="s">
-        <v>166</v>
-      </c>
-      <c r="C124" s="3" t="s">
-        <v>165</v>
+        <v>524</v>
+      </c>
+      <c r="C124" s="2" t="s">
+        <v>523</v>
       </c>
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A125" s="2" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="B125" s="2" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="C125" s="3" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A126" s="2" t="s">
-        <v>169</v>
+        <v>527</v>
       </c>
       <c r="B126" s="2" t="s">
-        <v>170</v>
+        <v>528</v>
       </c>
       <c r="C126" s="3" t="s">
-        <v>169</v>
+        <v>527</v>
       </c>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A127" s="2" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
       <c r="B127" s="2" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
       <c r="C127" s="3" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A128" s="2" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
       <c r="B128" s="2" t="s">
-        <v>162</v>
+        <v>168</v>
       </c>
       <c r="C128" s="3" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A129" s="2" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="B129" s="2" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="C129" s="3" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A130" s="1" t="s">
-        <v>473</v>
+      <c r="A130" s="2" t="s">
+        <v>171</v>
       </c>
       <c r="B130" s="2" t="s">
-        <v>484</v>
-      </c>
-      <c r="C130" s="1" t="s">
-        <v>473</v>
+        <v>162</v>
+      </c>
+      <c r="C130" s="3" t="s">
+        <v>171</v>
       </c>
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A131" s="2" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="B131" s="2" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="C131" s="3" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A132" s="1" t="s">
-        <v>398</v>
+        <v>471</v>
       </c>
       <c r="B132" s="2" t="s">
-        <v>399</v>
+        <v>482</v>
       </c>
       <c r="C132" s="1" t="s">
-        <v>398</v>
+        <v>471</v>
       </c>
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A133" s="2" t="s">
-        <v>352</v>
+        <v>174</v>
       </c>
       <c r="B133" s="2" t="s">
-        <v>353</v>
+        <v>175</v>
       </c>
       <c r="C133" s="3" t="s">
-        <v>352</v>
+        <v>174</v>
       </c>
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A134" s="2" t="s">
-        <v>178</v>
+      <c r="A134" s="1" t="s">
+        <v>396</v>
       </c>
       <c r="B134" s="2" t="s">
-        <v>179</v>
-      </c>
-      <c r="C134" s="2" t="s">
-        <v>178</v>
+        <v>397</v>
+      </c>
+      <c r="C134" s="1" t="s">
+        <v>396</v>
       </c>
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A135" s="2" t="s">
-        <v>390</v>
+        <v>350</v>
       </c>
       <c r="B135" s="2" t="s">
-        <v>393</v>
-      </c>
-      <c r="C135" s="2" t="s">
-        <v>390</v>
+        <v>351</v>
+      </c>
+      <c r="C135" s="3" t="s">
+        <v>350</v>
       </c>
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A136" s="1" t="s">
-        <v>477</v>
+      <c r="A136" s="2" t="s">
+        <v>176</v>
       </c>
       <c r="B136" s="2" t="s">
-        <v>489</v>
-      </c>
-      <c r="C136" s="1" t="s">
-        <v>477</v>
+        <v>177</v>
+      </c>
+      <c r="C136" s="2" t="s">
+        <v>176</v>
       </c>
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A137" s="2" t="s">
-        <v>180</v>
+        <v>388</v>
       </c>
       <c r="B137" s="2" t="s">
-        <v>181</v>
-      </c>
-      <c r="C137" s="3" t="s">
-        <v>180</v>
+        <v>391</v>
+      </c>
+      <c r="C137" s="2" t="s">
+        <v>388</v>
       </c>
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A138" s="2" t="s">
-        <v>182</v>
+      <c r="A138" s="1" t="s">
+        <v>475</v>
       </c>
       <c r="B138" s="2" t="s">
-        <v>183</v>
-      </c>
-      <c r="C138" s="3" t="s">
-        <v>182</v>
+        <v>487</v>
+      </c>
+      <c r="C138" s="1" t="s">
+        <v>475</v>
       </c>
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A139" s="2" t="s">
-        <v>184</v>
+        <v>178</v>
       </c>
       <c r="B139" s="2" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
       <c r="C139" s="3" t="s">
-        <v>184</v>
+        <v>178</v>
       </c>
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A140" s="2" t="s">
-        <v>340</v>
+        <v>180</v>
       </c>
       <c r="B140" s="2" t="s">
-        <v>341</v>
+        <v>181</v>
       </c>
       <c r="C140" s="3" t="s">
-        <v>340</v>
+        <v>180</v>
       </c>
     </row>
     <row r="141" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A141" s="2" t="s">
-        <v>356</v>
+        <v>182</v>
       </c>
       <c r="B141" s="2" t="s">
-        <v>357</v>
+        <v>183</v>
       </c>
       <c r="C141" s="3" t="s">
-        <v>356</v>
+        <v>182</v>
       </c>
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A142" s="2" t="s">
-        <v>354</v>
+        <v>338</v>
       </c>
       <c r="B142" s="2" t="s">
-        <v>355</v>
+        <v>339</v>
       </c>
       <c r="C142" s="3" t="s">
-        <v>354</v>
+        <v>338</v>
       </c>
     </row>
     <row r="143" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A143" s="2" t="s">
-        <v>186</v>
+        <v>354</v>
       </c>
       <c r="B143" s="2" t="s">
-        <v>187</v>
-      </c>
-      <c r="C143" s="2" t="s">
-        <v>186</v>
+        <v>355</v>
+      </c>
+      <c r="C143" s="3" t="s">
+        <v>354</v>
       </c>
     </row>
     <row r="144" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A144" s="2" t="s">
-        <v>188</v>
+        <v>352</v>
       </c>
       <c r="B144" s="2" t="s">
-        <v>189</v>
+        <v>353</v>
       </c>
       <c r="C144" s="3" t="s">
-        <v>188</v>
+        <v>352</v>
       </c>
     </row>
     <row r="145" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A145" s="2" t="s">
-        <v>190</v>
+        <v>184</v>
       </c>
       <c r="B145" s="2" t="s">
-        <v>191</v>
-      </c>
-      <c r="C145" s="3" t="s">
-        <v>190</v>
+        <v>185</v>
+      </c>
+      <c r="C145" s="2" t="s">
+        <v>184</v>
       </c>
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A146" s="1" t="s">
-        <v>433</v>
-      </c>
-      <c r="B146" s="1" t="s">
-        <v>434</v>
-      </c>
-      <c r="C146" s="1" t="s">
-        <v>433</v>
+      <c r="A146" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="B146" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="C146" s="3" t="s">
+        <v>186</v>
       </c>
     </row>
     <row r="147" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A147" s="2" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="B147" s="2" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="C147" s="3" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
     </row>
     <row r="148" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A148" s="2" t="s">
-        <v>342</v>
-      </c>
-      <c r="B148" s="2" t="s">
-        <v>343</v>
-      </c>
-      <c r="C148" s="3" t="s">
-        <v>342</v>
+      <c r="A148" s="1" t="s">
+        <v>431</v>
+      </c>
+      <c r="B148" s="1" t="s">
+        <v>432</v>
+      </c>
+      <c r="C148" s="1" t="s">
+        <v>431</v>
       </c>
     </row>
     <row r="149" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A149" s="2" t="s">
-        <v>456</v>
+        <v>190</v>
       </c>
       <c r="B149" s="2" t="s">
-        <v>457</v>
+        <v>191</v>
       </c>
       <c r="C149" s="3" t="s">
-        <v>456</v>
+        <v>190</v>
       </c>
     </row>
     <row r="150" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A150" s="2" t="s">
-        <v>194</v>
+        <v>340</v>
       </c>
       <c r="B150" s="2" t="s">
-        <v>195</v>
+        <v>341</v>
       </c>
       <c r="C150" s="3" t="s">
-        <v>194</v>
+        <v>340</v>
       </c>
     </row>
     <row r="151" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A151" s="2" t="s">
-        <v>196</v>
+        <v>454</v>
       </c>
       <c r="B151" s="2" t="s">
-        <v>197</v>
+        <v>455</v>
       </c>
       <c r="C151" s="3" t="s">
-        <v>196</v>
+        <v>454</v>
       </c>
     </row>
     <row r="152" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A152" s="1" t="s">
-        <v>502</v>
+      <c r="A152" s="2" t="s">
+        <v>192</v>
       </c>
       <c r="B152" s="2" t="s">
-        <v>503</v>
-      </c>
-      <c r="C152" s="1" t="s">
-        <v>502</v>
+        <v>193</v>
+      </c>
+      <c r="C152" s="3" t="s">
+        <v>192</v>
       </c>
     </row>
     <row r="153" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A153" s="2" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="B153" s="2" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="C153" s="3" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
     </row>
     <row r="154" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A154" s="2" t="s">
-        <v>200</v>
+      <c r="A154" s="1" t="s">
+        <v>500</v>
       </c>
       <c r="B154" s="2" t="s">
-        <v>201</v>
-      </c>
-      <c r="C154" s="3" t="s">
-        <v>200</v>
+        <v>501</v>
+      </c>
+      <c r="C154" s="1" t="s">
+        <v>500</v>
       </c>
     </row>
     <row r="155" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A155" s="2" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
       <c r="B155" s="2" t="s">
-        <v>203</v>
+        <v>197</v>
       </c>
       <c r="C155" s="3" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
     </row>
     <row r="156" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A156" s="2" t="s">
-        <v>204</v>
+        <v>198</v>
       </c>
       <c r="B156" s="2" t="s">
-        <v>205</v>
+        <v>199</v>
       </c>
       <c r="C156" s="3" t="s">
-        <v>204</v>
+        <v>198</v>
       </c>
     </row>
     <row r="157" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A157" s="2" t="s">
-        <v>206</v>
+        <v>200</v>
       </c>
       <c r="B157" s="2" t="s">
-        <v>207</v>
+        <v>201</v>
       </c>
       <c r="C157" s="3" t="s">
-        <v>206</v>
+        <v>200</v>
       </c>
     </row>
     <row r="158" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A158" s="2" t="s">
-        <v>208</v>
+        <v>202</v>
       </c>
       <c r="B158" s="2" t="s">
-        <v>209</v>
+        <v>203</v>
       </c>
       <c r="C158" s="3" t="s">
-        <v>208</v>
+        <v>202</v>
       </c>
     </row>
     <row r="159" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A159" s="1" t="s">
-        <v>498</v>
+      <c r="A159" s="2" t="s">
+        <v>204</v>
       </c>
       <c r="B159" s="2" t="s">
-        <v>499</v>
-      </c>
-      <c r="C159" s="1" t="s">
-        <v>498</v>
+        <v>205</v>
+      </c>
+      <c r="C159" s="3" t="s">
+        <v>204</v>
       </c>
     </row>
     <row r="160" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A160" s="2" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="B160" s="2" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="C160" s="3" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
     </row>
     <row r="161" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A161" s="2" t="s">
-        <v>360</v>
+      <c r="A161" s="1" t="s">
+        <v>496</v>
       </c>
       <c r="B161" s="2" t="s">
-        <v>361</v>
-      </c>
-      <c r="C161" s="2" t="s">
-        <v>360</v>
+        <v>497</v>
+      </c>
+      <c r="C161" s="1" t="s">
+        <v>496</v>
       </c>
     </row>
     <row r="162" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A162" s="2" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="B162" s="2" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="C162" s="3" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
     </row>
     <row r="163" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A163" s="2" t="s">
-        <v>214</v>
+        <v>358</v>
       </c>
       <c r="B163" s="2" t="s">
-        <v>215</v>
-      </c>
-      <c r="C163" s="3" t="s">
-        <v>214</v>
+        <v>359</v>
+      </c>
+      <c r="C163" s="2" t="s">
+        <v>358</v>
       </c>
     </row>
     <row r="164" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A164" s="2" t="s">
-        <v>391</v>
+        <v>210</v>
       </c>
       <c r="B164" s="2" t="s">
-        <v>394</v>
-      </c>
-      <c r="C164" s="2" t="s">
-        <v>391</v>
+        <v>211</v>
+      </c>
+      <c r="C164" s="3" t="s">
+        <v>210</v>
       </c>
     </row>
     <row r="165" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A165" s="1" t="s">
-        <v>412</v>
-      </c>
-      <c r="B165" s="1" t="s">
-        <v>423</v>
-      </c>
-      <c r="C165" s="1" t="s">
-        <v>412</v>
+      <c r="A165" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="B165" s="2" t="s">
+        <v>213</v>
+      </c>
+      <c r="C165" s="3" t="s">
+        <v>212</v>
       </c>
     </row>
     <row r="166" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A166" s="2" t="s">
-        <v>216</v>
+        <v>389</v>
       </c>
       <c r="B166" s="2" t="s">
-        <v>217</v>
-      </c>
-      <c r="C166" s="3" t="s">
-        <v>216</v>
+        <v>392</v>
+      </c>
+      <c r="C166" s="2" t="s">
+        <v>389</v>
       </c>
     </row>
     <row r="167" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A167" s="2" t="s">
-        <v>218</v>
-      </c>
-      <c r="B167" s="2" t="s">
-        <v>219</v>
-      </c>
-      <c r="C167" s="3" t="s">
-        <v>218</v>
+      <c r="A167" s="1" t="s">
+        <v>410</v>
+      </c>
+      <c r="B167" s="1" t="s">
+        <v>421</v>
+      </c>
+      <c r="C167" s="1" t="s">
+        <v>410</v>
       </c>
     </row>
     <row r="168" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A168" s="2" t="s">
-        <v>220</v>
+        <v>214</v>
       </c>
       <c r="B168" s="2" t="s">
-        <v>221</v>
+        <v>215</v>
       </c>
       <c r="C168" s="3" t="s">
-        <v>220</v>
+        <v>214</v>
       </c>
     </row>
     <row r="169" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A169" s="2" t="s">
-        <v>222</v>
+        <v>216</v>
       </c>
       <c r="B169" s="2" t="s">
-        <v>223</v>
-      </c>
-      <c r="C169" s="2" t="s">
-        <v>222</v>
+        <v>217</v>
+      </c>
+      <c r="C169" s="3" t="s">
+        <v>216</v>
       </c>
     </row>
     <row r="170" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A170" s="1" t="s">
-        <v>446</v>
-      </c>
-      <c r="B170" s="1" t="s">
-        <v>448</v>
-      </c>
-      <c r="C170" s="1" t="s">
-        <v>446</v>
+      <c r="A170" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="B170" s="2" t="s">
+        <v>219</v>
+      </c>
+      <c r="C170" s="3" t="s">
+        <v>218</v>
       </c>
     </row>
     <row r="171" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A171" s="2" t="s">
-        <v>378</v>
+        <v>220</v>
       </c>
       <c r="B171" s="2" t="s">
-        <v>379</v>
+        <v>221</v>
       </c>
       <c r="C171" s="2" t="s">
-        <v>378</v>
+        <v>220</v>
       </c>
     </row>
     <row r="172" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A172" s="2" t="s">
-        <v>224</v>
-      </c>
-      <c r="B172" s="2" t="s">
-        <v>225</v>
-      </c>
-      <c r="C172" s="3" t="s">
-        <v>224</v>
+      <c r="A172" s="1" t="s">
+        <v>444</v>
+      </c>
+      <c r="B172" s="1" t="s">
+        <v>446</v>
+      </c>
+      <c r="C172" s="1" t="s">
+        <v>444</v>
       </c>
     </row>
     <row r="173" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A173" s="2" t="s">
-        <v>348</v>
+        <v>376</v>
       </c>
       <c r="B173" s="2" t="s">
-        <v>349</v>
-      </c>
-      <c r="C173" s="3" t="s">
-        <v>348</v>
+        <v>377</v>
+      </c>
+      <c r="C173" s="2" t="s">
+        <v>376</v>
       </c>
     </row>
     <row r="174" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A174" s="1" t="s">
-        <v>450</v>
+      <c r="A174" s="2" t="s">
+        <v>222</v>
       </c>
       <c r="B174" s="2" t="s">
-        <v>451</v>
-      </c>
-      <c r="C174" s="1" t="s">
-        <v>450</v>
+        <v>223</v>
+      </c>
+      <c r="C174" s="3" t="s">
+        <v>222</v>
       </c>
     </row>
     <row r="175" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A175" s="2" t="s">
-        <v>226</v>
+        <v>346</v>
       </c>
       <c r="B175" s="2" t="s">
-        <v>227</v>
-      </c>
-      <c r="C175" s="2" t="s">
-        <v>226</v>
+        <v>347</v>
+      </c>
+      <c r="C175" s="3" t="s">
+        <v>346</v>
       </c>
     </row>
     <row r="176" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A176" s="1" t="s">
-        <v>470</v>
+        <v>448</v>
       </c>
       <c r="B176" s="2" t="s">
-        <v>482</v>
+        <v>449</v>
       </c>
       <c r="C176" s="1" t="s">
-        <v>470</v>
+        <v>448</v>
       </c>
     </row>
     <row r="177" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A177" s="2" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="B177" s="2" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="C177" s="2" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
     </row>
     <row r="178" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A178" s="2" t="s">
-        <v>230</v>
+      <c r="A178" s="1" t="s">
+        <v>468</v>
       </c>
       <c r="B178" s="2" t="s">
-        <v>231</v>
-      </c>
-      <c r="C178" s="3" t="s">
-        <v>230</v>
+        <v>480</v>
+      </c>
+      <c r="C178" s="1" t="s">
+        <v>468</v>
       </c>
     </row>
     <row r="179" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A179" s="2" t="s">
-        <v>232</v>
+        <v>226</v>
       </c>
       <c r="B179" s="2" t="s">
-        <v>233</v>
+        <v>227</v>
       </c>
       <c r="C179" s="2" t="s">
-        <v>232</v>
+        <v>226</v>
       </c>
     </row>
     <row r="180" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A180" s="2" t="s">
-        <v>234</v>
+        <v>228</v>
       </c>
       <c r="B180" s="2" t="s">
-        <v>235</v>
+        <v>229</v>
       </c>
       <c r="C180" s="3" t="s">
-        <v>234</v>
+        <v>228</v>
       </c>
     </row>
     <row r="181" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A181" s="2" t="s">
-        <v>236</v>
+        <v>230</v>
       </c>
       <c r="B181" s="2" t="s">
-        <v>237</v>
-      </c>
-      <c r="C181" s="3" t="s">
-        <v>236</v>
+        <v>231</v>
+      </c>
+      <c r="C181" s="2" t="s">
+        <v>230</v>
       </c>
     </row>
     <row r="182" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A182" s="2" t="s">
-        <v>496</v>
+        <v>232</v>
       </c>
       <c r="B182" s="2" t="s">
-        <v>497</v>
-      </c>
-      <c r="C182" s="2" t="s">
-        <v>496</v>
+        <v>233</v>
+      </c>
+      <c r="C182" s="3" t="s">
+        <v>232</v>
       </c>
     </row>
     <row r="183" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A183" s="2" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="B183" s="2" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="C183" s="3" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
     </row>
     <row r="184" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A184" s="2" t="s">
-        <v>240</v>
+        <v>494</v>
       </c>
       <c r="B184" s="2" t="s">
-        <v>404</v>
+        <v>495</v>
       </c>
       <c r="C184" s="2" t="s">
-        <v>240</v>
+        <v>494</v>
       </c>
     </row>
     <row r="185" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A185" s="2" t="s">
-        <v>396</v>
+        <v>236</v>
       </c>
       <c r="B185" s="2" t="s">
-        <v>397</v>
-      </c>
-      <c r="C185" s="2" t="s">
-        <v>396</v>
+        <v>237</v>
+      </c>
+      <c r="C185" s="3" t="s">
+        <v>236</v>
       </c>
     </row>
     <row r="186" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A186" s="2" t="s">
-        <v>466</v>
+        <v>238</v>
       </c>
       <c r="B186" s="2" t="s">
-        <v>468</v>
+        <v>402</v>
       </c>
       <c r="C186" s="2" t="s">
-        <v>466</v>
+        <v>238</v>
       </c>
     </row>
     <row r="187" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A187" s="2" t="s">
-        <v>241</v>
+        <v>394</v>
       </c>
       <c r="B187" s="2" t="s">
-        <v>400</v>
+        <v>395</v>
       </c>
       <c r="C187" s="2" t="s">
-        <v>241</v>
+        <v>394</v>
       </c>
     </row>
     <row r="188" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A188" s="2" t="s">
-        <v>242</v>
+        <v>464</v>
       </c>
       <c r="B188" s="2" t="s">
-        <v>243</v>
+        <v>466</v>
       </c>
       <c r="C188" s="2" t="s">
-        <v>242</v>
+        <v>464</v>
       </c>
     </row>
     <row r="189" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A189" s="2" t="s">
-        <v>244</v>
+        <v>239</v>
       </c>
       <c r="B189" s="2" t="s">
-        <v>245</v>
-      </c>
-      <c r="C189" s="3" t="s">
-        <v>244</v>
+        <v>398</v>
+      </c>
+      <c r="C189" s="2" t="s">
+        <v>239</v>
       </c>
     </row>
     <row r="190" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A190" s="2" t="s">
-        <v>246</v>
+        <v>240</v>
       </c>
       <c r="B190" s="2" t="s">
-        <v>247</v>
-      </c>
-      <c r="C190" s="3" t="s">
-        <v>246</v>
+        <v>241</v>
+      </c>
+      <c r="C190" s="2" t="s">
+        <v>240</v>
       </c>
     </row>
     <row r="191" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A191" s="2" t="s">
-        <v>248</v>
+        <v>242</v>
       </c>
       <c r="B191" s="2" t="s">
-        <v>249</v>
-      </c>
-      <c r="C191" s="2" t="s">
-        <v>248</v>
+        <v>243</v>
+      </c>
+      <c r="C191" s="3" t="s">
+        <v>242</v>
       </c>
     </row>
     <row r="192" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A192" s="2" t="s">
-        <v>250</v>
+        <v>244</v>
       </c>
       <c r="B192" s="2" t="s">
-        <v>431</v>
+        <v>245</v>
       </c>
       <c r="C192" s="3" t="s">
-        <v>250</v>
+        <v>244</v>
       </c>
     </row>
     <row r="193" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A193" s="2" t="s">
-        <v>251</v>
+        <v>246</v>
       </c>
       <c r="B193" s="2" t="s">
-        <v>432</v>
-      </c>
-      <c r="C193" s="3" t="s">
-        <v>251</v>
+        <v>247</v>
+      </c>
+      <c r="C193" s="2" t="s">
+        <v>246</v>
       </c>
     </row>
     <row r="194" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A194" s="2" t="s">
-        <v>464</v>
+        <v>248</v>
       </c>
       <c r="B194" s="2" t="s">
-        <v>465</v>
-      </c>
-      <c r="C194" s="2" t="s">
-        <v>464</v>
+        <v>429</v>
+      </c>
+      <c r="C194" s="3" t="s">
+        <v>248</v>
       </c>
     </row>
     <row r="195" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A195" s="2" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="B195" s="2" t="s">
-        <v>253</v>
-      </c>
-      <c r="C195" s="2" t="s">
-        <v>252</v>
+        <v>430</v>
+      </c>
+      <c r="C195" s="3" t="s">
+        <v>249</v>
       </c>
     </row>
     <row r="196" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A196" s="2" t="s">
-        <v>254</v>
+        <v>462</v>
       </c>
       <c r="B196" s="2" t="s">
-        <v>255</v>
-      </c>
-      <c r="C196" s="3" t="s">
-        <v>254</v>
+        <v>463</v>
+      </c>
+      <c r="C196" s="2" t="s">
+        <v>462</v>
       </c>
     </row>
     <row r="197" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A197" s="2" t="s">
-        <v>256</v>
+        <v>250</v>
       </c>
       <c r="B197" s="2" t="s">
-        <v>257</v>
-      </c>
-      <c r="C197" s="3" t="s">
-        <v>256</v>
+        <v>251</v>
+      </c>
+      <c r="C197" s="2" t="s">
+        <v>250</v>
       </c>
     </row>
     <row r="198" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A198" s="2" t="s">
-        <v>258</v>
+        <v>252</v>
       </c>
       <c r="B198" s="2" t="s">
-        <v>259</v>
-      </c>
-      <c r="C198" s="2" t="s">
-        <v>258</v>
+        <v>253</v>
+      </c>
+      <c r="C198" s="3" t="s">
+        <v>252</v>
       </c>
     </row>
     <row r="199" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A199" s="2" t="s">
-        <v>260</v>
+        <v>254</v>
       </c>
       <c r="B199" s="2" t="s">
-        <v>261</v>
+        <v>255</v>
       </c>
       <c r="C199" s="3" t="s">
-        <v>260</v>
+        <v>254</v>
       </c>
     </row>
     <row r="200" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A200" s="2" t="s">
-        <v>262</v>
+        <v>256</v>
       </c>
       <c r="B200" s="2" t="s">
-        <v>263</v>
-      </c>
-      <c r="C200" s="3" t="s">
-        <v>262</v>
+        <v>257</v>
+      </c>
+      <c r="C200" s="2" t="s">
+        <v>256</v>
       </c>
     </row>
     <row r="201" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A201" s="1" t="s">
-        <v>440</v>
-      </c>
-      <c r="B201" s="1" t="s">
-        <v>442</v>
-      </c>
-      <c r="C201" s="1" t="s">
-        <v>440</v>
+      <c r="A201" s="2" t="s">
+        <v>258</v>
+      </c>
+      <c r="B201" s="2" t="s">
+        <v>259</v>
+      </c>
+      <c r="C201" s="3" t="s">
+        <v>258</v>
       </c>
     </row>
     <row r="202" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A202" s="1" t="s">
-        <v>441</v>
-      </c>
-      <c r="B202" s="1" t="s">
-        <v>443</v>
-      </c>
-      <c r="C202" s="1" t="s">
-        <v>441</v>
+      <c r="A202" s="2" t="s">
+        <v>260</v>
+      </c>
+      <c r="B202" s="2" t="s">
+        <v>261</v>
+      </c>
+      <c r="C202" s="3" t="s">
+        <v>260</v>
       </c>
     </row>
     <row r="203" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A203" s="1" t="s">
-        <v>517</v>
+        <v>438</v>
       </c>
       <c r="B203" s="1" t="s">
-        <v>524</v>
+        <v>440</v>
       </c>
       <c r="C203" s="1" t="s">
-        <v>517</v>
+        <v>438</v>
       </c>
     </row>
     <row r="204" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A204" s="2" t="s">
-        <v>264</v>
-      </c>
-      <c r="B204" s="2" t="s">
-        <v>265</v>
-      </c>
-      <c r="C204" s="3" t="s">
-        <v>264</v>
+      <c r="A204" s="1" t="s">
+        <v>439</v>
+      </c>
+      <c r="B204" s="1" t="s">
+        <v>441</v>
+      </c>
+      <c r="C204" s="1" t="s">
+        <v>439</v>
       </c>
     </row>
     <row r="205" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A205" s="2" t="s">
-        <v>402</v>
-      </c>
-      <c r="B205" s="2" t="s">
-        <v>403</v>
-      </c>
-      <c r="C205" s="2" t="s">
-        <v>402</v>
+      <c r="A205" s="1" t="s">
+        <v>515</v>
+      </c>
+      <c r="B205" s="1" t="s">
+        <v>522</v>
+      </c>
+      <c r="C205" s="1" t="s">
+        <v>515</v>
       </c>
     </row>
     <row r="206" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A206" s="2" t="s">
-        <v>376</v>
+        <v>262</v>
       </c>
       <c r="B206" s="2" t="s">
-        <v>377</v>
-      </c>
-      <c r="C206" s="2" t="s">
-        <v>376</v>
+        <v>263</v>
+      </c>
+      <c r="C206" s="3" t="s">
+        <v>262</v>
       </c>
     </row>
     <row r="207" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A207" s="2" t="s">
-        <v>266</v>
+        <v>400</v>
       </c>
       <c r="B207" s="2" t="s">
         <v>401</v>
       </c>
       <c r="C207" s="2" t="s">
-        <v>266</v>
+        <v>400</v>
       </c>
     </row>
     <row r="208" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A208" s="2" t="s">
-        <v>267</v>
+        <v>374</v>
       </c>
       <c r="B208" s="2" t="s">
-        <v>268</v>
-      </c>
-      <c r="C208" s="3" t="s">
-        <v>267</v>
+        <v>375</v>
+      </c>
+      <c r="C208" s="2" t="s">
+        <v>374</v>
       </c>
     </row>
     <row r="209" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A209" s="2" t="s">
-        <v>269</v>
+        <v>264</v>
       </c>
       <c r="B209" s="2" t="s">
-        <v>270</v>
+        <v>399</v>
       </c>
       <c r="C209" s="2" t="s">
-        <v>269</v>
+        <v>264</v>
       </c>
     </row>
     <row r="210" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A210" s="1" t="s">
-        <v>405</v>
+      <c r="A210" s="2" t="s">
+        <v>265</v>
       </c>
       <c r="B210" s="2" t="s">
-        <v>416</v>
-      </c>
-      <c r="C210" s="1" t="s">
-        <v>405</v>
+        <v>266</v>
+      </c>
+      <c r="C210" s="3" t="s">
+        <v>265</v>
       </c>
     </row>
     <row r="211" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A211" s="2" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
       <c r="B211" s="2" t="s">
-        <v>272</v>
-      </c>
-      <c r="C211" s="3" t="s">
-        <v>271</v>
+        <v>268</v>
+      </c>
+      <c r="C211" s="2" t="s">
+        <v>267</v>
       </c>
     </row>
     <row r="212" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A212" s="2" t="s">
-        <v>273</v>
+      <c r="A212" s="1" t="s">
+        <v>403</v>
       </c>
       <c r="B212" s="2" t="s">
-        <v>274</v>
-      </c>
-      <c r="C212" s="2" t="s">
-        <v>273</v>
+        <v>414</v>
+      </c>
+      <c r="C212" s="1" t="s">
+        <v>403</v>
       </c>
     </row>
     <row r="213" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A213" s="2" t="s">
-        <v>275</v>
+        <v>269</v>
       </c>
       <c r="B213" s="2" t="s">
-        <v>276</v>
+        <v>270</v>
       </c>
       <c r="C213" s="3" t="s">
-        <v>275</v>
+        <v>269</v>
       </c>
     </row>
     <row r="214" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A214" s="2" t="s">
-        <v>9</v>
+        <v>271</v>
       </c>
       <c r="B214" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C214" s="3" t="s">
-        <v>9</v>
+        <v>272</v>
+      </c>
+      <c r="C214" s="2" t="s">
+        <v>271</v>
       </c>
     </row>
     <row r="215" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A215" s="2" t="s">
-        <v>508</v>
+        <v>273</v>
       </c>
       <c r="B215" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C215" s="2" t="s">
-        <v>508</v>
+        <v>274</v>
+      </c>
+      <c r="C215" s="3" t="s">
+        <v>273</v>
       </c>
     </row>
     <row r="216" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A216" s="2" t="s">
-        <v>277</v>
+        <v>9</v>
       </c>
       <c r="B216" s="2" t="s">
-        <v>278</v>
+        <v>10</v>
       </c>
       <c r="C216" s="3" t="s">
-        <v>277</v>
+        <v>9</v>
       </c>
     </row>
     <row r="217" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A217" s="1" t="s">
-        <v>475</v>
+      <c r="A217" s="2" t="s">
+        <v>506</v>
       </c>
       <c r="B217" s="2" t="s">
-        <v>486</v>
-      </c>
-      <c r="C217" s="1" t="s">
-        <v>475</v>
+        <v>1</v>
+      </c>
+      <c r="C217" s="2" t="s">
+        <v>506</v>
       </c>
     </row>
     <row r="218" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A218" s="2" t="s">
-        <v>380</v>
+        <v>275</v>
       </c>
       <c r="B218" s="2" t="s">
-        <v>381</v>
-      </c>
-      <c r="C218" s="2" t="s">
-        <v>380</v>
+        <v>276</v>
+      </c>
+      <c r="C218" s="3" t="s">
+        <v>275</v>
       </c>
     </row>
     <row r="219" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A219" s="2" t="s">
-        <v>279</v>
+      <c r="A219" s="1" t="s">
+        <v>473</v>
       </c>
       <c r="B219" s="2" t="s">
-        <v>280</v>
-      </c>
-      <c r="C219" s="3" t="s">
-        <v>279</v>
+        <v>484</v>
+      </c>
+      <c r="C219" s="1" t="s">
+        <v>473</v>
       </c>
     </row>
     <row r="220" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A220" s="1" t="s">
-        <v>480</v>
+      <c r="A220" s="2" t="s">
+        <v>378</v>
       </c>
       <c r="B220" s="2" t="s">
-        <v>492</v>
-      </c>
-      <c r="C220" s="1" t="s">
-        <v>480</v>
+        <v>379</v>
+      </c>
+      <c r="C220" s="2" t="s">
+        <v>378</v>
       </c>
     </row>
     <row r="221" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A221" s="1" t="s">
-        <v>504</v>
+      <c r="A221" s="2" t="s">
+        <v>277</v>
       </c>
       <c r="B221" s="2" t="s">
-        <v>505</v>
-      </c>
-      <c r="C221" s="1" t="s">
-        <v>504</v>
+        <v>278</v>
+      </c>
+      <c r="C221" s="3" t="s">
+        <v>277</v>
       </c>
     </row>
     <row r="222" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A222" s="2" t="s">
-        <v>281</v>
+      <c r="A222" s="1" t="s">
+        <v>478</v>
       </c>
       <c r="B222" s="2" t="s">
-        <v>282</v>
-      </c>
-      <c r="C222" s="3" t="s">
-        <v>281</v>
+        <v>490</v>
+      </c>
+      <c r="C222" s="1" t="s">
+        <v>478</v>
       </c>
     </row>
     <row r="223" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A223" s="2" t="s">
-        <v>5</v>
+      <c r="A223" s="1" t="s">
+        <v>502</v>
       </c>
       <c r="B223" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C223" s="3" t="s">
-        <v>5</v>
+        <v>503</v>
+      </c>
+      <c r="C223" s="1" t="s">
+        <v>502</v>
       </c>
     </row>
     <row r="224" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A224" s="2" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
       <c r="B224" s="2" t="s">
-        <v>284</v>
-      </c>
-      <c r="C224" s="2" t="s">
-        <v>283</v>
+        <v>280</v>
+      </c>
+      <c r="C224" s="3" t="s">
+        <v>279</v>
       </c>
     </row>
     <row r="225" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A225" s="2" t="s">
-        <v>285</v>
+        <v>5</v>
       </c>
       <c r="B225" s="2" t="s">
-        <v>286</v>
+        <v>6</v>
       </c>
       <c r="C225" s="3" t="s">
-        <v>285</v>
+        <v>5</v>
       </c>
     </row>
     <row r="226" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A226" s="2" t="s">
-        <v>287</v>
+        <v>281</v>
       </c>
       <c r="B226" s="2" t="s">
-        <v>286</v>
-      </c>
-      <c r="C226" s="3" t="s">
-        <v>287</v>
+        <v>282</v>
+      </c>
+      <c r="C226" s="2" t="s">
+        <v>281</v>
       </c>
     </row>
     <row r="227" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A227" s="2" t="s">
-        <v>288</v>
+        <v>283</v>
       </c>
       <c r="B227" s="2" t="s">
-        <v>289</v>
+        <v>284</v>
       </c>
       <c r="C227" s="3" t="s">
-        <v>288</v>
+        <v>283</v>
       </c>
     </row>
     <row r="228" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A228" s="2" t="s">
-        <v>290</v>
+        <v>285</v>
       </c>
       <c r="B228" s="2" t="s">
-        <v>291</v>
+        <v>284</v>
       </c>
       <c r="C228" s="3" t="s">
-        <v>290</v>
+        <v>285</v>
       </c>
     </row>
     <row r="229" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A229" s="2" t="s">
-        <v>292</v>
+        <v>286</v>
       </c>
       <c r="B229" s="2" t="s">
-        <v>293</v>
+        <v>287</v>
       </c>
       <c r="C229" s="3" t="s">
-        <v>292</v>
+        <v>286</v>
       </c>
     </row>
     <row r="230" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A230" s="2" t="s">
-        <v>294</v>
+        <v>288</v>
       </c>
       <c r="B230" s="2" t="s">
-        <v>295</v>
+        <v>289</v>
       </c>
       <c r="C230" s="3" t="s">
-        <v>294</v>
+        <v>288</v>
       </c>
     </row>
     <row r="231" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A231" s="2" t="s">
-        <v>296</v>
+        <v>290</v>
       </c>
       <c r="B231" s="2" t="s">
-        <v>297</v>
+        <v>291</v>
       </c>
       <c r="C231" s="3" t="s">
-        <v>296</v>
+        <v>290</v>
       </c>
     </row>
     <row r="232" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A232" s="2" t="s">
-        <v>298</v>
+        <v>292</v>
       </c>
       <c r="B232" s="2" t="s">
-        <v>299</v>
+        <v>293</v>
       </c>
       <c r="C232" s="3" t="s">
-        <v>298</v>
+        <v>292</v>
       </c>
     </row>
     <row r="233" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A233" s="2" t="s">
-        <v>300</v>
+        <v>294</v>
       </c>
       <c r="B233" s="2" t="s">
-        <v>301</v>
-      </c>
-      <c r="C233" s="2" t="s">
-        <v>300</v>
+        <v>295</v>
+      </c>
+      <c r="C233" s="3" t="s">
+        <v>294</v>
       </c>
     </row>
     <row r="234" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A234" s="1" t="s">
-        <v>411</v>
+      <c r="A234" s="2" t="s">
+        <v>296</v>
       </c>
       <c r="B234" s="2" t="s">
-        <v>420</v>
-      </c>
-      <c r="C234" s="1" t="s">
-        <v>411</v>
+        <v>297</v>
+      </c>
+      <c r="C234" s="3" t="s">
+        <v>296</v>
       </c>
     </row>
     <row r="235" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A235" s="2" t="s">
-        <v>302</v>
+        <v>298</v>
       </c>
       <c r="B235" s="2" t="s">
-        <v>303</v>
-      </c>
-      <c r="C235" s="3" t="s">
-        <v>302</v>
+        <v>299</v>
+      </c>
+      <c r="C235" s="2" t="s">
+        <v>298</v>
       </c>
     </row>
     <row r="236" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A236" s="1" t="s">
-        <v>474</v>
+        <v>409</v>
       </c>
       <c r="B236" s="2" t="s">
-        <v>485</v>
+        <v>418</v>
       </c>
       <c r="C236" s="1" t="s">
-        <v>474</v>
+        <v>409</v>
       </c>
     </row>
     <row r="237" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A237" s="2" t="s">
-        <v>304</v>
+        <v>300</v>
       </c>
       <c r="B237" s="2" t="s">
-        <v>305</v>
+        <v>301</v>
       </c>
       <c r="C237" s="3" t="s">
-        <v>304</v>
+        <v>300</v>
       </c>
     </row>
     <row r="238" spans="1:3" x14ac:dyDescent="0.45">
@@ -4592,345 +4604,367 @@
         <v>472</v>
       </c>
       <c r="B238" s="2" t="s">
-        <v>488</v>
+        <v>483</v>
       </c>
       <c r="C238" s="1" t="s">
         <v>472</v>
       </c>
     </row>
     <row r="239" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A239" s="1" t="s">
-        <v>415</v>
-      </c>
-      <c r="B239" s="1" t="s">
-        <v>422</v>
-      </c>
-      <c r="C239" s="1" t="s">
-        <v>415</v>
+      <c r="A239" s="2" t="s">
+        <v>302</v>
+      </c>
+      <c r="B239" s="2" t="s">
+        <v>303</v>
+      </c>
+      <c r="C239" s="3" t="s">
+        <v>302</v>
       </c>
     </row>
     <row r="240" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A240" s="1" t="s">
-        <v>476</v>
+        <v>470</v>
       </c>
       <c r="B240" s="2" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="C240" s="1" t="s">
-        <v>476</v>
+        <v>470</v>
       </c>
     </row>
     <row r="241" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A241" s="2" t="s">
-        <v>306</v>
-      </c>
-      <c r="B241" s="2" t="s">
-        <v>307</v>
-      </c>
-      <c r="C241" s="3" t="s">
-        <v>306</v>
+      <c r="A241" s="1" t="s">
+        <v>413</v>
+      </c>
+      <c r="B241" s="1" t="s">
+        <v>420</v>
+      </c>
+      <c r="C241" s="1" t="s">
+        <v>413</v>
       </c>
     </row>
     <row r="242" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A242" s="1" t="s">
-        <v>494</v>
+        <v>474</v>
       </c>
       <c r="B242" s="2" t="s">
-        <v>495</v>
+        <v>485</v>
       </c>
       <c r="C242" s="1" t="s">
-        <v>494</v>
+        <v>474</v>
       </c>
     </row>
     <row r="243" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A243" s="2" t="s">
-        <v>308</v>
+        <v>304</v>
       </c>
       <c r="B243" s="2" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
       <c r="C243" s="3" t="s">
-        <v>308</v>
+        <v>304</v>
       </c>
     </row>
     <row r="244" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A244" s="2" t="s">
-        <v>310</v>
+      <c r="A244" s="1" t="s">
+        <v>492</v>
       </c>
       <c r="B244" s="2" t="s">
-        <v>311</v>
-      </c>
-      <c r="C244" s="3" t="s">
-        <v>310</v>
+        <v>493</v>
+      </c>
+      <c r="C244" s="1" t="s">
+        <v>492</v>
       </c>
     </row>
     <row r="245" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A245" s="2" t="s">
-        <v>312</v>
+        <v>306</v>
       </c>
       <c r="B245" s="2" t="s">
-        <v>313</v>
+        <v>307</v>
       </c>
       <c r="C245" s="3" t="s">
-        <v>312</v>
+        <v>306</v>
       </c>
     </row>
     <row r="246" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A246" s="1" t="s">
-        <v>410</v>
+      <c r="A246" s="2" t="s">
+        <v>308</v>
       </c>
       <c r="B246" s="2" t="s">
-        <v>425</v>
-      </c>
-      <c r="C246" s="1" t="s">
-        <v>410</v>
+        <v>309</v>
+      </c>
+      <c r="C246" s="3" t="s">
+        <v>308</v>
       </c>
     </row>
     <row r="247" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A247" s="2" t="s">
-        <v>366</v>
+        <v>310</v>
       </c>
       <c r="B247" s="2" t="s">
-        <v>367</v>
-      </c>
-      <c r="C247" s="2" t="s">
-        <v>366</v>
+        <v>311</v>
+      </c>
+      <c r="C247" s="3" t="s">
+        <v>310</v>
       </c>
     </row>
     <row r="248" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A248" s="2" t="s">
-        <v>372</v>
+      <c r="A248" s="1" t="s">
+        <v>408</v>
       </c>
       <c r="B248" s="2" t="s">
-        <v>373</v>
-      </c>
-      <c r="C248" s="2" t="s">
-        <v>372</v>
+        <v>423</v>
+      </c>
+      <c r="C248" s="1" t="s">
+        <v>408</v>
       </c>
     </row>
     <row r="249" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A249" s="2" t="s">
-        <v>314</v>
+        <v>364</v>
       </c>
       <c r="B249" s="2" t="s">
-        <v>315</v>
-      </c>
-      <c r="C249" s="3" t="s">
-        <v>314</v>
+        <v>365</v>
+      </c>
+      <c r="C249" s="2" t="s">
+        <v>364</v>
       </c>
     </row>
     <row r="250" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A250" s="2" t="s">
-        <v>11</v>
+        <v>370</v>
       </c>
       <c r="B250" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C250" s="3" t="s">
-        <v>11</v>
+        <v>371</v>
+      </c>
+      <c r="C250" s="2" t="s">
+        <v>370</v>
       </c>
     </row>
     <row r="251" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A251" s="2" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="B251" s="2" t="s">
-        <v>317</v>
-      </c>
-      <c r="C251" s="2" t="s">
-        <v>316</v>
+        <v>313</v>
+      </c>
+      <c r="C251" s="3" t="s">
+        <v>312</v>
       </c>
     </row>
     <row r="252" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A252" s="2" t="s">
-        <v>318</v>
+        <v>11</v>
       </c>
       <c r="B252" s="2" t="s">
-        <v>319</v>
+        <v>12</v>
       </c>
       <c r="C252" s="3" t="s">
-        <v>318</v>
+        <v>11</v>
       </c>
     </row>
     <row r="253" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A253" s="2" t="s">
-        <v>320</v>
+        <v>314</v>
       </c>
       <c r="B253" s="2" t="s">
-        <v>321</v>
-      </c>
-      <c r="C253" s="3" t="s">
-        <v>320</v>
+        <v>315</v>
+      </c>
+      <c r="C253" s="2" t="s">
+        <v>314</v>
       </c>
     </row>
     <row r="254" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A254" s="2" t="s">
-        <v>322</v>
+        <v>316</v>
       </c>
       <c r="B254" s="2" t="s">
-        <v>323</v>
-      </c>
-      <c r="C254" s="2" t="s">
-        <v>322</v>
+        <v>317</v>
+      </c>
+      <c r="C254" s="3" t="s">
+        <v>316</v>
       </c>
     </row>
     <row r="255" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A255" s="1" t="s">
-        <v>447</v>
-      </c>
-      <c r="B255" s="1" t="s">
-        <v>449</v>
-      </c>
-      <c r="C255" s="1" t="s">
-        <v>447</v>
+      <c r="A255" s="2" t="s">
+        <v>318</v>
+      </c>
+      <c r="B255" s="2" t="s">
+        <v>319</v>
+      </c>
+      <c r="C255" s="3" t="s">
+        <v>318</v>
       </c>
     </row>
     <row r="256" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A256" s="2" t="s">
-        <v>324</v>
+        <v>320</v>
       </c>
       <c r="B256" s="2" t="s">
-        <v>325</v>
-      </c>
-      <c r="C256" s="3" t="s">
-        <v>324</v>
+        <v>321</v>
+      </c>
+      <c r="C256" s="2" t="s">
+        <v>320</v>
       </c>
     </row>
     <row r="257" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A257" s="2" t="s">
-        <v>326</v>
-      </c>
-      <c r="B257" s="2" t="s">
-        <v>327</v>
-      </c>
-      <c r="C257" s="2" t="s">
-        <v>326</v>
+      <c r="A257" s="1" t="s">
+        <v>445</v>
+      </c>
+      <c r="B257" s="1" t="s">
+        <v>447</v>
+      </c>
+      <c r="C257" s="1" t="s">
+        <v>445</v>
       </c>
     </row>
     <row r="258" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A258" s="2" t="s">
-        <v>328</v>
+        <v>322</v>
       </c>
       <c r="B258" s="2" t="s">
-        <v>329</v>
-      </c>
-      <c r="C258" s="2" t="s">
-        <v>328</v>
+        <v>323</v>
+      </c>
+      <c r="C258" s="3" t="s">
+        <v>322</v>
       </c>
     </row>
     <row r="259" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A259" s="2" t="s">
-        <v>330</v>
+        <v>324</v>
       </c>
       <c r="B259" s="2" t="s">
-        <v>331</v>
-      </c>
-      <c r="C259" s="3" t="s">
-        <v>330</v>
+        <v>325</v>
+      </c>
+      <c r="C259" s="2" t="s">
+        <v>324</v>
       </c>
     </row>
     <row r="260" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A260" s="2" t="s">
-        <v>427</v>
+        <v>326</v>
       </c>
       <c r="B260" s="2" t="s">
-        <v>430</v>
+        <v>327</v>
       </c>
       <c r="C260" s="2" t="s">
-        <v>427</v>
+        <v>326</v>
       </c>
     </row>
     <row r="261" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A261" s="2" t="s">
-        <v>332</v>
+        <v>328</v>
       </c>
       <c r="B261" s="2" t="s">
-        <v>333</v>
-      </c>
-      <c r="C261" s="2" t="s">
-        <v>332</v>
+        <v>329</v>
+      </c>
+      <c r="C261" s="3" t="s">
+        <v>328</v>
       </c>
     </row>
     <row r="262" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A262" s="1" t="s">
-        <v>511</v>
+      <c r="A262" s="2" t="s">
+        <v>425</v>
       </c>
       <c r="B262" s="2" t="s">
-        <v>518</v>
-      </c>
-      <c r="C262" s="1" t="s">
-        <v>511</v>
+        <v>428</v>
+      </c>
+      <c r="C262" s="2" t="s">
+        <v>425</v>
       </c>
     </row>
     <row r="263" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A263" s="1" t="s">
-        <v>513</v>
+      <c r="A263" s="2" t="s">
+        <v>330</v>
       </c>
       <c r="B263" s="2" t="s">
-        <v>520</v>
-      </c>
-      <c r="C263" s="1" t="s">
-        <v>513</v>
+        <v>331</v>
+      </c>
+      <c r="C263" s="2" t="s">
+        <v>330</v>
       </c>
     </row>
     <row r="264" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A264" s="1" t="s">
-        <v>512</v>
+        <v>509</v>
       </c>
       <c r="B264" s="2" t="s">
-        <v>519</v>
+        <v>516</v>
       </c>
       <c r="C264" s="1" t="s">
-        <v>512</v>
+        <v>509</v>
       </c>
     </row>
     <row r="265" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A265" s="2" t="s">
-        <v>334</v>
+      <c r="A265" s="1" t="s">
+        <v>511</v>
       </c>
       <c r="B265" s="2" t="s">
-        <v>335</v>
-      </c>
-      <c r="C265" s="3" t="s">
-        <v>334</v>
+        <v>518</v>
+      </c>
+      <c r="C265" s="1" t="s">
+        <v>511</v>
       </c>
     </row>
     <row r="266" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A266" s="2" t="s">
-        <v>336</v>
+      <c r="A266" s="1" t="s">
+        <v>510</v>
       </c>
       <c r="B266" s="2" t="s">
-        <v>337</v>
-      </c>
-      <c r="C266" s="3" t="s">
-        <v>336</v>
+        <v>517</v>
+      </c>
+      <c r="C266" s="1" t="s">
+        <v>510</v>
       </c>
     </row>
     <row r="267" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A267" s="2" t="s">
-        <v>368</v>
+        <v>332</v>
       </c>
       <c r="B267" s="2" t="s">
-        <v>369</v>
-      </c>
-      <c r="C267" s="2" t="s">
-        <v>368</v>
+        <v>333</v>
+      </c>
+      <c r="C267" s="3" t="s">
+        <v>332</v>
       </c>
     </row>
     <row r="268" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A268" s="2" t="s">
-        <v>344</v>
+        <v>334</v>
       </c>
       <c r="B268" s="2" t="s">
-        <v>345</v>
+        <v>335</v>
       </c>
       <c r="C268" s="3" t="s">
-        <v>344</v>
+        <v>334</v>
+      </c>
+    </row>
+    <row r="269" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A269" s="2" t="s">
+        <v>366</v>
+      </c>
+      <c r="B269" s="2" t="s">
+        <v>367</v>
+      </c>
+      <c r="C269" s="2" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="270" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A270" s="2" t="s">
+        <v>342</v>
+      </c>
+      <c r="B270" s="2" t="s">
+        <v>343</v>
+      </c>
+      <c r="C270" s="3" t="s">
+        <v>342</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:C1" xr:uid="{56EE5BC3-7B0A-4577-92C7-56F73F7DDC8B}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C268">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C270">
       <sortCondition ref="A1"/>
     </sortState>
   </autoFilter>

</xml_diff>

<commit_message>
Updates to descriptive statistics, grouping for normality tests
</commit_message>
<xml_diff>
--- a/translations/source.xlsx
+++ b/translations/source.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/e6c7874704bc5dfb/Documents/R Studio/DataSuite/translations/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="237" documentId="8_{D77EC384-F39F-4BA6-8963-4B8AF986F7DE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{74E0BBAB-F522-43AB-A081-5DE5C0F0188C}"/>
+  <xr:revisionPtr revIDLastSave="276" documentId="8_{D77EC384-F39F-4BA6-8963-4B8AF986F7DE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{5B4140CA-931A-48CA-80DD-68CC15B7E4E6}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="16395" xr2:uid="{BD840C99-A56D-4EBC-B1B7-A6018ADC22A6}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="810" uniqueCount="529">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="861" uniqueCount="563">
   <si>
     <t>base</t>
   </si>
@@ -1621,6 +1621,108 @@
   </si>
   <si>
     <t>{method_title} for normality of distribution</t>
+  </si>
+  <si>
+    <t>Мода</t>
+  </si>
+  <si>
+    <t>Несколько</t>
+  </si>
+  <si>
+    <t>Mode</t>
+  </si>
+  <si>
+    <t>Multiple</t>
+  </si>
+  <si>
+    <t>Крайние значения</t>
+  </si>
+  <si>
+    <t>Размах</t>
+  </si>
+  <si>
+    <t>Стандартная ошибка среднего</t>
+  </si>
+  <si>
+    <t>Дисперсия</t>
+  </si>
+  <si>
+    <t>Коридор нормы</t>
+  </si>
+  <si>
+    <t>Доверительный интервал</t>
+  </si>
+  <si>
+    <t>Квартили</t>
+  </si>
+  <si>
+    <t>Квартильный размах</t>
+  </si>
+  <si>
+    <t>Эксцесс</t>
+  </si>
+  <si>
+    <t>Асимметрия</t>
+  </si>
+  <si>
+    <t>Inter-Quartile Range</t>
+  </si>
+  <si>
+    <t>Quartiles</t>
+  </si>
+  <si>
+    <t>Extrema</t>
+  </si>
+  <si>
+    <t>Range</t>
+  </si>
+  <si>
+    <t>Variance</t>
+  </si>
+  <si>
+    <t>Confidence Interval</t>
+  </si>
+  <si>
+    <t>Mean ± SD</t>
+  </si>
+  <si>
+    <t>Mean Standard Error</t>
+  </si>
+  <si>
+    <t>Mean Absolute Deviation</t>
+  </si>
+  <si>
+    <t>Среднее абсолютное отклонение</t>
+  </si>
+  <si>
+    <t>Kurtosis</t>
+  </si>
+  <si>
+    <t>Skewness</t>
+  </si>
+  <si>
+    <t>Частота моды</t>
+  </si>
+  <si>
+    <t>Frequency of Mode</t>
+  </si>
+  <si>
+    <t>Рассчитать</t>
+  </si>
+  <si>
+    <t>Calculate</t>
+  </si>
+  <si>
+    <t>Нижняя граница ДИ</t>
+  </si>
+  <si>
+    <t>Верхняя граница ДИ</t>
+  </si>
+  <si>
+    <t>CI Upper Boundary</t>
+  </si>
+  <si>
+    <t>CI Lower Boundary</t>
   </si>
 </sst>
 </file>
@@ -1978,10 +2080,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C853ECA4-158B-4D85-A448-9ECE56776B5F}">
-  <dimension ref="A1:C270"/>
+  <dimension ref="A1:C287"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A100" workbookViewId="0">
-      <selection activeCell="B107" sqref="B107"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -2016,2955 +2118,3142 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A3" s="2" t="s">
-        <v>13</v>
+        <v>527</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>14</v>
+        <v>528</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>13</v>
+        <v>527</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A4" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>14</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A5" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A6" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B6" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C6" s="3" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A6" s="1" t="s">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A7" s="1" t="s">
         <v>443</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B7" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C7" s="1" t="s">
         <v>443</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A7" s="2" t="s">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A8" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B8" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C8" s="3" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A8" s="1" t="s">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A9" s="1" t="s">
         <v>442</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B9" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="C9" s="1" t="s">
         <v>442</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A9" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A10" s="2" t="s">
-        <v>380</v>
+        <v>20</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>381</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>380</v>
+        <v>21</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A11" s="2" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A12" s="2" t="s">
-        <v>433</v>
+        <v>382</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>23</v>
+        <v>383</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>433</v>
+        <v>382</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A13" s="2" t="s">
-        <v>22</v>
+        <v>433</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C13" s="3" t="s">
-        <v>22</v>
+      <c r="C13" s="2" t="s">
+        <v>433</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A14" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A15" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A16" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>27</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A17" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A18" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>30</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A19" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A20" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>33</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A21" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A22" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>36</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A23" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A24" s="2" t="s">
         <v>450</v>
       </c>
-      <c r="B23" s="2" t="s">
+      <c r="B24" s="2" t="s">
         <v>451</v>
       </c>
-      <c r="C23" s="3" t="s">
+      <c r="C24" s="3" t="s">
         <v>450</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A24" s="1" t="s">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A25" s="1" t="s">
         <v>469</v>
       </c>
-      <c r="B24" s="2" t="s">
+      <c r="B25" s="2" t="s">
         <v>481</v>
       </c>
-      <c r="C24" s="1" t="s">
+      <c r="C25" s="1" t="s">
         <v>469</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A25" s="2" t="s">
-        <v>356</v>
-      </c>
-      <c r="B25" s="2" t="s">
-        <v>357</v>
-      </c>
-      <c r="C25" s="3" t="s">
-        <v>356</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A26" s="2" t="s">
-        <v>38</v>
+        <v>356</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>39</v>
+        <v>357</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>38</v>
+        <v>356</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A27" s="2" t="s">
-        <v>7</v>
+        <v>38</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>8</v>
+        <v>39</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>7</v>
+        <v>38</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A28" s="2" t="s">
-        <v>40</v>
+        <v>7</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>434</v>
+        <v>8</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>40</v>
+        <v>7</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A29" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>42</v>
+        <v>434</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A30" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A31" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="B30" s="2" t="s">
+      <c r="B31" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="C30" s="3" t="s">
+      <c r="C31" s="3" t="s">
         <v>43</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A31" s="1" t="s">
-        <v>514</v>
-      </c>
-      <c r="B31" s="1" t="s">
-        <v>520</v>
-      </c>
-      <c r="C31" s="1" t="s">
-        <v>514</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A32" s="1" t="s">
-        <v>513</v>
+        <v>542</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>521</v>
+        <v>554</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>513</v>
+        <v>542</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A33" s="2" t="s">
-        <v>384</v>
-      </c>
-      <c r="B33" s="2" t="s">
-        <v>385</v>
-      </c>
-      <c r="C33" s="2" t="s">
-        <v>384</v>
+      <c r="A33" s="1" t="s">
+        <v>514</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>520</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>514</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A34" s="1" t="s">
-        <v>512</v>
-      </c>
-      <c r="B34" s="2" t="s">
-        <v>519</v>
+        <v>513</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>521</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>512</v>
+        <v>513</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A35" s="2" t="s">
-        <v>45</v>
+        <v>384</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="C35" s="3" t="s">
-        <v>45</v>
+        <v>385</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>384</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A36" s="2" t="s">
-        <v>504</v>
+      <c r="A36" s="1" t="s">
+        <v>512</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>505</v>
-      </c>
-      <c r="C36" s="2" t="s">
-        <v>504</v>
+        <v>519</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>512</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A37" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A38" s="2" t="s">
-        <v>49</v>
+        <v>504</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="C38" s="3" t="s">
-        <v>49</v>
+        <v>505</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>504</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A39" s="2" t="s">
-        <v>360</v>
+        <v>47</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>361</v>
-      </c>
-      <c r="C39" s="2" t="s">
-        <v>360</v>
+        <v>48</v>
+      </c>
+      <c r="C39" s="3" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A40" s="2" t="s">
-        <v>368</v>
+        <v>49</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>369</v>
-      </c>
-      <c r="C40" s="2" t="s">
-        <v>368</v>
+        <v>50</v>
+      </c>
+      <c r="C40" s="3" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A41" s="2" t="s">
-        <v>51</v>
+        <v>360</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="C41" s="3" t="s">
-        <v>51</v>
+        <v>361</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>360</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A42" s="2" t="s">
-        <v>390</v>
+        <v>368</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>393</v>
+        <v>369</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>390</v>
+        <v>368</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A43" s="1" t="s">
-        <v>411</v>
+      <c r="A43" s="2" t="s">
+        <v>51</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>422</v>
-      </c>
-      <c r="C43" s="1" t="s">
-        <v>411</v>
+        <v>52</v>
+      </c>
+      <c r="C43" s="3" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A44" s="2" t="s">
-        <v>53</v>
+        <v>390</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="C44" s="3" t="s">
-        <v>53</v>
+        <v>393</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>390</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A45" s="2" t="s">
-        <v>344</v>
+        <v>560</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>345</v>
-      </c>
-      <c r="C45" s="3" t="s">
-        <v>344</v>
+        <v>562</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>560</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A46" s="2" t="s">
-        <v>55</v>
+      <c r="A46" s="1" t="s">
+        <v>411</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="C46" s="3" t="s">
-        <v>55</v>
+        <v>422</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>411</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A47" s="1" t="s">
-        <v>406</v>
-      </c>
-      <c r="B47" s="1" t="s">
-        <v>424</v>
-      </c>
-      <c r="C47" s="1" t="s">
-        <v>406</v>
+      <c r="A47" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="C47" s="3" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A48" s="2" t="s">
-        <v>57</v>
+        <v>344</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>58</v>
+        <v>345</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>57</v>
+        <v>344</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A49" s="2" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="C49" s="3" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A50" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="B50" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="C50" s="3" t="s">
-        <v>61</v>
+      <c r="A50" s="1" t="s">
+        <v>406</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>424</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>406</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A51" s="2" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="C51" s="2" t="s">
-        <v>63</v>
+        <v>58</v>
+      </c>
+      <c r="C51" s="3" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A52" s="1" t="s">
-        <v>507</v>
+      <c r="A52" s="2" t="s">
+        <v>59</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>508</v>
-      </c>
-      <c r="C52" s="1" t="s">
-        <v>507</v>
+        <v>60</v>
+      </c>
+      <c r="C52" s="3" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A53" s="2" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="C53" s="2" t="s">
-        <v>65</v>
+        <v>62</v>
+      </c>
+      <c r="C53" s="3" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A54" s="2" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="C54" s="3" t="s">
-        <v>67</v>
+        <v>64</v>
+      </c>
+      <c r="C54" s="2" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A55" s="2" t="s">
-        <v>69</v>
+      <c r="A55" s="1" t="s">
+        <v>507</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="C55" s="3" t="s">
-        <v>69</v>
+        <v>508</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>507</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A56" s="2" t="s">
-        <v>465</v>
+        <v>65</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>467</v>
+        <v>66</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>465</v>
+        <v>65</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A57" s="2" t="s">
-        <v>336</v>
+        <v>67</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>337</v>
+        <v>68</v>
       </c>
       <c r="C57" s="3" t="s">
-        <v>336</v>
+        <v>67</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A58" s="2" t="s">
-        <v>348</v>
+        <v>69</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>349</v>
-      </c>
-      <c r="C58" s="2" t="s">
-        <v>348</v>
+        <v>70</v>
+      </c>
+      <c r="C58" s="3" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A59" s="1" t="s">
-        <v>436</v>
-      </c>
-      <c r="B59" s="1" t="s">
-        <v>437</v>
-      </c>
-      <c r="C59" s="1" t="s">
-        <v>436</v>
+      <c r="A59" s="2" t="s">
+        <v>465</v>
+      </c>
+      <c r="B59" s="2" t="s">
+        <v>467</v>
+      </c>
+      <c r="C59" s="2" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A60" s="2" t="s">
-        <v>71</v>
+        <v>336</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>72</v>
+        <v>337</v>
       </c>
       <c r="C60" s="3" t="s">
-        <v>71</v>
+        <v>336</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A61" s="2" t="s">
-        <v>73</v>
+        <v>348</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="C61" s="3" t="s">
-        <v>73</v>
+        <v>349</v>
+      </c>
+      <c r="C61" s="2" t="s">
+        <v>348</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A62" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="B62" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="C62" s="3" t="s">
-        <v>75</v>
+      <c r="A62" s="1" t="s">
+        <v>436</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>437</v>
+      </c>
+      <c r="C62" s="1" t="s">
+        <v>436</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A63" s="2" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="C63" s="3" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A64" s="2" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="C64" s="3" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A65" s="2" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="C65" s="3" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A66" s="2" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="C66" s="2" t="s">
-        <v>83</v>
+        <v>78</v>
+      </c>
+      <c r="C66" s="3" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A67" s="2" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="C67" s="3" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A68" s="2" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="C68" s="3" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A69" s="2" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="C69" s="3" t="s">
-        <v>89</v>
+        <v>84</v>
+      </c>
+      <c r="C69" s="2" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A70" s="1" t="s">
-        <v>405</v>
+      <c r="A70" s="2" t="s">
+        <v>85</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>416</v>
-      </c>
-      <c r="C70" s="1" t="s">
-        <v>405</v>
+        <v>86</v>
+      </c>
+      <c r="C70" s="3" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A71" s="1" t="s">
-        <v>404</v>
+      <c r="A71" s="2" t="s">
+        <v>87</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>415</v>
-      </c>
-      <c r="C71" s="1" t="s">
-        <v>404</v>
+        <v>88</v>
+      </c>
+      <c r="C71" s="3" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A72" s="2" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="C72" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
+      </c>
+      <c r="C72" s="3" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A73" s="2" t="s">
-        <v>372</v>
+      <c r="A73" s="1" t="s">
+        <v>405</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>373</v>
-      </c>
-      <c r="C73" s="2" t="s">
-        <v>372</v>
+        <v>416</v>
+      </c>
+      <c r="C73" s="1" t="s">
+        <v>405</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A74" s="2" t="s">
-        <v>93</v>
+      <c r="A74" s="1" t="s">
+        <v>404</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="C74" s="3" t="s">
-        <v>93</v>
+        <v>415</v>
+      </c>
+      <c r="C74" s="1" t="s">
+        <v>404</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A75" s="2" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>435</v>
-      </c>
-      <c r="C75" s="3" t="s">
-        <v>95</v>
+        <v>92</v>
+      </c>
+      <c r="C75" s="2" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A76" s="2" t="s">
-        <v>96</v>
+        <v>372</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="C76" s="3" t="s">
-        <v>96</v>
+        <v>373</v>
+      </c>
+      <c r="C76" s="2" t="s">
+        <v>372</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A77" s="2" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="C77" s="3" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A78" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>101</v>
+        <v>435</v>
       </c>
       <c r="C78" s="3" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A79" s="2" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="C79" s="3" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A80" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="B80" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="C80" s="3" t="s">
-        <v>104</v>
+      <c r="A80" s="1" t="s">
+        <v>536</v>
+      </c>
+      <c r="B80" s="1" t="s">
+        <v>547</v>
+      </c>
+      <c r="C80" s="1" t="s">
+        <v>536</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A81" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="B81" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="C81" s="3" t="s">
-        <v>106</v>
+      <c r="A81" s="1" t="s">
+        <v>538</v>
+      </c>
+      <c r="B81" s="1" t="s">
+        <v>548</v>
+      </c>
+      <c r="C81" s="1" t="s">
+        <v>538</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A82" s="2" t="s">
-        <v>498</v>
+        <v>98</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>499</v>
-      </c>
-      <c r="C82" s="2" t="s">
-        <v>498</v>
+        <v>99</v>
+      </c>
+      <c r="C82" s="3" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A83" s="2" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="B83" s="2" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="C83" s="3" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A84" s="2" t="s">
-        <v>110</v>
+        <v>102</v>
       </c>
       <c r="B84" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="C84" s="2" t="s">
-        <v>110</v>
+        <v>103</v>
+      </c>
+      <c r="C84" s="3" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A85" s="2" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
       <c r="B85" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="C85" s="2" t="s">
-        <v>112</v>
+        <v>105</v>
+      </c>
+      <c r="C85" s="3" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A86" s="2" t="s">
-        <v>114</v>
+        <v>106</v>
       </c>
       <c r="B86" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="C86" s="2" t="s">
-        <v>114</v>
+        <v>107</v>
+      </c>
+      <c r="C86" s="3" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A87" s="1" t="s">
-        <v>452</v>
+      <c r="A87" s="2" t="s">
+        <v>498</v>
       </c>
       <c r="B87" s="2" t="s">
-        <v>453</v>
-      </c>
-      <c r="C87" s="1" t="s">
-        <v>452</v>
+        <v>499</v>
+      </c>
+      <c r="C87" s="2" t="s">
+        <v>498</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A88" s="2" t="s">
-        <v>116</v>
+        <v>108</v>
       </c>
       <c r="B88" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="C88" s="2" t="s">
-        <v>116</v>
+        <v>109</v>
+      </c>
+      <c r="C88" s="3" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A89" s="2" t="s">
-        <v>456</v>
+        <v>110</v>
       </c>
       <c r="B89" s="2" t="s">
-        <v>461</v>
-      </c>
-      <c r="C89" s="3" t="s">
-        <v>456</v>
+        <v>111</v>
+      </c>
+      <c r="C89" s="2" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A90" s="2" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="B90" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="C90" s="3" t="s">
-        <v>118</v>
+        <v>113</v>
+      </c>
+      <c r="C90" s="2" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A91" s="2" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="B91" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="C91" s="3" t="s">
-        <v>120</v>
+        <v>115</v>
+      </c>
+      <c r="C91" s="2" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A92" s="2" t="s">
-        <v>122</v>
+      <c r="A92" s="1" t="s">
+        <v>452</v>
       </c>
       <c r="B92" s="2" t="s">
-        <v>123</v>
-      </c>
-      <c r="C92" s="3" t="s">
-        <v>122</v>
+        <v>453</v>
+      </c>
+      <c r="C92" s="1" t="s">
+        <v>452</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A93" s="2" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
       <c r="B93" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="C93" s="3" t="s">
-        <v>124</v>
+        <v>117</v>
+      </c>
+      <c r="C93" s="2" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A94" s="2" t="s">
-        <v>126</v>
+        <v>456</v>
       </c>
       <c r="B94" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="C94" s="2" t="s">
-        <v>126</v>
+        <v>461</v>
+      </c>
+      <c r="C94" s="3" t="s">
+        <v>456</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A95" s="2" t="s">
-        <v>362</v>
+        <v>118</v>
       </c>
       <c r="B95" s="2" t="s">
-        <v>363</v>
-      </c>
-      <c r="C95" s="2" t="s">
-        <v>362</v>
+        <v>119</v>
+      </c>
+      <c r="C95" s="3" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A96" s="2" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="B96" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="C96" s="2" t="s">
-        <v>128</v>
+        <v>121</v>
+      </c>
+      <c r="C96" s="3" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A97" s="2" t="s">
-        <v>386</v>
+        <v>122</v>
       </c>
       <c r="B97" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="C97" s="2" t="s">
-        <v>386</v>
+        <v>123</v>
+      </c>
+      <c r="C97" s="3" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A98" s="2" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="B98" s="2" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="C98" s="3" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A99" s="2" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="B99" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="C99" s="3" t="s">
-        <v>132</v>
+        <v>127</v>
+      </c>
+      <c r="C99" s="2" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A100" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="B100" s="2" t="s">
-        <v>135</v>
-      </c>
-      <c r="C100" s="2" t="s">
-        <v>134</v>
+      <c r="A100" s="1" t="s">
+        <v>539</v>
+      </c>
+      <c r="B100" s="1" t="s">
+        <v>544</v>
+      </c>
+      <c r="C100" s="1" t="s">
+        <v>539</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A101" s="2" t="s">
-        <v>136</v>
-      </c>
-      <c r="B101" s="2" t="s">
-        <v>137</v>
-      </c>
-      <c r="C101" s="3" t="s">
-        <v>136</v>
+      <c r="A101" s="1" t="s">
+        <v>540</v>
+      </c>
+      <c r="B101" s="1" t="s">
+        <v>543</v>
+      </c>
+      <c r="C101" s="1" t="s">
+        <v>540</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A102" s="1" t="s">
-        <v>407</v>
+      <c r="A102" s="2" t="s">
+        <v>362</v>
       </c>
       <c r="B102" s="2" t="s">
-        <v>417</v>
-      </c>
-      <c r="C102" s="1" t="s">
-        <v>407</v>
+        <v>363</v>
+      </c>
+      <c r="C102" s="2" t="s">
+        <v>362</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A103" s="2" t="s">
-        <v>138</v>
+        <v>128</v>
       </c>
       <c r="B103" s="2" t="s">
-        <v>139</v>
-      </c>
-      <c r="C103" s="3" t="s">
-        <v>138</v>
+        <v>129</v>
+      </c>
+      <c r="C103" s="2" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A104" s="2" t="s">
-        <v>140</v>
+        <v>386</v>
       </c>
       <c r="B104" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="C104" s="3" t="s">
-        <v>140</v>
+        <v>129</v>
+      </c>
+      <c r="C104" s="2" t="s">
+        <v>386</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A105" s="2" t="s">
-        <v>142</v>
+        <v>130</v>
       </c>
       <c r="B105" s="2" t="s">
-        <v>143</v>
+        <v>131</v>
       </c>
       <c r="C105" s="3" t="s">
-        <v>142</v>
+        <v>130</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A106" s="2" t="s">
-        <v>144</v>
+        <v>132</v>
       </c>
       <c r="B106" s="2" t="s">
-        <v>145</v>
+        <v>133</v>
       </c>
       <c r="C106" s="3" t="s">
-        <v>144</v>
+        <v>132</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A107" s="2" t="s">
-        <v>146</v>
+        <v>134</v>
       </c>
       <c r="B107" s="2" t="s">
-        <v>147</v>
-      </c>
-      <c r="C107" s="3" t="s">
-        <v>146</v>
+        <v>135</v>
+      </c>
+      <c r="C107" s="2" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A108" s="2" t="s">
-        <v>148</v>
+        <v>136</v>
       </c>
       <c r="B108" s="2" t="s">
-        <v>149</v>
+        <v>137</v>
       </c>
       <c r="C108" s="3" t="s">
-        <v>148</v>
+        <v>136</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A109" s="2" t="s">
-        <v>150</v>
+      <c r="A109" s="1" t="s">
+        <v>407</v>
       </c>
       <c r="B109" s="2" t="s">
-        <v>151</v>
-      </c>
-      <c r="C109" s="3" t="s">
-        <v>150</v>
+        <v>417</v>
+      </c>
+      <c r="C109" s="1" t="s">
+        <v>407</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A110" s="2" t="s">
-        <v>152</v>
+        <v>138</v>
       </c>
       <c r="B110" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="C110" s="2" t="s">
-        <v>152</v>
+        <v>139</v>
+      </c>
+      <c r="C110" s="3" t="s">
+        <v>138</v>
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A111" s="2" t="s">
-        <v>426</v>
+        <v>140</v>
       </c>
       <c r="B111" s="2" t="s">
-        <v>427</v>
-      </c>
-      <c r="C111" s="2" t="s">
-        <v>426</v>
+        <v>141</v>
+      </c>
+      <c r="C111" s="3" t="s">
+        <v>140</v>
       </c>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A112" s="2" t="s">
-        <v>154</v>
+        <v>142</v>
       </c>
       <c r="B112" s="2" t="s">
-        <v>155</v>
-      </c>
-      <c r="C112" s="2" t="s">
-        <v>154</v>
+        <v>143</v>
+      </c>
+      <c r="C112" s="3" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A113" s="2" t="s">
-        <v>457</v>
+        <v>144</v>
       </c>
       <c r="B113" s="2" t="s">
-        <v>460</v>
+        <v>145</v>
       </c>
       <c r="C113" s="3" t="s">
-        <v>457</v>
+        <v>144</v>
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A114" s="2" t="s">
-        <v>458</v>
+        <v>146</v>
       </c>
       <c r="B114" s="2" t="s">
-        <v>459</v>
+        <v>147</v>
       </c>
       <c r="C114" s="3" t="s">
-        <v>458</v>
+        <v>146</v>
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A115" s="1" t="s">
-        <v>412</v>
-      </c>
-      <c r="B115" s="1" t="s">
-        <v>419</v>
-      </c>
-      <c r="C115" s="1" t="s">
-        <v>412</v>
+      <c r="A115" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="B115" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="C115" s="3" t="s">
+        <v>148</v>
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A116" s="2" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="B116" s="2" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="C116" s="3" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A117" s="1" t="s">
-        <v>479</v>
+      <c r="A117" s="2" t="s">
+        <v>152</v>
       </c>
       <c r="B117" s="2" t="s">
-        <v>491</v>
-      </c>
-      <c r="C117" s="1" t="s">
-        <v>479</v>
+        <v>153</v>
+      </c>
+      <c r="C117" s="2" t="s">
+        <v>152</v>
       </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A118" s="1" t="s">
-        <v>476</v>
+      <c r="A118" s="2" t="s">
+        <v>426</v>
       </c>
       <c r="B118" s="2" t="s">
-        <v>488</v>
-      </c>
-      <c r="C118" s="1" t="s">
-        <v>476</v>
+        <v>427</v>
+      </c>
+      <c r="C118" s="2" t="s">
+        <v>426</v>
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A119" s="1" t="s">
-        <v>477</v>
+      <c r="A119" s="2" t="s">
+        <v>154</v>
       </c>
       <c r="B119" s="2" t="s">
-        <v>489</v>
-      </c>
-      <c r="C119" s="1" t="s">
-        <v>477</v>
+        <v>155</v>
+      </c>
+      <c r="C119" s="2" t="s">
+        <v>154</v>
       </c>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A120" s="2" t="s">
-        <v>158</v>
+        <v>457</v>
       </c>
       <c r="B120" s="2" t="s">
-        <v>159</v>
-      </c>
-      <c r="C120" s="2" t="s">
-        <v>158</v>
+        <v>460</v>
+      </c>
+      <c r="C120" s="3" t="s">
+        <v>457</v>
       </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A121" s="2" t="s">
-        <v>160</v>
+        <v>458</v>
       </c>
       <c r="B121" s="2" t="s">
-        <v>387</v>
+        <v>459</v>
       </c>
       <c r="C121" s="3" t="s">
-        <v>160</v>
+        <v>458</v>
       </c>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A122" s="2" t="s">
-        <v>161</v>
-      </c>
-      <c r="B122" s="2" t="s">
-        <v>162</v>
-      </c>
-      <c r="C122" s="3" t="s">
-        <v>161</v>
+      <c r="A122" s="1" t="s">
+        <v>537</v>
+      </c>
+      <c r="B122" s="1" t="s">
+        <v>549</v>
+      </c>
+      <c r="C122" s="1" t="s">
+        <v>537</v>
       </c>
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A123" s="2" t="s">
-        <v>525</v>
-      </c>
-      <c r="B123" s="2" t="s">
-        <v>526</v>
-      </c>
-      <c r="C123" s="2" t="s">
-        <v>525</v>
+      <c r="A123" s="1" t="s">
+        <v>412</v>
+      </c>
+      <c r="B123" s="1" t="s">
+        <v>419</v>
+      </c>
+      <c r="C123" s="1" t="s">
+        <v>412</v>
       </c>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A124" s="2" t="s">
-        <v>523</v>
+        <v>156</v>
       </c>
       <c r="B124" s="2" t="s">
-        <v>524</v>
-      </c>
-      <c r="C124" s="2" t="s">
-        <v>523</v>
+        <v>157</v>
+      </c>
+      <c r="C124" s="3" t="s">
+        <v>156</v>
       </c>
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A125" s="2" t="s">
-        <v>163</v>
+      <c r="A125" s="1" t="s">
+        <v>479</v>
       </c>
       <c r="B125" s="2" t="s">
-        <v>164</v>
-      </c>
-      <c r="C125" s="3" t="s">
-        <v>163</v>
+        <v>491</v>
+      </c>
+      <c r="C125" s="1" t="s">
+        <v>479</v>
       </c>
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A126" s="2" t="s">
-        <v>527</v>
+      <c r="A126" s="1" t="s">
+        <v>476</v>
       </c>
       <c r="B126" s="2" t="s">
-        <v>528</v>
-      </c>
-      <c r="C126" s="3" t="s">
-        <v>527</v>
+        <v>488</v>
+      </c>
+      <c r="C126" s="1" t="s">
+        <v>476</v>
       </c>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A127" s="2" t="s">
-        <v>165</v>
+      <c r="A127" s="1" t="s">
+        <v>477</v>
       </c>
       <c r="B127" s="2" t="s">
-        <v>166</v>
-      </c>
-      <c r="C127" s="3" t="s">
-        <v>165</v>
+        <v>489</v>
+      </c>
+      <c r="C127" s="1" t="s">
+        <v>477</v>
       </c>
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A128" s="2" t="s">
-        <v>167</v>
+        <v>158</v>
       </c>
       <c r="B128" s="2" t="s">
-        <v>168</v>
-      </c>
-      <c r="C128" s="3" t="s">
-        <v>167</v>
+        <v>159</v>
+      </c>
+      <c r="C128" s="2" t="s">
+        <v>158</v>
       </c>
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A129" s="2" t="s">
-        <v>169</v>
+        <v>160</v>
       </c>
       <c r="B129" s="2" t="s">
-        <v>170</v>
+        <v>387</v>
       </c>
       <c r="C129" s="3" t="s">
-        <v>169</v>
+        <v>160</v>
       </c>
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A130" s="2" t="s">
-        <v>171</v>
+      <c r="A130" s="1" t="s">
+        <v>533</v>
       </c>
       <c r="B130" s="2" t="s">
-        <v>162</v>
-      </c>
-      <c r="C130" s="3" t="s">
-        <v>171</v>
+        <v>545</v>
+      </c>
+      <c r="C130" s="1" t="s">
+        <v>533</v>
       </c>
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A131" s="2" t="s">
-        <v>172</v>
+        <v>161</v>
       </c>
       <c r="B131" s="2" t="s">
-        <v>173</v>
+        <v>162</v>
       </c>
       <c r="C131" s="3" t="s">
-        <v>172</v>
+        <v>161</v>
       </c>
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A132" s="1" t="s">
-        <v>471</v>
+      <c r="A132" s="2" t="s">
+        <v>525</v>
       </c>
       <c r="B132" s="2" t="s">
-        <v>482</v>
-      </c>
-      <c r="C132" s="1" t="s">
-        <v>471</v>
+        <v>526</v>
+      </c>
+      <c r="C132" s="2" t="s">
+        <v>525</v>
       </c>
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A133" s="2" t="s">
-        <v>174</v>
+        <v>523</v>
       </c>
       <c r="B133" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="C133" s="3" t="s">
-        <v>174</v>
+        <v>524</v>
+      </c>
+      <c r="C133" s="2" t="s">
+        <v>523</v>
       </c>
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A134" s="1" t="s">
-        <v>396</v>
+      <c r="A134" s="2" t="s">
+        <v>163</v>
       </c>
       <c r="B134" s="2" t="s">
-        <v>397</v>
-      </c>
-      <c r="C134" s="1" t="s">
-        <v>396</v>
+        <v>164</v>
+      </c>
+      <c r="C134" s="3" t="s">
+        <v>163</v>
       </c>
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A135" s="2" t="s">
-        <v>350</v>
+        <v>165</v>
       </c>
       <c r="B135" s="2" t="s">
-        <v>351</v>
+        <v>166</v>
       </c>
       <c r="C135" s="3" t="s">
-        <v>350</v>
+        <v>165</v>
       </c>
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A136" s="2" t="s">
-        <v>176</v>
+        <v>167</v>
       </c>
       <c r="B136" s="2" t="s">
-        <v>177</v>
-      </c>
-      <c r="C136" s="2" t="s">
-        <v>176</v>
+        <v>168</v>
+      </c>
+      <c r="C136" s="3" t="s">
+        <v>167</v>
       </c>
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A137" s="2" t="s">
-        <v>388</v>
+        <v>169</v>
       </c>
       <c r="B137" s="2" t="s">
-        <v>391</v>
-      </c>
-      <c r="C137" s="2" t="s">
-        <v>388</v>
+        <v>170</v>
+      </c>
+      <c r="C137" s="3" t="s">
+        <v>169</v>
       </c>
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A138" s="1" t="s">
-        <v>475</v>
+      <c r="A138" s="2" t="s">
+        <v>171</v>
       </c>
       <c r="B138" s="2" t="s">
-        <v>487</v>
-      </c>
-      <c r="C138" s="1" t="s">
-        <v>475</v>
+        <v>162</v>
+      </c>
+      <c r="C138" s="3" t="s">
+        <v>171</v>
       </c>
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A139" s="2" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="B139" s="2" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
       <c r="C139" s="3" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A140" s="2" t="s">
-        <v>180</v>
+      <c r="A140" s="1" t="s">
+        <v>471</v>
       </c>
       <c r="B140" s="2" t="s">
-        <v>181</v>
-      </c>
-      <c r="C140" s="3" t="s">
-        <v>180</v>
+        <v>482</v>
+      </c>
+      <c r="C140" s="1" t="s">
+        <v>471</v>
       </c>
     </row>
     <row r="141" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A141" s="2" t="s">
-        <v>182</v>
+        <v>174</v>
       </c>
       <c r="B141" s="2" t="s">
-        <v>183</v>
+        <v>175</v>
       </c>
       <c r="C141" s="3" t="s">
-        <v>182</v>
+        <v>174</v>
       </c>
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A142" s="2" t="s">
-        <v>338</v>
+      <c r="A142" s="1" t="s">
+        <v>396</v>
       </c>
       <c r="B142" s="2" t="s">
-        <v>339</v>
-      </c>
-      <c r="C142" s="3" t="s">
-        <v>338</v>
+        <v>397</v>
+      </c>
+      <c r="C142" s="1" t="s">
+        <v>396</v>
       </c>
     </row>
     <row r="143" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A143" s="2" t="s">
-        <v>354</v>
+        <v>350</v>
       </c>
       <c r="B143" s="2" t="s">
-        <v>355</v>
+        <v>351</v>
       </c>
       <c r="C143" s="3" t="s">
-        <v>354</v>
+        <v>350</v>
       </c>
     </row>
     <row r="144" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A144" s="2" t="s">
-        <v>352</v>
+        <v>176</v>
       </c>
       <c r="B144" s="2" t="s">
-        <v>353</v>
-      </c>
-      <c r="C144" s="3" t="s">
-        <v>352</v>
+        <v>177</v>
+      </c>
+      <c r="C144" s="2" t="s">
+        <v>176</v>
       </c>
     </row>
     <row r="145" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A145" s="2" t="s">
-        <v>184</v>
+        <v>388</v>
       </c>
       <c r="B145" s="2" t="s">
-        <v>185</v>
+        <v>391</v>
       </c>
       <c r="C145" s="2" t="s">
-        <v>184</v>
+        <v>388</v>
       </c>
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A146" s="2" t="s">
-        <v>186</v>
+      <c r="A146" s="1" t="s">
+        <v>475</v>
       </c>
       <c r="B146" s="2" t="s">
-        <v>187</v>
-      </c>
-      <c r="C146" s="3" t="s">
-        <v>186</v>
+        <v>487</v>
+      </c>
+      <c r="C146" s="1" t="s">
+        <v>475</v>
       </c>
     </row>
     <row r="147" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A147" s="2" t="s">
-        <v>188</v>
+        <v>178</v>
       </c>
       <c r="B147" s="2" t="s">
-        <v>189</v>
+        <v>179</v>
       </c>
       <c r="C147" s="3" t="s">
-        <v>188</v>
+        <v>178</v>
       </c>
     </row>
     <row r="148" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A148" s="1" t="s">
-        <v>431</v>
-      </c>
-      <c r="B148" s="1" t="s">
-        <v>432</v>
-      </c>
-      <c r="C148" s="1" t="s">
-        <v>431</v>
+      <c r="A148" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="B148" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="C148" s="3" t="s">
+        <v>180</v>
       </c>
     </row>
     <row r="149" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A149" s="2" t="s">
-        <v>190</v>
+        <v>182</v>
       </c>
       <c r="B149" s="2" t="s">
-        <v>191</v>
+        <v>183</v>
       </c>
       <c r="C149" s="3" t="s">
-        <v>190</v>
+        <v>182</v>
       </c>
     </row>
     <row r="150" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A150" s="2" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="B150" s="2" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="C150" s="3" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
     </row>
     <row r="151" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A151" s="2" t="s">
-        <v>454</v>
+        <v>354</v>
       </c>
       <c r="B151" s="2" t="s">
-        <v>455</v>
+        <v>355</v>
       </c>
       <c r="C151" s="3" t="s">
-        <v>454</v>
+        <v>354</v>
       </c>
     </row>
     <row r="152" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A152" s="2" t="s">
-        <v>192</v>
+        <v>352</v>
       </c>
       <c r="B152" s="2" t="s">
-        <v>193</v>
+        <v>353</v>
       </c>
       <c r="C152" s="3" t="s">
-        <v>192</v>
+        <v>352</v>
       </c>
     </row>
     <row r="153" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A153" s="2" t="s">
-        <v>194</v>
+        <v>184</v>
       </c>
       <c r="B153" s="2" t="s">
-        <v>195</v>
-      </c>
-      <c r="C153" s="3" t="s">
-        <v>194</v>
+        <v>185</v>
+      </c>
+      <c r="C153" s="2" t="s">
+        <v>184</v>
       </c>
     </row>
     <row r="154" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A154" s="1" t="s">
-        <v>500</v>
+      <c r="A154" s="2" t="s">
+        <v>186</v>
       </c>
       <c r="B154" s="2" t="s">
-        <v>501</v>
-      </c>
-      <c r="C154" s="1" t="s">
-        <v>500</v>
+        <v>187</v>
+      </c>
+      <c r="C154" s="3" t="s">
+        <v>186</v>
       </c>
     </row>
     <row r="155" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A155" s="2" t="s">
-        <v>196</v>
+        <v>529</v>
       </c>
       <c r="B155" s="2" t="s">
-        <v>197</v>
-      </c>
-      <c r="C155" s="3" t="s">
-        <v>196</v>
+        <v>531</v>
+      </c>
+      <c r="C155" s="2" t="s">
+        <v>529</v>
       </c>
     </row>
     <row r="156" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A156" s="2" t="s">
-        <v>198</v>
+        <v>188</v>
       </c>
       <c r="B156" s="2" t="s">
-        <v>199</v>
+        <v>189</v>
       </c>
       <c r="C156" s="3" t="s">
-        <v>198</v>
+        <v>188</v>
       </c>
     </row>
     <row r="157" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A157" s="2" t="s">
-        <v>200</v>
-      </c>
-      <c r="B157" s="2" t="s">
-        <v>201</v>
-      </c>
-      <c r="C157" s="3" t="s">
-        <v>200</v>
+      <c r="A157" s="1" t="s">
+        <v>431</v>
+      </c>
+      <c r="B157" s="1" t="s">
+        <v>432</v>
+      </c>
+      <c r="C157" s="1" t="s">
+        <v>431</v>
       </c>
     </row>
     <row r="158" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A158" s="2" t="s">
-        <v>202</v>
+        <v>190</v>
       </c>
       <c r="B158" s="2" t="s">
-        <v>203</v>
+        <v>191</v>
       </c>
       <c r="C158" s="3" t="s">
-        <v>202</v>
+        <v>190</v>
       </c>
     </row>
     <row r="159" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A159" s="2" t="s">
-        <v>204</v>
+        <v>340</v>
       </c>
       <c r="B159" s="2" t="s">
-        <v>205</v>
+        <v>341</v>
       </c>
       <c r="C159" s="3" t="s">
-        <v>204</v>
+        <v>340</v>
       </c>
     </row>
     <row r="160" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A160" s="2" t="s">
-        <v>206</v>
+        <v>454</v>
       </c>
       <c r="B160" s="2" t="s">
-        <v>207</v>
+        <v>455</v>
       </c>
       <c r="C160" s="3" t="s">
-        <v>206</v>
+        <v>454</v>
       </c>
     </row>
     <row r="161" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A161" s="1" t="s">
-        <v>496</v>
+      <c r="A161" s="2" t="s">
+        <v>192</v>
       </c>
       <c r="B161" s="2" t="s">
-        <v>497</v>
-      </c>
-      <c r="C161" s="1" t="s">
-        <v>496</v>
+        <v>193</v>
+      </c>
+      <c r="C161" s="3" t="s">
+        <v>192</v>
       </c>
     </row>
     <row r="162" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A162" s="2" t="s">
-        <v>208</v>
+        <v>194</v>
       </c>
       <c r="B162" s="2" t="s">
-        <v>209</v>
+        <v>195</v>
       </c>
       <c r="C162" s="3" t="s">
-        <v>208</v>
+        <v>194</v>
       </c>
     </row>
     <row r="163" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A163" s="2" t="s">
-        <v>358</v>
+      <c r="A163" s="1" t="s">
+        <v>500</v>
       </c>
       <c r="B163" s="2" t="s">
-        <v>359</v>
-      </c>
-      <c r="C163" s="2" t="s">
-        <v>358</v>
+        <v>501</v>
+      </c>
+      <c r="C163" s="1" t="s">
+        <v>500</v>
       </c>
     </row>
     <row r="164" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A164" s="2" t="s">
-        <v>210</v>
+        <v>196</v>
       </c>
       <c r="B164" s="2" t="s">
-        <v>211</v>
+        <v>197</v>
       </c>
       <c r="C164" s="3" t="s">
-        <v>210</v>
+        <v>196</v>
       </c>
     </row>
     <row r="165" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A165" s="2" t="s">
-        <v>212</v>
+        <v>198</v>
       </c>
       <c r="B165" s="2" t="s">
-        <v>213</v>
+        <v>199</v>
       </c>
       <c r="C165" s="3" t="s">
-        <v>212</v>
+        <v>198</v>
       </c>
     </row>
     <row r="166" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A166" s="2" t="s">
-        <v>389</v>
+        <v>200</v>
       </c>
       <c r="B166" s="2" t="s">
-        <v>392</v>
-      </c>
-      <c r="C166" s="2" t="s">
-        <v>389</v>
+        <v>201</v>
+      </c>
+      <c r="C166" s="3" t="s">
+        <v>200</v>
       </c>
     </row>
     <row r="167" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A167" s="1" t="s">
-        <v>410</v>
-      </c>
-      <c r="B167" s="1" t="s">
-        <v>421</v>
-      </c>
-      <c r="C167" s="1" t="s">
-        <v>410</v>
+      <c r="A167" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="B167" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="C167" s="3" t="s">
+        <v>202</v>
       </c>
     </row>
     <row r="168" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A168" s="2" t="s">
-        <v>214</v>
+        <v>204</v>
       </c>
       <c r="B168" s="2" t="s">
-        <v>215</v>
+        <v>205</v>
       </c>
       <c r="C168" s="3" t="s">
-        <v>214</v>
+        <v>204</v>
       </c>
     </row>
     <row r="169" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A169" s="2" t="s">
-        <v>216</v>
+        <v>206</v>
       </c>
       <c r="B169" s="2" t="s">
-        <v>217</v>
+        <v>207</v>
       </c>
       <c r="C169" s="3" t="s">
-        <v>216</v>
+        <v>206</v>
       </c>
     </row>
     <row r="170" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A170" s="2" t="s">
-        <v>218</v>
+      <c r="A170" s="1" t="s">
+        <v>496</v>
       </c>
       <c r="B170" s="2" t="s">
-        <v>219</v>
-      </c>
-      <c r="C170" s="3" t="s">
-        <v>218</v>
+        <v>497</v>
+      </c>
+      <c r="C170" s="1" t="s">
+        <v>496</v>
       </c>
     </row>
     <row r="171" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A171" s="2" t="s">
-        <v>220</v>
+        <v>530</v>
       </c>
       <c r="B171" s="2" t="s">
-        <v>221</v>
+        <v>532</v>
       </c>
       <c r="C171" s="2" t="s">
-        <v>220</v>
+        <v>530</v>
       </c>
     </row>
     <row r="172" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A172" s="1" t="s">
-        <v>444</v>
-      </c>
-      <c r="B172" s="1" t="s">
-        <v>446</v>
-      </c>
-      <c r="C172" s="1" t="s">
-        <v>444</v>
+      <c r="A172" s="2" t="s">
+        <v>208</v>
+      </c>
+      <c r="B172" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="C172" s="3" t="s">
+        <v>208</v>
       </c>
     </row>
     <row r="173" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A173" s="2" t="s">
-        <v>376</v>
+        <v>358</v>
       </c>
       <c r="B173" s="2" t="s">
-        <v>377</v>
+        <v>359</v>
       </c>
       <c r="C173" s="2" t="s">
-        <v>376</v>
+        <v>358</v>
       </c>
     </row>
     <row r="174" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A174" s="2" t="s">
-        <v>222</v>
+        <v>210</v>
       </c>
       <c r="B174" s="2" t="s">
-        <v>223</v>
+        <v>211</v>
       </c>
       <c r="C174" s="3" t="s">
-        <v>222</v>
+        <v>210</v>
       </c>
     </row>
     <row r="175" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A175" s="2" t="s">
-        <v>346</v>
+        <v>212</v>
       </c>
       <c r="B175" s="2" t="s">
-        <v>347</v>
+        <v>213</v>
       </c>
       <c r="C175" s="3" t="s">
-        <v>346</v>
+        <v>212</v>
       </c>
     </row>
     <row r="176" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A176" s="1" t="s">
-        <v>448</v>
+      <c r="A176" s="2" t="s">
+        <v>389</v>
       </c>
       <c r="B176" s="2" t="s">
-        <v>449</v>
-      </c>
-      <c r="C176" s="1" t="s">
-        <v>448</v>
+        <v>392</v>
+      </c>
+      <c r="C176" s="2" t="s">
+        <v>389</v>
       </c>
     </row>
     <row r="177" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A177" s="2" t="s">
-        <v>224</v>
+        <v>559</v>
       </c>
       <c r="B177" s="2" t="s">
-        <v>225</v>
+        <v>561</v>
       </c>
       <c r="C177" s="2" t="s">
-        <v>224</v>
+        <v>559</v>
       </c>
     </row>
     <row r="178" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A178" s="1" t="s">
-        <v>468</v>
-      </c>
-      <c r="B178" s="2" t="s">
-        <v>480</v>
+        <v>410</v>
+      </c>
+      <c r="B178" s="1" t="s">
+        <v>421</v>
       </c>
       <c r="C178" s="1" t="s">
-        <v>468</v>
+        <v>410</v>
       </c>
     </row>
     <row r="179" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A179" s="2" t="s">
-        <v>226</v>
+        <v>214</v>
       </c>
       <c r="B179" s="2" t="s">
-        <v>227</v>
-      </c>
-      <c r="C179" s="2" t="s">
-        <v>226</v>
+        <v>215</v>
+      </c>
+      <c r="C179" s="3" t="s">
+        <v>214</v>
       </c>
     </row>
     <row r="180" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A180" s="2" t="s">
-        <v>228</v>
+        <v>216</v>
       </c>
       <c r="B180" s="2" t="s">
-        <v>229</v>
+        <v>217</v>
       </c>
       <c r="C180" s="3" t="s">
-        <v>228</v>
+        <v>216</v>
       </c>
     </row>
     <row r="181" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A181" s="2" t="s">
-        <v>230</v>
+        <v>218</v>
       </c>
       <c r="B181" s="2" t="s">
-        <v>231</v>
-      </c>
-      <c r="C181" s="2" t="s">
-        <v>230</v>
+        <v>219</v>
+      </c>
+      <c r="C181" s="3" t="s">
+        <v>218</v>
       </c>
     </row>
     <row r="182" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A182" s="2" t="s">
-        <v>232</v>
+        <v>220</v>
       </c>
       <c r="B182" s="2" t="s">
-        <v>233</v>
-      </c>
-      <c r="C182" s="3" t="s">
-        <v>232</v>
+        <v>221</v>
+      </c>
+      <c r="C182" s="2" t="s">
+        <v>220</v>
       </c>
     </row>
     <row r="183" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A183" s="2" t="s">
-        <v>234</v>
-      </c>
-      <c r="B183" s="2" t="s">
-        <v>235</v>
-      </c>
-      <c r="C183" s="3" t="s">
-        <v>234</v>
+      <c r="A183" s="1" t="s">
+        <v>444</v>
+      </c>
+      <c r="B183" s="1" t="s">
+        <v>446</v>
+      </c>
+      <c r="C183" s="1" t="s">
+        <v>444</v>
       </c>
     </row>
     <row r="184" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A184" s="2" t="s">
-        <v>494</v>
+        <v>376</v>
       </c>
       <c r="B184" s="2" t="s">
-        <v>495</v>
+        <v>377</v>
       </c>
       <c r="C184" s="2" t="s">
-        <v>494</v>
+        <v>376</v>
       </c>
     </row>
     <row r="185" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A185" s="2" t="s">
-        <v>236</v>
+        <v>222</v>
       </c>
       <c r="B185" s="2" t="s">
-        <v>237</v>
+        <v>223</v>
       </c>
       <c r="C185" s="3" t="s">
-        <v>236</v>
+        <v>222</v>
       </c>
     </row>
     <row r="186" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A186" s="2" t="s">
-        <v>238</v>
+        <v>346</v>
       </c>
       <c r="B186" s="2" t="s">
-        <v>402</v>
-      </c>
-      <c r="C186" s="2" t="s">
-        <v>238</v>
+        <v>347</v>
+      </c>
+      <c r="C186" s="3" t="s">
+        <v>346</v>
       </c>
     </row>
     <row r="187" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A187" s="2" t="s">
-        <v>394</v>
+      <c r="A187" s="1" t="s">
+        <v>448</v>
       </c>
       <c r="B187" s="2" t="s">
-        <v>395</v>
-      </c>
-      <c r="C187" s="2" t="s">
-        <v>394</v>
+        <v>449</v>
+      </c>
+      <c r="C187" s="1" t="s">
+        <v>448</v>
       </c>
     </row>
     <row r="188" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A188" s="2" t="s">
-        <v>464</v>
+        <v>224</v>
       </c>
       <c r="B188" s="2" t="s">
-        <v>466</v>
+        <v>225</v>
       </c>
       <c r="C188" s="2" t="s">
-        <v>464</v>
+        <v>224</v>
       </c>
     </row>
     <row r="189" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A189" s="2" t="s">
-        <v>239</v>
+      <c r="A189" s="1" t="s">
+        <v>468</v>
       </c>
       <c r="B189" s="2" t="s">
-        <v>398</v>
-      </c>
-      <c r="C189" s="2" t="s">
-        <v>239</v>
+        <v>480</v>
+      </c>
+      <c r="C189" s="1" t="s">
+        <v>468</v>
       </c>
     </row>
     <row r="190" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A190" s="2" t="s">
-        <v>240</v>
+        <v>226</v>
       </c>
       <c r="B190" s="2" t="s">
-        <v>241</v>
+        <v>227</v>
       </c>
       <c r="C190" s="2" t="s">
-        <v>240</v>
+        <v>226</v>
       </c>
     </row>
     <row r="191" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A191" s="2" t="s">
-        <v>242</v>
+        <v>228</v>
       </c>
       <c r="B191" s="2" t="s">
-        <v>243</v>
+        <v>229</v>
       </c>
       <c r="C191" s="3" t="s">
-        <v>242</v>
+        <v>228</v>
       </c>
     </row>
     <row r="192" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A192" s="2" t="s">
-        <v>244</v>
+        <v>230</v>
       </c>
       <c r="B192" s="2" t="s">
-        <v>245</v>
-      </c>
-      <c r="C192" s="3" t="s">
-        <v>244</v>
+        <v>231</v>
+      </c>
+      <c r="C192" s="2" t="s">
+        <v>230</v>
       </c>
     </row>
     <row r="193" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A193" s="2" t="s">
-        <v>246</v>
+        <v>232</v>
       </c>
       <c r="B193" s="2" t="s">
-        <v>247</v>
-      </c>
-      <c r="C193" s="2" t="s">
-        <v>246</v>
+        <v>233</v>
+      </c>
+      <c r="C193" s="3" t="s">
+        <v>232</v>
       </c>
     </row>
     <row r="194" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A194" s="2" t="s">
-        <v>248</v>
+        <v>234</v>
       </c>
       <c r="B194" s="2" t="s">
-        <v>429</v>
+        <v>235</v>
       </c>
       <c r="C194" s="3" t="s">
-        <v>248</v>
+        <v>234</v>
       </c>
     </row>
     <row r="195" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A195" s="2" t="s">
-        <v>249</v>
+        <v>494</v>
       </c>
       <c r="B195" s="2" t="s">
-        <v>430</v>
-      </c>
-      <c r="C195" s="3" t="s">
-        <v>249</v>
+        <v>495</v>
+      </c>
+      <c r="C195" s="2" t="s">
+        <v>494</v>
       </c>
     </row>
     <row r="196" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A196" s="2" t="s">
-        <v>462</v>
+        <v>236</v>
       </c>
       <c r="B196" s="2" t="s">
-        <v>463</v>
-      </c>
-      <c r="C196" s="2" t="s">
-        <v>462</v>
+        <v>237</v>
+      </c>
+      <c r="C196" s="3" t="s">
+        <v>236</v>
       </c>
     </row>
     <row r="197" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A197" s="2" t="s">
-        <v>250</v>
+        <v>238</v>
       </c>
       <c r="B197" s="2" t="s">
-        <v>251</v>
+        <v>402</v>
       </c>
       <c r="C197" s="2" t="s">
-        <v>250</v>
+        <v>238</v>
       </c>
     </row>
     <row r="198" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A198" s="2" t="s">
-        <v>252</v>
+        <v>394</v>
       </c>
       <c r="B198" s="2" t="s">
-        <v>253</v>
-      </c>
-      <c r="C198" s="3" t="s">
-        <v>252</v>
+        <v>395</v>
+      </c>
+      <c r="C198" s="2" t="s">
+        <v>394</v>
       </c>
     </row>
     <row r="199" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A199" s="2" t="s">
-        <v>254</v>
+        <v>464</v>
       </c>
       <c r="B199" s="2" t="s">
-        <v>255</v>
-      </c>
-      <c r="C199" s="3" t="s">
-        <v>254</v>
+        <v>466</v>
+      </c>
+      <c r="C199" s="2" t="s">
+        <v>464</v>
       </c>
     </row>
     <row r="200" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A200" s="2" t="s">
-        <v>256</v>
+        <v>239</v>
       </c>
       <c r="B200" s="2" t="s">
-        <v>257</v>
+        <v>398</v>
       </c>
       <c r="C200" s="2" t="s">
-        <v>256</v>
+        <v>239</v>
       </c>
     </row>
     <row r="201" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A201" s="2" t="s">
-        <v>258</v>
+        <v>240</v>
       </c>
       <c r="B201" s="2" t="s">
-        <v>259</v>
-      </c>
-      <c r="C201" s="3" t="s">
-        <v>258</v>
+        <v>241</v>
+      </c>
+      <c r="C201" s="2" t="s">
+        <v>240</v>
       </c>
     </row>
     <row r="202" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A202" s="2" t="s">
-        <v>260</v>
+        <v>242</v>
       </c>
       <c r="B202" s="2" t="s">
-        <v>261</v>
+        <v>243</v>
       </c>
       <c r="C202" s="3" t="s">
-        <v>260</v>
+        <v>242</v>
       </c>
     </row>
     <row r="203" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A203" s="1" t="s">
-        <v>438</v>
-      </c>
-      <c r="B203" s="1" t="s">
-        <v>440</v>
-      </c>
-      <c r="C203" s="1" t="s">
-        <v>438</v>
+      <c r="A203" s="2" t="s">
+        <v>244</v>
+      </c>
+      <c r="B203" s="2" t="s">
+        <v>245</v>
+      </c>
+      <c r="C203" s="3" t="s">
+        <v>244</v>
       </c>
     </row>
     <row r="204" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A204" s="1" t="s">
-        <v>439</v>
-      </c>
-      <c r="B204" s="1" t="s">
-        <v>441</v>
-      </c>
-      <c r="C204" s="1" t="s">
-        <v>439</v>
+      <c r="A204" s="2" t="s">
+        <v>246</v>
+      </c>
+      <c r="B204" s="2" t="s">
+        <v>247</v>
+      </c>
+      <c r="C204" s="2" t="s">
+        <v>246</v>
       </c>
     </row>
     <row r="205" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A205" s="1" t="s">
-        <v>515</v>
-      </c>
-      <c r="B205" s="1" t="s">
-        <v>522</v>
-      </c>
-      <c r="C205" s="1" t="s">
-        <v>515</v>
+      <c r="A205" s="2" t="s">
+        <v>248</v>
+      </c>
+      <c r="B205" s="2" t="s">
+        <v>429</v>
+      </c>
+      <c r="C205" s="3" t="s">
+        <v>248</v>
       </c>
     </row>
     <row r="206" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A206" s="2" t="s">
-        <v>262</v>
+        <v>249</v>
       </c>
       <c r="B206" s="2" t="s">
-        <v>263</v>
+        <v>430</v>
       </c>
       <c r="C206" s="3" t="s">
-        <v>262</v>
+        <v>249</v>
       </c>
     </row>
     <row r="207" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A207" s="2" t="s">
-        <v>400</v>
+        <v>462</v>
       </c>
       <c r="B207" s="2" t="s">
-        <v>401</v>
+        <v>463</v>
       </c>
       <c r="C207" s="2" t="s">
-        <v>400</v>
+        <v>462</v>
       </c>
     </row>
     <row r="208" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A208" s="2" t="s">
-        <v>374</v>
+        <v>250</v>
       </c>
       <c r="B208" s="2" t="s">
-        <v>375</v>
+        <v>251</v>
       </c>
       <c r="C208" s="2" t="s">
-        <v>374</v>
+        <v>250</v>
       </c>
     </row>
     <row r="209" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A209" s="2" t="s">
-        <v>264</v>
+        <v>252</v>
       </c>
       <c r="B209" s="2" t="s">
-        <v>399</v>
-      </c>
-      <c r="C209" s="2" t="s">
-        <v>264</v>
+        <v>253</v>
+      </c>
+      <c r="C209" s="3" t="s">
+        <v>252</v>
       </c>
     </row>
     <row r="210" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A210" s="2" t="s">
-        <v>265</v>
+        <v>254</v>
       </c>
       <c r="B210" s="2" t="s">
-        <v>266</v>
+        <v>255</v>
       </c>
       <c r="C210" s="3" t="s">
-        <v>265</v>
+        <v>254</v>
       </c>
     </row>
     <row r="211" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A211" s="2" t="s">
-        <v>267</v>
+        <v>256</v>
       </c>
       <c r="B211" s="2" t="s">
-        <v>268</v>
+        <v>257</v>
       </c>
       <c r="C211" s="2" t="s">
-        <v>267</v>
+        <v>256</v>
       </c>
     </row>
     <row r="212" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A212" s="1" t="s">
-        <v>403</v>
+      <c r="A212" s="2" t="s">
+        <v>258</v>
       </c>
       <c r="B212" s="2" t="s">
-        <v>414</v>
-      </c>
-      <c r="C212" s="1" t="s">
-        <v>403</v>
+        <v>259</v>
+      </c>
+      <c r="C212" s="3" t="s">
+        <v>258</v>
       </c>
     </row>
     <row r="213" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A213" s="2" t="s">
-        <v>269</v>
+        <v>260</v>
       </c>
       <c r="B213" s="2" t="s">
-        <v>270</v>
+        <v>261</v>
       </c>
       <c r="C213" s="3" t="s">
-        <v>269</v>
+        <v>260</v>
       </c>
     </row>
     <row r="214" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A214" s="2" t="s">
-        <v>271</v>
-      </c>
-      <c r="B214" s="2" t="s">
-        <v>272</v>
-      </c>
-      <c r="C214" s="2" t="s">
-        <v>271</v>
+      <c r="A214" s="1" t="s">
+        <v>438</v>
+      </c>
+      <c r="B214" s="1" t="s">
+        <v>440</v>
+      </c>
+      <c r="C214" s="1" t="s">
+        <v>438</v>
       </c>
     </row>
     <row r="215" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A215" s="2" t="s">
-        <v>273</v>
-      </c>
-      <c r="B215" s="2" t="s">
-        <v>274</v>
-      </c>
-      <c r="C215" s="3" t="s">
-        <v>273</v>
+      <c r="A215" s="1" t="s">
+        <v>439</v>
+      </c>
+      <c r="B215" s="1" t="s">
+        <v>441</v>
+      </c>
+      <c r="C215" s="1" t="s">
+        <v>439</v>
       </c>
     </row>
     <row r="216" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A216" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B216" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C216" s="3" t="s">
-        <v>9</v>
+      <c r="A216" s="1" t="s">
+        <v>515</v>
+      </c>
+      <c r="B216" s="1" t="s">
+        <v>522</v>
+      </c>
+      <c r="C216" s="1" t="s">
+        <v>515</v>
       </c>
     </row>
     <row r="217" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A217" s="2" t="s">
-        <v>506</v>
+        <v>262</v>
       </c>
       <c r="B217" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C217" s="2" t="s">
-        <v>506</v>
+        <v>263</v>
+      </c>
+      <c r="C217" s="3" t="s">
+        <v>262</v>
       </c>
     </row>
     <row r="218" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A218" s="2" t="s">
-        <v>275</v>
+        <v>400</v>
       </c>
       <c r="B218" s="2" t="s">
-        <v>276</v>
-      </c>
-      <c r="C218" s="3" t="s">
-        <v>275</v>
+        <v>401</v>
+      </c>
+      <c r="C218" s="2" t="s">
+        <v>400</v>
       </c>
     </row>
     <row r="219" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A219" s="1" t="s">
-        <v>473</v>
+      <c r="A219" s="2" t="s">
+        <v>374</v>
       </c>
       <c r="B219" s="2" t="s">
-        <v>484</v>
-      </c>
-      <c r="C219" s="1" t="s">
-        <v>473</v>
+        <v>375</v>
+      </c>
+      <c r="C219" s="2" t="s">
+        <v>374</v>
       </c>
     </row>
     <row r="220" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A220" s="2" t="s">
-        <v>378</v>
+        <v>264</v>
       </c>
       <c r="B220" s="2" t="s">
-        <v>379</v>
+        <v>399</v>
       </c>
       <c r="C220" s="2" t="s">
-        <v>378</v>
+        <v>264</v>
       </c>
     </row>
     <row r="221" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A221" s="2" t="s">
-        <v>277</v>
+      <c r="A221" s="1" t="s">
+        <v>534</v>
       </c>
       <c r="B221" s="2" t="s">
-        <v>278</v>
-      </c>
-      <c r="C221" s="3" t="s">
-        <v>277</v>
+        <v>546</v>
+      </c>
+      <c r="C221" s="1" t="s">
+        <v>534</v>
       </c>
     </row>
     <row r="222" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A222" s="1" t="s">
-        <v>478</v>
+      <c r="A222" s="2" t="s">
+        <v>265</v>
       </c>
       <c r="B222" s="2" t="s">
-        <v>490</v>
-      </c>
-      <c r="C222" s="1" t="s">
-        <v>478</v>
+        <v>266</v>
+      </c>
+      <c r="C222" s="3" t="s">
+        <v>265</v>
       </c>
     </row>
     <row r="223" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A223" s="1" t="s">
-        <v>502</v>
+      <c r="A223" s="2" t="s">
+        <v>267</v>
       </c>
       <c r="B223" s="2" t="s">
-        <v>503</v>
-      </c>
-      <c r="C223" s="1" t="s">
-        <v>502</v>
+        <v>268</v>
+      </c>
+      <c r="C223" s="2" t="s">
+        <v>267</v>
       </c>
     </row>
     <row r="224" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A224" s="2" t="s">
-        <v>279</v>
+        <v>557</v>
       </c>
       <c r="B224" s="2" t="s">
-        <v>280</v>
-      </c>
-      <c r="C224" s="3" t="s">
-        <v>279</v>
+        <v>558</v>
+      </c>
+      <c r="C224" s="2" t="s">
+        <v>557</v>
       </c>
     </row>
     <row r="225" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A225" s="2" t="s">
-        <v>5</v>
+      <c r="A225" s="1" t="s">
+        <v>403</v>
       </c>
       <c r="B225" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C225" s="3" t="s">
-        <v>5</v>
+        <v>414</v>
+      </c>
+      <c r="C225" s="1" t="s">
+        <v>403</v>
       </c>
     </row>
     <row r="226" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A226" s="2" t="s">
-        <v>281</v>
+        <v>269</v>
       </c>
       <c r="B226" s="2" t="s">
-        <v>282</v>
-      </c>
-      <c r="C226" s="2" t="s">
-        <v>281</v>
+        <v>270</v>
+      </c>
+      <c r="C226" s="3" t="s">
+        <v>269</v>
       </c>
     </row>
     <row r="227" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A227" s="2" t="s">
-        <v>283</v>
+        <v>271</v>
       </c>
       <c r="B227" s="2" t="s">
-        <v>284</v>
-      </c>
-      <c r="C227" s="3" t="s">
-        <v>283</v>
+        <v>272</v>
+      </c>
+      <c r="C227" s="2" t="s">
+        <v>271</v>
       </c>
     </row>
     <row r="228" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A228" s="2" t="s">
-        <v>285</v>
+        <v>273</v>
       </c>
       <c r="B228" s="2" t="s">
-        <v>284</v>
+        <v>274</v>
       </c>
       <c r="C228" s="3" t="s">
-        <v>285</v>
+        <v>273</v>
       </c>
     </row>
     <row r="229" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A229" s="2" t="s">
-        <v>286</v>
+        <v>9</v>
       </c>
       <c r="B229" s="2" t="s">
-        <v>287</v>
+        <v>10</v>
       </c>
       <c r="C229" s="3" t="s">
-        <v>286</v>
+        <v>9</v>
       </c>
     </row>
     <row r="230" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A230" s="2" t="s">
-        <v>288</v>
+        <v>506</v>
       </c>
       <c r="B230" s="2" t="s">
-        <v>289</v>
-      </c>
-      <c r="C230" s="3" t="s">
-        <v>288</v>
+        <v>1</v>
+      </c>
+      <c r="C230" s="2" t="s">
+        <v>506</v>
       </c>
     </row>
     <row r="231" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A231" s="2" t="s">
-        <v>290</v>
+        <v>275</v>
       </c>
       <c r="B231" s="2" t="s">
-        <v>291</v>
+        <v>276</v>
       </c>
       <c r="C231" s="3" t="s">
-        <v>290</v>
+        <v>275</v>
       </c>
     </row>
     <row r="232" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A232" s="2" t="s">
-        <v>292</v>
+      <c r="A232" s="1" t="s">
+        <v>473</v>
       </c>
       <c r="B232" s="2" t="s">
-        <v>293</v>
-      </c>
-      <c r="C232" s="3" t="s">
-        <v>292</v>
+        <v>484</v>
+      </c>
+      <c r="C232" s="1" t="s">
+        <v>473</v>
       </c>
     </row>
     <row r="233" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A233" s="2" t="s">
-        <v>294</v>
+        <v>378</v>
       </c>
       <c r="B233" s="2" t="s">
-        <v>295</v>
-      </c>
-      <c r="C233" s="3" t="s">
-        <v>294</v>
+        <v>379</v>
+      </c>
+      <c r="C233" s="2" t="s">
+        <v>378</v>
       </c>
     </row>
     <row r="234" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A234" s="2" t="s">
-        <v>296</v>
+        <v>277</v>
       </c>
       <c r="B234" s="2" t="s">
-        <v>297</v>
+        <v>278</v>
       </c>
       <c r="C234" s="3" t="s">
-        <v>296</v>
+        <v>277</v>
       </c>
     </row>
     <row r="235" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A235" s="2" t="s">
-        <v>298</v>
+      <c r="A235" s="1" t="s">
+        <v>478</v>
       </c>
       <c r="B235" s="2" t="s">
-        <v>299</v>
-      </c>
-      <c r="C235" s="2" t="s">
-        <v>298</v>
+        <v>490</v>
+      </c>
+      <c r="C235" s="1" t="s">
+        <v>478</v>
       </c>
     </row>
     <row r="236" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A236" s="1" t="s">
-        <v>409</v>
+        <v>502</v>
       </c>
       <c r="B236" s="2" t="s">
-        <v>418</v>
+        <v>503</v>
       </c>
       <c r="C236" s="1" t="s">
-        <v>409</v>
+        <v>502</v>
       </c>
     </row>
     <row r="237" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A237" s="2" t="s">
-        <v>300</v>
+        <v>279</v>
       </c>
       <c r="B237" s="2" t="s">
-        <v>301</v>
+        <v>280</v>
       </c>
       <c r="C237" s="3" t="s">
-        <v>300</v>
+        <v>279</v>
       </c>
     </row>
     <row r="238" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A238" s="1" t="s">
-        <v>472</v>
+      <c r="A238" s="2" t="s">
+        <v>5</v>
       </c>
       <c r="B238" s="2" t="s">
-        <v>483</v>
-      </c>
-      <c r="C238" s="1" t="s">
-        <v>472</v>
+        <v>6</v>
+      </c>
+      <c r="C238" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="239" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A239" s="2" t="s">
-        <v>302</v>
+        <v>281</v>
       </c>
       <c r="B239" s="2" t="s">
-        <v>303</v>
-      </c>
-      <c r="C239" s="3" t="s">
-        <v>302</v>
+        <v>282</v>
+      </c>
+      <c r="C239" s="2" t="s">
+        <v>281</v>
       </c>
     </row>
     <row r="240" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A240" s="1" t="s">
-        <v>470</v>
+      <c r="A240" s="2" t="s">
+        <v>283</v>
       </c>
       <c r="B240" s="2" t="s">
-        <v>486</v>
-      </c>
-      <c r="C240" s="1" t="s">
-        <v>470</v>
+        <v>284</v>
+      </c>
+      <c r="C240" s="3" t="s">
+        <v>283</v>
       </c>
     </row>
     <row r="241" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A241" s="1" t="s">
-        <v>413</v>
-      </c>
-      <c r="B241" s="1" t="s">
-        <v>420</v>
-      </c>
-      <c r="C241" s="1" t="s">
-        <v>413</v>
+      <c r="A241" s="2" t="s">
+        <v>285</v>
+      </c>
+      <c r="B241" s="2" t="s">
+        <v>284</v>
+      </c>
+      <c r="C241" s="3" t="s">
+        <v>285</v>
       </c>
     </row>
     <row r="242" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A242" s="1" t="s">
-        <v>474</v>
+      <c r="A242" s="2" t="s">
+        <v>286</v>
       </c>
       <c r="B242" s="2" t="s">
-        <v>485</v>
-      </c>
-      <c r="C242" s="1" t="s">
-        <v>474</v>
+        <v>287</v>
+      </c>
+      <c r="C242" s="3" t="s">
+        <v>286</v>
       </c>
     </row>
     <row r="243" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A243" s="2" t="s">
-        <v>304</v>
+        <v>288</v>
       </c>
       <c r="B243" s="2" t="s">
-        <v>305</v>
+        <v>289</v>
       </c>
       <c r="C243" s="3" t="s">
-        <v>304</v>
+        <v>288</v>
       </c>
     </row>
     <row r="244" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A244" s="1" t="s">
-        <v>492</v>
+      <c r="A244" s="2" t="s">
+        <v>290</v>
       </c>
       <c r="B244" s="2" t="s">
-        <v>493</v>
-      </c>
-      <c r="C244" s="1" t="s">
-        <v>492</v>
+        <v>291</v>
+      </c>
+      <c r="C244" s="3" t="s">
+        <v>290</v>
       </c>
     </row>
     <row r="245" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A245" s="2" t="s">
-        <v>306</v>
+        <v>292</v>
       </c>
       <c r="B245" s="2" t="s">
-        <v>307</v>
+        <v>293</v>
       </c>
       <c r="C245" s="3" t="s">
-        <v>306</v>
+        <v>292</v>
       </c>
     </row>
     <row r="246" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A246" s="2" t="s">
-        <v>308</v>
+        <v>294</v>
       </c>
       <c r="B246" s="2" t="s">
-        <v>309</v>
+        <v>295</v>
       </c>
       <c r="C246" s="3" t="s">
-        <v>308</v>
+        <v>294</v>
       </c>
     </row>
     <row r="247" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A247" s="2" t="s">
-        <v>310</v>
+        <v>296</v>
       </c>
       <c r="B247" s="2" t="s">
-        <v>311</v>
+        <v>297</v>
       </c>
       <c r="C247" s="3" t="s">
-        <v>310</v>
+        <v>296</v>
       </c>
     </row>
     <row r="248" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A248" s="1" t="s">
-        <v>408</v>
+      <c r="A248" s="2" t="s">
+        <v>298</v>
       </c>
       <c r="B248" s="2" t="s">
-        <v>423</v>
-      </c>
-      <c r="C248" s="1" t="s">
-        <v>408</v>
+        <v>299</v>
+      </c>
+      <c r="C248" s="2" t="s">
+        <v>298</v>
       </c>
     </row>
     <row r="249" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A249" s="2" t="s">
-        <v>364</v>
-      </c>
-      <c r="B249" s="2" t="s">
-        <v>365</v>
-      </c>
-      <c r="C249" s="2" t="s">
-        <v>364</v>
+      <c r="A249" s="1" t="s">
+        <v>552</v>
+      </c>
+      <c r="B249" s="1" t="s">
+        <v>551</v>
+      </c>
+      <c r="C249" s="1" t="s">
+        <v>552</v>
       </c>
     </row>
     <row r="250" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A250" s="2" t="s">
-        <v>370</v>
+      <c r="A250" s="1" t="s">
+        <v>409</v>
       </c>
       <c r="B250" s="2" t="s">
-        <v>371</v>
-      </c>
-      <c r="C250" s="2" t="s">
-        <v>370</v>
+        <v>418</v>
+      </c>
+      <c r="C250" s="1" t="s">
+        <v>409</v>
       </c>
     </row>
     <row r="251" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A251" s="2" t="s">
-        <v>312</v>
+        <v>300</v>
       </c>
       <c r="B251" s="2" t="s">
-        <v>313</v>
+        <v>301</v>
       </c>
       <c r="C251" s="3" t="s">
-        <v>312</v>
+        <v>300</v>
       </c>
     </row>
     <row r="252" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A252" s="2" t="s">
-        <v>11</v>
+      <c r="A252" s="1" t="s">
+        <v>472</v>
       </c>
       <c r="B252" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C252" s="3" t="s">
-        <v>11</v>
+        <v>483</v>
+      </c>
+      <c r="C252" s="1" t="s">
+        <v>472</v>
       </c>
     </row>
     <row r="253" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A253" s="2" t="s">
-        <v>314</v>
+        <v>302</v>
       </c>
       <c r="B253" s="2" t="s">
-        <v>315</v>
-      </c>
-      <c r="C253" s="2" t="s">
-        <v>314</v>
+        <v>303</v>
+      </c>
+      <c r="C253" s="3" t="s">
+        <v>302</v>
       </c>
     </row>
     <row r="254" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A254" s="2" t="s">
-        <v>316</v>
+      <c r="A254" s="1" t="s">
+        <v>470</v>
       </c>
       <c r="B254" s="2" t="s">
-        <v>317</v>
-      </c>
-      <c r="C254" s="3" t="s">
-        <v>316</v>
+        <v>486</v>
+      </c>
+      <c r="C254" s="1" t="s">
+        <v>470</v>
       </c>
     </row>
     <row r="255" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A255" s="2" t="s">
-        <v>318</v>
-      </c>
-      <c r="B255" s="2" t="s">
-        <v>319</v>
-      </c>
-      <c r="C255" s="3" t="s">
-        <v>318</v>
+      <c r="A255" s="1" t="s">
+        <v>413</v>
+      </c>
+      <c r="B255" s="1" t="s">
+        <v>420</v>
+      </c>
+      <c r="C255" s="1" t="s">
+        <v>413</v>
       </c>
     </row>
     <row r="256" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A256" s="2" t="s">
-        <v>320</v>
+      <c r="A256" s="1" t="s">
+        <v>474</v>
       </c>
       <c r="B256" s="2" t="s">
-        <v>321</v>
-      </c>
-      <c r="C256" s="2" t="s">
-        <v>320</v>
+        <v>485</v>
+      </c>
+      <c r="C256" s="1" t="s">
+        <v>474</v>
       </c>
     </row>
     <row r="257" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A257" s="1" t="s">
-        <v>445</v>
-      </c>
-      <c r="B257" s="1" t="s">
-        <v>447</v>
+        <v>535</v>
+      </c>
+      <c r="B257" s="2" t="s">
+        <v>550</v>
       </c>
       <c r="C257" s="1" t="s">
-        <v>445</v>
+        <v>535</v>
       </c>
     </row>
     <row r="258" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A258" s="2" t="s">
-        <v>322</v>
+        <v>304</v>
       </c>
       <c r="B258" s="2" t="s">
-        <v>323</v>
+        <v>305</v>
       </c>
       <c r="C258" s="3" t="s">
-        <v>322</v>
+        <v>304</v>
       </c>
     </row>
     <row r="259" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A259" s="2" t="s">
-        <v>324</v>
+      <c r="A259" s="1" t="s">
+        <v>492</v>
       </c>
       <c r="B259" s="2" t="s">
-        <v>325</v>
-      </c>
-      <c r="C259" s="2" t="s">
-        <v>324</v>
+        <v>493</v>
+      </c>
+      <c r="C259" s="1" t="s">
+        <v>492</v>
       </c>
     </row>
     <row r="260" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A260" s="2" t="s">
-        <v>326</v>
+        <v>306</v>
       </c>
       <c r="B260" s="2" t="s">
-        <v>327</v>
-      </c>
-      <c r="C260" s="2" t="s">
-        <v>326</v>
+        <v>307</v>
+      </c>
+      <c r="C260" s="3" t="s">
+        <v>306</v>
       </c>
     </row>
     <row r="261" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A261" s="2" t="s">
-        <v>328</v>
+        <v>308</v>
       </c>
       <c r="B261" s="2" t="s">
-        <v>329</v>
+        <v>309</v>
       </c>
       <c r="C261" s="3" t="s">
-        <v>328</v>
+        <v>308</v>
       </c>
     </row>
     <row r="262" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A262" s="2" t="s">
-        <v>425</v>
+        <v>310</v>
       </c>
       <c r="B262" s="2" t="s">
-        <v>428</v>
-      </c>
-      <c r="C262" s="2" t="s">
-        <v>425</v>
+        <v>311</v>
+      </c>
+      <c r="C262" s="3" t="s">
+        <v>310</v>
       </c>
     </row>
     <row r="263" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A263" s="2" t="s">
-        <v>330</v>
+      <c r="A263" s="1" t="s">
+        <v>408</v>
       </c>
       <c r="B263" s="2" t="s">
-        <v>331</v>
-      </c>
-      <c r="C263" s="2" t="s">
-        <v>330</v>
+        <v>423</v>
+      </c>
+      <c r="C263" s="1" t="s">
+        <v>408</v>
       </c>
     </row>
     <row r="264" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A264" s="1" t="s">
-        <v>509</v>
+      <c r="A264" s="2" t="s">
+        <v>364</v>
       </c>
       <c r="B264" s="2" t="s">
-        <v>516</v>
-      </c>
-      <c r="C264" s="1" t="s">
-        <v>509</v>
+        <v>365</v>
+      </c>
+      <c r="C264" s="2" t="s">
+        <v>364</v>
       </c>
     </row>
     <row r="265" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A265" s="1" t="s">
-        <v>511</v>
+      <c r="A265" s="2" t="s">
+        <v>370</v>
       </c>
       <c r="B265" s="2" t="s">
-        <v>518</v>
-      </c>
-      <c r="C265" s="1" t="s">
-        <v>511</v>
+        <v>371</v>
+      </c>
+      <c r="C265" s="2" t="s">
+        <v>370</v>
       </c>
     </row>
     <row r="266" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A266" s="1" t="s">
-        <v>510</v>
+      <c r="A266" s="2" t="s">
+        <v>312</v>
       </c>
       <c r="B266" s="2" t="s">
-        <v>517</v>
-      </c>
-      <c r="C266" s="1" t="s">
-        <v>510</v>
+        <v>313</v>
+      </c>
+      <c r="C266" s="3" t="s">
+        <v>312</v>
       </c>
     </row>
     <row r="267" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A267" s="2" t="s">
-        <v>332</v>
+        <v>11</v>
       </c>
       <c r="B267" s="2" t="s">
-        <v>333</v>
+        <v>12</v>
       </c>
       <c r="C267" s="3" t="s">
-        <v>332</v>
+        <v>11</v>
       </c>
     </row>
     <row r="268" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A268" s="2" t="s">
-        <v>334</v>
+        <v>314</v>
       </c>
       <c r="B268" s="2" t="s">
-        <v>335</v>
-      </c>
-      <c r="C268" s="3" t="s">
-        <v>334</v>
+        <v>315</v>
+      </c>
+      <c r="C268" s="2" t="s">
+        <v>314</v>
       </c>
     </row>
     <row r="269" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A269" s="2" t="s">
-        <v>366</v>
+        <v>316</v>
       </c>
       <c r="B269" s="2" t="s">
-        <v>367</v>
-      </c>
-      <c r="C269" s="2" t="s">
-        <v>366</v>
+        <v>317</v>
+      </c>
+      <c r="C269" s="3" t="s">
+        <v>316</v>
       </c>
     </row>
     <row r="270" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A270" s="2" t="s">
+        <v>318</v>
+      </c>
+      <c r="B270" s="2" t="s">
+        <v>319</v>
+      </c>
+      <c r="C270" s="3" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="271" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A271" s="2" t="s">
+        <v>320</v>
+      </c>
+      <c r="B271" s="2" t="s">
+        <v>321</v>
+      </c>
+      <c r="C271" s="2" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="272" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A272" s="1" t="s">
+        <v>445</v>
+      </c>
+      <c r="B272" s="1" t="s">
+        <v>447</v>
+      </c>
+      <c r="C272" s="1" t="s">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="273" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A273" s="2" t="s">
+        <v>322</v>
+      </c>
+      <c r="B273" s="2" t="s">
+        <v>323</v>
+      </c>
+      <c r="C273" s="3" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="274" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A274" s="2" t="s">
+        <v>324</v>
+      </c>
+      <c r="B274" s="2" t="s">
+        <v>325</v>
+      </c>
+      <c r="C274" s="2" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="275" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A275" s="2" t="s">
+        <v>326</v>
+      </c>
+      <c r="B275" s="2" t="s">
+        <v>327</v>
+      </c>
+      <c r="C275" s="2" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="276" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A276" s="2" t="s">
+        <v>328</v>
+      </c>
+      <c r="B276" s="2" t="s">
+        <v>329</v>
+      </c>
+      <c r="C276" s="3" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="277" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A277" s="2" t="s">
+        <v>425</v>
+      </c>
+      <c r="B277" s="2" t="s">
+        <v>428</v>
+      </c>
+      <c r="C277" s="2" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="278" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A278" s="2" t="s">
+        <v>330</v>
+      </c>
+      <c r="B278" s="2" t="s">
+        <v>331</v>
+      </c>
+      <c r="C278" s="2" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="279" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A279" s="1" t="s">
+        <v>509</v>
+      </c>
+      <c r="B279" s="2" t="s">
+        <v>516</v>
+      </c>
+      <c r="C279" s="1" t="s">
+        <v>509</v>
+      </c>
+    </row>
+    <row r="280" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A280" s="1" t="s">
+        <v>511</v>
+      </c>
+      <c r="B280" s="2" t="s">
+        <v>518</v>
+      </c>
+      <c r="C280" s="1" t="s">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="281" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A281" s="1" t="s">
+        <v>510</v>
+      </c>
+      <c r="B281" s="2" t="s">
+        <v>517</v>
+      </c>
+      <c r="C281" s="1" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="282" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A282" s="2" t="s">
+        <v>555</v>
+      </c>
+      <c r="B282" s="2" t="s">
+        <v>556</v>
+      </c>
+      <c r="C282" s="3" t="s">
+        <v>555</v>
+      </c>
+    </row>
+    <row r="283" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A283" s="2" t="s">
+        <v>332</v>
+      </c>
+      <c r="B283" s="2" t="s">
+        <v>333</v>
+      </c>
+      <c r="C283" s="3" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="284" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A284" s="2" t="s">
+        <v>334</v>
+      </c>
+      <c r="B284" s="2" t="s">
+        <v>335</v>
+      </c>
+      <c r="C284" s="3" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="285" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A285" s="2" t="s">
+        <v>366</v>
+      </c>
+      <c r="B285" s="2" t="s">
+        <v>367</v>
+      </c>
+      <c r="C285" s="2" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="286" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A286" s="1" t="s">
+        <v>541</v>
+      </c>
+      <c r="B286" s="1" t="s">
+        <v>553</v>
+      </c>
+      <c r="C286" s="1" t="s">
+        <v>541</v>
+      </c>
+    </row>
+    <row r="287" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A287" s="2" t="s">
         <v>342</v>
       </c>
-      <c r="B270" s="2" t="s">
+      <c r="B287" s="2" t="s">
         <v>343</v>
       </c>
-      <c r="C270" s="3" t="s">
+      <c r="C287" s="3" t="s">
         <v>342</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:C1" xr:uid="{56EE5BC3-7B0A-4577-92C7-56F73F7DDC8B}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C270">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C287">
       <sortCondition ref="A1"/>
     </sortState>
   </autoFilter>

</xml_diff>

<commit_message>
Faster dependent samples comparison
</commit_message>
<xml_diff>
--- a/translations/source.xlsx
+++ b/translations/source.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/e6c7874704bc5dfb/Documents/R Studio/DataSuite/translations/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="276" documentId="8_{D77EC384-F39F-4BA6-8963-4B8AF986F7DE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{5B4140CA-931A-48CA-80DD-68CC15B7E4E6}"/>
+  <xr:revisionPtr revIDLastSave="277" documentId="8_{D77EC384-F39F-4BA6-8963-4B8AF986F7DE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{D44286DA-A677-4504-98E9-74CC7BC813CE}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="16395" xr2:uid="{BD840C99-A56D-4EBC-B1B7-A6018ADC22A6}"/>
   </bookViews>
@@ -1608,9 +1608,6 @@
     <t>Критерий Лиллиефорса</t>
   </si>
   <si>
-    <t>Lilliefors</t>
-  </si>
-  <si>
     <t>Критерий Колмогорова-Смирнова</t>
   </si>
   <si>
@@ -1723,6 +1720,9 @@
   </si>
   <si>
     <t>CI Lower Boundary</t>
+  </si>
+  <si>
+    <t>Lilliefors' test</t>
   </si>
 </sst>
 </file>
@@ -2082,8 +2082,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C853ECA4-158B-4D85-A448-9ECE56776B5F}">
   <dimension ref="A1:C287"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" topLeftCell="A103" workbookViewId="0">
+      <selection activeCell="B119" sqref="B119"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -2118,13 +2118,13 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A3" s="2" t="s">
+        <v>526</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>527</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>528</v>
-      </c>
       <c r="C3" s="3" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.45">
@@ -2437,13 +2437,13 @@
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A32" s="1" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.45">
@@ -2580,13 +2580,13 @@
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A45" s="2" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.45">
@@ -2965,24 +2965,24 @@
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A80" s="1" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A81" s="1" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.45">
@@ -3185,24 +3185,24 @@
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A100" s="1" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="B100" s="1" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="C100" s="1" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A101" s="1" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="B101" s="1" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="C101" s="1" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.45">
@@ -3427,13 +3427,13 @@
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A122" s="1" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="B122" s="1" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="C122" s="1" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.45">
@@ -3515,13 +3515,13 @@
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A130" s="1" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="B130" s="2" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="C130" s="1" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.45">
@@ -3537,13 +3537,13 @@
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A132" s="2" t="s">
+        <v>524</v>
+      </c>
+      <c r="B132" s="2" t="s">
         <v>525</v>
       </c>
-      <c r="B132" s="2" t="s">
-        <v>526</v>
-      </c>
       <c r="C132" s="2" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.45">
@@ -3551,7 +3551,7 @@
         <v>523</v>
       </c>
       <c r="B133" s="2" t="s">
-        <v>524</v>
+        <v>562</v>
       </c>
       <c r="C133" s="2" t="s">
         <v>523</v>
@@ -3790,13 +3790,13 @@
     </row>
     <row r="155" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A155" s="2" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="B155" s="2" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="C155" s="2" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
     </row>
     <row r="156" spans="1:3" x14ac:dyDescent="0.45">
@@ -3966,13 +3966,13 @@
     </row>
     <row r="171" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A171" s="2" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="B171" s="2" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="C171" s="2" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
     </row>
     <row r="172" spans="1:3" x14ac:dyDescent="0.45">
@@ -4032,13 +4032,13 @@
     </row>
     <row r="177" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A177" s="2" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="B177" s="2" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="C177" s="2" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
     </row>
     <row r="178" spans="1:3" x14ac:dyDescent="0.45">
@@ -4516,13 +4516,13 @@
     </row>
     <row r="221" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A221" s="1" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="B221" s="2" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="C221" s="1" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
     </row>
     <row r="222" spans="1:3" x14ac:dyDescent="0.45">
@@ -4549,13 +4549,13 @@
     </row>
     <row r="224" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A224" s="2" t="s">
+        <v>556</v>
+      </c>
+      <c r="B224" s="2" t="s">
         <v>557</v>
       </c>
-      <c r="B224" s="2" t="s">
-        <v>558</v>
-      </c>
       <c r="C224" s="2" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
     </row>
     <row r="225" spans="1:3" x14ac:dyDescent="0.45">
@@ -4824,13 +4824,13 @@
     </row>
     <row r="249" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A249" s="1" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="B249" s="1" t="s">
+        <v>550</v>
+      </c>
+      <c r="C249" s="1" t="s">
         <v>551</v>
-      </c>
-      <c r="C249" s="1" t="s">
-        <v>552</v>
       </c>
     </row>
     <row r="250" spans="1:3" x14ac:dyDescent="0.45">
@@ -4912,13 +4912,13 @@
     </row>
     <row r="257" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A257" s="1" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="B257" s="2" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="C257" s="1" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
     </row>
     <row r="258" spans="1:3" x14ac:dyDescent="0.45">
@@ -5187,13 +5187,13 @@
     </row>
     <row r="282" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A282" s="2" t="s">
+        <v>554</v>
+      </c>
+      <c r="B282" s="2" t="s">
         <v>555</v>
       </c>
-      <c r="B282" s="2" t="s">
-        <v>556</v>
-      </c>
       <c r="C282" s="3" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
     </row>
     <row r="283" spans="1:3" x14ac:dyDescent="0.45">
@@ -5231,13 +5231,13 @@
     </row>
     <row r="286" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A286" s="1" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="B286" s="1" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="C286" s="1" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
     </row>
     <row r="287" spans="1:3" x14ac:dyDescent="0.45">

</xml_diff>

<commit_message>
Bugfixes, plot types for distribution
</commit_message>
<xml_diff>
--- a/translations/source.xlsx
+++ b/translations/source.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/e6c7874704bc5dfb/Documents/R Studio/DataSuite/translations/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="277" documentId="8_{D77EC384-F39F-4BA6-8963-4B8AF986F7DE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{D44286DA-A677-4504-98E9-74CC7BC813CE}"/>
+  <xr:revisionPtr revIDLastSave="300" documentId="8_{D77EC384-F39F-4BA6-8963-4B8AF986F7DE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{602C5BE0-599F-4AB8-8383-B39F0D99F1B3}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="16395" xr2:uid="{BD840C99-A56D-4EBC-B1B7-A6018ADC22A6}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="861" uniqueCount="563">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="906" uniqueCount="592">
   <si>
     <t>base</t>
   </si>
@@ -1723,6 +1723,93 @@
   </si>
   <si>
     <t>Lilliefors' test</t>
+  </si>
+  <si>
+    <t>Анализ мощности</t>
+  </si>
+  <si>
+    <t>Тип графиков для числовых переменных</t>
+  </si>
+  <si>
+    <t>Тип графиков для нечисловых переменных</t>
+  </si>
+  <si>
+    <t>Критерий хи-квадрат</t>
+  </si>
+  <si>
+    <t>Пропорция</t>
+  </si>
+  <si>
+    <t>Две пропорции</t>
+  </si>
+  <si>
+    <t>(одинаковые размеры выборок)</t>
+  </si>
+  <si>
+    <t>(различные размеры выборок)</t>
+  </si>
+  <si>
+    <t>Однофакторный дисперсионный анализ</t>
+  </si>
+  <si>
+    <t>Хи-квадрат</t>
+  </si>
+  <si>
+    <t>Обобщённая линейная модель</t>
+  </si>
+  <si>
+    <t>Тип критерия</t>
+  </si>
+  <si>
+    <t>Мощность</t>
+  </si>
+  <si>
+    <t>Размер выборки</t>
+  </si>
+  <si>
+    <t>Величина эффекта</t>
+  </si>
+  <si>
+    <t>Power Analysis</t>
+  </si>
+  <si>
+    <t>Effect Size</t>
+  </si>
+  <si>
+    <t>Sample size</t>
+  </si>
+  <si>
+    <t>Type of test</t>
+  </si>
+  <si>
+    <t>GLM</t>
+  </si>
+  <si>
+    <t>Chi-square</t>
+  </si>
+  <si>
+    <t>One-way ANOVA</t>
+  </si>
+  <si>
+    <t>Two proportions</t>
+  </si>
+  <si>
+    <t>Proportion</t>
+  </si>
+  <si>
+    <t>Chi-square test</t>
+  </si>
+  <si>
+    <t>Plot type for numeric variables</t>
+  </si>
+  <si>
+    <t>Plot type for non-numeric variables</t>
+  </si>
+  <si>
+    <t>(same sample sizes)</t>
+  </si>
+  <si>
+    <t>(different sample sizes)</t>
   </si>
 </sst>
 </file>
@@ -2080,10 +2167,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C853ECA4-158B-4D85-A448-9ECE56776B5F}">
-  <dimension ref="A1:C287"/>
+  <dimension ref="A1:C302"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A103" workbookViewId="0">
-      <selection activeCell="B119" sqref="B119"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -2106,3154 +2193,3319 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A2" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>3</v>
+      <c r="A2" s="1" t="s">
+        <v>569</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>590</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>569</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A3" s="2" t="s">
-        <v>526</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>527</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>526</v>
+      <c r="A3" s="1" t="s">
+        <v>570</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>591</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>570</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A4" s="2" t="s">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>13</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A5" s="2" t="s">
-        <v>15</v>
+        <v>526</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>14</v>
+        <v>527</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>15</v>
+        <v>526</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A6" s="2" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A7" s="1" t="s">
-        <v>443</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>443</v>
+      <c r="A7" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A8" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A9" s="1" t="s">
-        <v>442</v>
+        <v>443</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>442</v>
+        <v>443</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A10" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A11" s="2" t="s">
-        <v>380</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>381</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>380</v>
+      <c r="A11" s="1" t="s">
+        <v>442</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>442</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A12" s="2" t="s">
-        <v>382</v>
+        <v>20</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>383</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>382</v>
+        <v>21</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A13" s="2" t="s">
-        <v>433</v>
+        <v>380</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>23</v>
+        <v>381</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>433</v>
+        <v>380</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A14" s="2" t="s">
-        <v>22</v>
+        <v>382</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>22</v>
+        <v>383</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>382</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A15" s="2" t="s">
-        <v>24</v>
+        <v>433</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>433</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A16" s="2" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A17" s="2" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A18" s="2" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A19" s="2" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A20" s="2" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A21" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A22" s="2" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A23" s="2" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A24" s="2" t="s">
-        <v>450</v>
+        <v>35</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>451</v>
+        <v>36</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>450</v>
+        <v>35</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A25" s="1" t="s">
-        <v>469</v>
+      <c r="A25" s="2" t="s">
+        <v>37</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>481</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>469</v>
+        <v>36</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A26" s="2" t="s">
-        <v>356</v>
+        <v>450</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>357</v>
+        <v>451</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>356</v>
+        <v>450</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A27" s="2" t="s">
-        <v>38</v>
+      <c r="A27" s="1" t="s">
+        <v>469</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="C27" s="3" t="s">
-        <v>38</v>
+        <v>481</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>469</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A28" s="2" t="s">
-        <v>7</v>
+        <v>356</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>8</v>
+        <v>357</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>7</v>
+        <v>356</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A29" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>434</v>
+        <v>39</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A30" s="2" t="s">
-        <v>41</v>
+        <v>7</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>42</v>
+        <v>8</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>41</v>
+        <v>7</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A31" s="2" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>44</v>
+        <v>434</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A32" s="1" t="s">
+        <v>563</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>578</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>563</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A33" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A34" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C34" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A35" s="1" t="s">
         <v>541</v>
       </c>
-      <c r="B32" s="1" t="s">
+      <c r="B35" s="1" t="s">
         <v>553</v>
       </c>
-      <c r="C32" s="1" t="s">
+      <c r="C35" s="1" t="s">
         <v>541</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A33" s="1" t="s">
-        <v>514</v>
-      </c>
-      <c r="B33" s="1" t="s">
-        <v>520</v>
-      </c>
-      <c r="C33" s="1" t="s">
-        <v>514</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A34" s="1" t="s">
-        <v>513</v>
-      </c>
-      <c r="B34" s="1" t="s">
-        <v>521</v>
-      </c>
-      <c r="C34" s="1" t="s">
-        <v>513</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A35" s="2" t="s">
-        <v>384</v>
-      </c>
-      <c r="B35" s="2" t="s">
-        <v>385</v>
-      </c>
-      <c r="C35" s="2" t="s">
-        <v>384</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A36" s="1" t="s">
-        <v>512</v>
-      </c>
-      <c r="B36" s="2" t="s">
-        <v>519</v>
+        <v>514</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>520</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>512</v>
+        <v>514</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A37" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="B37" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="C37" s="3" t="s">
-        <v>45</v>
+      <c r="A37" s="1" t="s">
+        <v>513</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>521</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>513</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A38" s="2" t="s">
-        <v>504</v>
+        <v>384</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>505</v>
+        <v>385</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>504</v>
+        <v>384</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A39" s="2" t="s">
-        <v>47</v>
+      <c r="A39" s="1" t="s">
+        <v>512</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="C39" s="3" t="s">
-        <v>47</v>
+        <v>519</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>512</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A40" s="2" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A41" s="2" t="s">
-        <v>360</v>
+        <v>504</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>361</v>
+        <v>505</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>360</v>
+        <v>504</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A42" s="2" t="s">
-        <v>368</v>
+        <v>47</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>369</v>
-      </c>
-      <c r="C42" s="2" t="s">
-        <v>368</v>
+        <v>48</v>
+      </c>
+      <c r="C42" s="3" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A43" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A44" s="2" t="s">
-        <v>390</v>
+        <v>360</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>393</v>
+        <v>361</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>390</v>
+        <v>360</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A45" s="2" t="s">
-        <v>559</v>
+        <v>368</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>561</v>
+        <v>369</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>559</v>
+        <v>368</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A46" s="1" t="s">
-        <v>411</v>
+      <c r="A46" s="2" t="s">
+        <v>51</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>422</v>
-      </c>
-      <c r="C46" s="1" t="s">
-        <v>411</v>
+        <v>52</v>
+      </c>
+      <c r="C46" s="3" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A47" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="B47" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="C47" s="3" t="s">
-        <v>53</v>
+      <c r="A47" s="1" t="s">
+        <v>577</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>579</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>577</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A48" s="2" t="s">
-        <v>344</v>
+        <v>390</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>345</v>
-      </c>
-      <c r="C48" s="3" t="s">
-        <v>344</v>
+        <v>393</v>
+      </c>
+      <c r="C48" s="2" t="s">
+        <v>390</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A49" s="2" t="s">
-        <v>55</v>
+        <v>559</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="C49" s="3" t="s">
-        <v>55</v>
+        <v>561</v>
+      </c>
+      <c r="C49" s="2" t="s">
+        <v>559</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A50" s="1" t="s">
-        <v>406</v>
-      </c>
-      <c r="B50" s="1" t="s">
-        <v>424</v>
+        <v>411</v>
+      </c>
+      <c r="B50" s="2" t="s">
+        <v>422</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>406</v>
+        <v>411</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A51" s="2" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A52" s="2" t="s">
-        <v>59</v>
+        <v>344</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>60</v>
+        <v>345</v>
       </c>
       <c r="C52" s="3" t="s">
-        <v>59</v>
+        <v>344</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A53" s="2" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="C53" s="3" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A54" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="B54" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="C54" s="2" t="s">
-        <v>63</v>
+      <c r="A54" s="1" t="s">
+        <v>406</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>424</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>406</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A55" s="1" t="s">
-        <v>507</v>
+      <c r="A55" s="2" t="s">
+        <v>57</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>508</v>
-      </c>
-      <c r="C55" s="1" t="s">
-        <v>507</v>
+        <v>58</v>
+      </c>
+      <c r="C55" s="3" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A56" s="2" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="C56" s="2" t="s">
-        <v>65</v>
+        <v>60</v>
+      </c>
+      <c r="C56" s="3" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A57" s="2" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="C57" s="3" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A58" s="2" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="C58" s="3" t="s">
-        <v>69</v>
+        <v>64</v>
+      </c>
+      <c r="C58" s="2" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A59" s="2" t="s">
-        <v>465</v>
+      <c r="A59" s="1" t="s">
+        <v>507</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>467</v>
-      </c>
-      <c r="C59" s="2" t="s">
-        <v>465</v>
+        <v>508</v>
+      </c>
+      <c r="C59" s="1" t="s">
+        <v>507</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A60" s="2" t="s">
-        <v>336</v>
+        <v>65</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>337</v>
-      </c>
-      <c r="C60" s="3" t="s">
-        <v>336</v>
+        <v>66</v>
+      </c>
+      <c r="C60" s="2" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A61" s="2" t="s">
-        <v>348</v>
+        <v>67</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>349</v>
-      </c>
-      <c r="C61" s="2" t="s">
-        <v>348</v>
+        <v>68</v>
+      </c>
+      <c r="C61" s="3" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A62" s="1" t="s">
-        <v>436</v>
-      </c>
-      <c r="B62" s="1" t="s">
-        <v>437</v>
-      </c>
-      <c r="C62" s="1" t="s">
-        <v>436</v>
+      <c r="A62" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="B62" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="C62" s="3" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A63" s="2" t="s">
-        <v>71</v>
+        <v>465</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="C63" s="3" t="s">
-        <v>71</v>
+        <v>467</v>
+      </c>
+      <c r="C63" s="2" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A64" s="2" t="s">
-        <v>73</v>
+        <v>336</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>74</v>
+        <v>337</v>
       </c>
       <c r="C64" s="3" t="s">
-        <v>73</v>
+        <v>336</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A65" s="2" t="s">
-        <v>75</v>
+        <v>348</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="C65" s="3" t="s">
-        <v>75</v>
+        <v>349</v>
+      </c>
+      <c r="C65" s="2" t="s">
+        <v>348</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A66" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="B66" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="C66" s="3" t="s">
-        <v>77</v>
+      <c r="A66" s="1" t="s">
+        <v>436</v>
+      </c>
+      <c r="B66" s="1" t="s">
+        <v>437</v>
+      </c>
+      <c r="C66" s="1" t="s">
+        <v>436</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A67" s="2" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="C67" s="3" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A68" s="2" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="C68" s="3" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A69" s="2" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="C69" s="2" t="s">
-        <v>83</v>
+        <v>76</v>
+      </c>
+      <c r="C69" s="3" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A70" s="2" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="C70" s="3" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A71" s="2" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
       <c r="C71" s="3" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A72" s="2" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
       <c r="C72" s="3" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A73" s="1" t="s">
-        <v>405</v>
+      <c r="A73" s="2" t="s">
+        <v>83</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>416</v>
-      </c>
-      <c r="C73" s="1" t="s">
-        <v>405</v>
+        <v>84</v>
+      </c>
+      <c r="C73" s="2" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A74" s="1" t="s">
-        <v>404</v>
+      <c r="A74" s="2" t="s">
+        <v>85</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>415</v>
-      </c>
-      <c r="C74" s="1" t="s">
-        <v>404</v>
+        <v>86</v>
+      </c>
+      <c r="C74" s="3" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A75" s="2" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="C75" s="2" t="s">
-        <v>91</v>
+        <v>88</v>
+      </c>
+      <c r="C75" s="3" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A76" s="2" t="s">
-        <v>372</v>
+        <v>89</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>373</v>
-      </c>
-      <c r="C76" s="2" t="s">
-        <v>372</v>
+        <v>90</v>
+      </c>
+      <c r="C76" s="3" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A77" s="2" t="s">
-        <v>93</v>
+      <c r="A77" s="1" t="s">
+        <v>405</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="C77" s="3" t="s">
-        <v>93</v>
+        <v>416</v>
+      </c>
+      <c r="C77" s="1" t="s">
+        <v>405</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A78" s="2" t="s">
-        <v>95</v>
+      <c r="A78" s="1" t="s">
+        <v>404</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>435</v>
-      </c>
-      <c r="C78" s="3" t="s">
-        <v>95</v>
+        <v>415</v>
+      </c>
+      <c r="C78" s="1" t="s">
+        <v>404</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A79" s="2" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="C79" s="3" t="s">
-        <v>96</v>
+        <v>92</v>
+      </c>
+      <c r="C79" s="2" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A80" s="1" t="s">
-        <v>535</v>
+        <v>568</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>546</v>
+        <v>585</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>535</v>
+        <v>568</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A81" s="1" t="s">
-        <v>537</v>
-      </c>
-      <c r="B81" s="1" t="s">
-        <v>547</v>
-      </c>
-      <c r="C81" s="1" t="s">
-        <v>537</v>
+      <c r="A81" s="2" t="s">
+        <v>372</v>
+      </c>
+      <c r="B81" s="2" t="s">
+        <v>373</v>
+      </c>
+      <c r="C81" s="2" t="s">
+        <v>372</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A82" s="2" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="C82" s="3" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A83" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="B83" s="2" t="s">
-        <v>101</v>
+        <v>435</v>
       </c>
       <c r="C83" s="3" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A84" s="2" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="B84" s="2" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="C84" s="3" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A85" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="B85" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="C85" s="3" t="s">
-        <v>104</v>
+      <c r="A85" s="1" t="s">
+        <v>535</v>
+      </c>
+      <c r="B85" s="1" t="s">
+        <v>546</v>
+      </c>
+      <c r="C85" s="1" t="s">
+        <v>535</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A86" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="B86" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="C86" s="3" t="s">
-        <v>106</v>
+      <c r="A86" s="1" t="s">
+        <v>537</v>
+      </c>
+      <c r="B86" s="1" t="s">
+        <v>547</v>
+      </c>
+      <c r="C86" s="1" t="s">
+        <v>537</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A87" s="2" t="s">
-        <v>498</v>
+        <v>98</v>
       </c>
       <c r="B87" s="2" t="s">
-        <v>499</v>
-      </c>
-      <c r="C87" s="2" t="s">
-        <v>498</v>
+        <v>99</v>
+      </c>
+      <c r="C87" s="3" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A88" s="2" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="B88" s="2" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="C88" s="3" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A89" s="2" t="s">
-        <v>110</v>
+        <v>102</v>
       </c>
       <c r="B89" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="C89" s="2" t="s">
-        <v>110</v>
+        <v>103</v>
+      </c>
+      <c r="C89" s="3" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A90" s="2" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
       <c r="B90" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="C90" s="2" t="s">
-        <v>112</v>
+        <v>105</v>
+      </c>
+      <c r="C90" s="3" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A91" s="2" t="s">
-        <v>114</v>
+        <v>106</v>
       </c>
       <c r="B91" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="C91" s="2" t="s">
-        <v>114</v>
+        <v>107</v>
+      </c>
+      <c r="C91" s="3" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A92" s="1" t="s">
-        <v>452</v>
+      <c r="A92" s="2" t="s">
+        <v>498</v>
       </c>
       <c r="B92" s="2" t="s">
-        <v>453</v>
-      </c>
-      <c r="C92" s="1" t="s">
-        <v>452</v>
+        <v>499</v>
+      </c>
+      <c r="C92" s="2" t="s">
+        <v>498</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A93" s="2" t="s">
-        <v>116</v>
+        <v>108</v>
       </c>
       <c r="B93" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="C93" s="2" t="s">
-        <v>116</v>
+        <v>109</v>
+      </c>
+      <c r="C93" s="3" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A94" s="2" t="s">
-        <v>456</v>
+        <v>110</v>
       </c>
       <c r="B94" s="2" t="s">
-        <v>461</v>
-      </c>
-      <c r="C94" s="3" t="s">
-        <v>456</v>
+        <v>111</v>
+      </c>
+      <c r="C94" s="2" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A95" s="2" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="B95" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="C95" s="3" t="s">
-        <v>118</v>
+        <v>113</v>
+      </c>
+      <c r="C95" s="2" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A96" s="2" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="B96" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="C96" s="3" t="s">
-        <v>120</v>
+        <v>115</v>
+      </c>
+      <c r="C96" s="2" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A97" s="2" t="s">
-        <v>122</v>
+      <c r="A97" s="1" t="s">
+        <v>452</v>
       </c>
       <c r="B97" s="2" t="s">
-        <v>123</v>
-      </c>
-      <c r="C97" s="3" t="s">
-        <v>122</v>
+        <v>453</v>
+      </c>
+      <c r="C97" s="1" t="s">
+        <v>452</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A98" s="2" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
       <c r="B98" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="C98" s="3" t="s">
-        <v>124</v>
+        <v>117</v>
+      </c>
+      <c r="C98" s="2" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A99" s="2" t="s">
-        <v>126</v>
+        <v>456</v>
       </c>
       <c r="B99" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="C99" s="2" t="s">
-        <v>126</v>
+        <v>461</v>
+      </c>
+      <c r="C99" s="3" t="s">
+        <v>456</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A100" s="1" t="s">
-        <v>538</v>
-      </c>
-      <c r="B100" s="1" t="s">
-        <v>543</v>
-      </c>
-      <c r="C100" s="1" t="s">
-        <v>538</v>
+      <c r="A100" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="B100" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="C100" s="3" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A101" s="1" t="s">
-        <v>539</v>
-      </c>
-      <c r="B101" s="1" t="s">
-        <v>542</v>
-      </c>
-      <c r="C101" s="1" t="s">
-        <v>539</v>
+      <c r="A101" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="B101" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="C101" s="3" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A102" s="2" t="s">
-        <v>362</v>
+        <v>122</v>
       </c>
       <c r="B102" s="2" t="s">
-        <v>363</v>
-      </c>
-      <c r="C102" s="2" t="s">
-        <v>362</v>
+        <v>123</v>
+      </c>
+      <c r="C102" s="3" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A103" s="2" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="B103" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="C103" s="2" t="s">
-        <v>128</v>
+        <v>125</v>
+      </c>
+      <c r="C103" s="3" t="s">
+        <v>124</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A104" s="2" t="s">
-        <v>386</v>
+        <v>126</v>
       </c>
       <c r="B104" s="2" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="C104" s="2" t="s">
-        <v>386</v>
+        <v>126</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A105" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="B105" s="2" t="s">
-        <v>131</v>
-      </c>
-      <c r="C105" s="3" t="s">
-        <v>130</v>
+      <c r="A105" s="1" t="s">
+        <v>538</v>
+      </c>
+      <c r="B105" s="1" t="s">
+        <v>543</v>
+      </c>
+      <c r="C105" s="1" t="s">
+        <v>538</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A106" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="B106" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="C106" s="3" t="s">
-        <v>132</v>
+      <c r="A106" s="1" t="s">
+        <v>539</v>
+      </c>
+      <c r="B106" s="1" t="s">
+        <v>542</v>
+      </c>
+      <c r="C106" s="1" t="s">
+        <v>539</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A107" s="2" t="s">
-        <v>134</v>
+        <v>362</v>
       </c>
       <c r="B107" s="2" t="s">
-        <v>135</v>
+        <v>363</v>
       </c>
       <c r="C107" s="2" t="s">
-        <v>134</v>
+        <v>362</v>
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A108" s="2" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
       <c r="B108" s="2" t="s">
-        <v>137</v>
-      </c>
-      <c r="C108" s="3" t="s">
-        <v>136</v>
+        <v>129</v>
+      </c>
+      <c r="C108" s="2" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A109" s="1" t="s">
-        <v>407</v>
+      <c r="A109" s="2" t="s">
+        <v>386</v>
       </c>
       <c r="B109" s="2" t="s">
-        <v>417</v>
-      </c>
-      <c r="C109" s="1" t="s">
-        <v>407</v>
+        <v>129</v>
+      </c>
+      <c r="C109" s="2" t="s">
+        <v>386</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A110" s="2" t="s">
-        <v>138</v>
+        <v>130</v>
       </c>
       <c r="B110" s="2" t="s">
-        <v>139</v>
+        <v>131</v>
       </c>
       <c r="C110" s="3" t="s">
-        <v>138</v>
+        <v>130</v>
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A111" s="2" t="s">
-        <v>140</v>
+        <v>132</v>
       </c>
       <c r="B111" s="2" t="s">
-        <v>141</v>
+        <v>133</v>
       </c>
       <c r="C111" s="3" t="s">
-        <v>140</v>
+        <v>132</v>
       </c>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A112" s="2" t="s">
-        <v>142</v>
+        <v>134</v>
       </c>
       <c r="B112" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="C112" s="3" t="s">
-        <v>142</v>
+        <v>135</v>
+      </c>
+      <c r="C112" s="2" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A113" s="2" t="s">
-        <v>144</v>
+        <v>136</v>
       </c>
       <c r="B113" s="2" t="s">
-        <v>145</v>
+        <v>137</v>
       </c>
       <c r="C113" s="3" t="s">
-        <v>144</v>
+        <v>136</v>
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A114" s="2" t="s">
-        <v>146</v>
+      <c r="A114" s="1" t="s">
+        <v>407</v>
       </c>
       <c r="B114" s="2" t="s">
-        <v>147</v>
-      </c>
-      <c r="C114" s="3" t="s">
-        <v>146</v>
+        <v>417</v>
+      </c>
+      <c r="C114" s="1" t="s">
+        <v>407</v>
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A115" s="2" t="s">
-        <v>148</v>
+        <v>138</v>
       </c>
       <c r="B115" s="2" t="s">
-        <v>149</v>
+        <v>139</v>
       </c>
       <c r="C115" s="3" t="s">
-        <v>148</v>
+        <v>138</v>
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A116" s="2" t="s">
-        <v>150</v>
+        <v>140</v>
       </c>
       <c r="B116" s="2" t="s">
-        <v>151</v>
+        <v>141</v>
       </c>
       <c r="C116" s="3" t="s">
-        <v>150</v>
+        <v>140</v>
       </c>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A117" s="2" t="s">
-        <v>152</v>
+        <v>142</v>
       </c>
       <c r="B117" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="C117" s="2" t="s">
-        <v>152</v>
+        <v>143</v>
+      </c>
+      <c r="C117" s="3" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A118" s="2" t="s">
-        <v>426</v>
+        <v>144</v>
       </c>
       <c r="B118" s="2" t="s">
-        <v>427</v>
-      </c>
-      <c r="C118" s="2" t="s">
-        <v>426</v>
+        <v>145</v>
+      </c>
+      <c r="C118" s="3" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A119" s="2" t="s">
-        <v>154</v>
+        <v>146</v>
       </c>
       <c r="B119" s="2" t="s">
-        <v>155</v>
-      </c>
-      <c r="C119" s="2" t="s">
-        <v>154</v>
+        <v>147</v>
+      </c>
+      <c r="C119" s="3" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A120" s="2" t="s">
-        <v>457</v>
+        <v>148</v>
       </c>
       <c r="B120" s="2" t="s">
-        <v>460</v>
+        <v>149</v>
       </c>
       <c r="C120" s="3" t="s">
-        <v>457</v>
+        <v>148</v>
       </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A121" s="2" t="s">
-        <v>458</v>
+        <v>150</v>
       </c>
       <c r="B121" s="2" t="s">
-        <v>459</v>
+        <v>151</v>
       </c>
       <c r="C121" s="3" t="s">
-        <v>458</v>
+        <v>150</v>
       </c>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A122" s="1" t="s">
-        <v>536</v>
-      </c>
-      <c r="B122" s="1" t="s">
-        <v>548</v>
-      </c>
-      <c r="C122" s="1" t="s">
-        <v>536</v>
+      <c r="A122" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="B122" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="C122" s="2" t="s">
+        <v>152</v>
       </c>
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A123" s="1" t="s">
-        <v>412</v>
-      </c>
-      <c r="B123" s="1" t="s">
-        <v>419</v>
-      </c>
-      <c r="C123" s="1" t="s">
-        <v>412</v>
+      <c r="A123" s="2" t="s">
+        <v>426</v>
+      </c>
+      <c r="B123" s="2" t="s">
+        <v>427</v>
+      </c>
+      <c r="C123" s="2" t="s">
+        <v>426</v>
       </c>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A124" s="2" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B124" s="2" t="s">
-        <v>157</v>
-      </c>
-      <c r="C124" s="3" t="s">
-        <v>156</v>
+        <v>155</v>
+      </c>
+      <c r="C124" s="2" t="s">
+        <v>154</v>
       </c>
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A125" s="1" t="s">
-        <v>479</v>
+      <c r="A125" s="2" t="s">
+        <v>457</v>
       </c>
       <c r="B125" s="2" t="s">
-        <v>491</v>
-      </c>
-      <c r="C125" s="1" t="s">
-        <v>479</v>
+        <v>460</v>
+      </c>
+      <c r="C125" s="3" t="s">
+        <v>457</v>
       </c>
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A126" s="1" t="s">
-        <v>476</v>
+      <c r="A126" s="2" t="s">
+        <v>458</v>
       </c>
       <c r="B126" s="2" t="s">
-        <v>488</v>
-      </c>
-      <c r="C126" s="1" t="s">
-        <v>476</v>
+        <v>459</v>
+      </c>
+      <c r="C126" s="3" t="s">
+        <v>458</v>
       </c>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A127" s="1" t="s">
-        <v>477</v>
-      </c>
-      <c r="B127" s="2" t="s">
-        <v>489</v>
+        <v>536</v>
+      </c>
+      <c r="B127" s="1" t="s">
+        <v>548</v>
       </c>
       <c r="C127" s="1" t="s">
-        <v>477</v>
+        <v>536</v>
       </c>
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A128" s="2" t="s">
-        <v>158</v>
-      </c>
-      <c r="B128" s="2" t="s">
-        <v>159</v>
-      </c>
-      <c r="C128" s="2" t="s">
-        <v>158</v>
+      <c r="A128" s="1" t="s">
+        <v>412</v>
+      </c>
+      <c r="B128" s="1" t="s">
+        <v>419</v>
+      </c>
+      <c r="C128" s="1" t="s">
+        <v>412</v>
       </c>
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A129" s="2" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="B129" s="2" t="s">
-        <v>387</v>
+        <v>157</v>
       </c>
       <c r="C129" s="3" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A130" s="1" t="s">
-        <v>532</v>
+        <v>479</v>
       </c>
       <c r="B130" s="2" t="s">
-        <v>544</v>
+        <v>491</v>
       </c>
       <c r="C130" s="1" t="s">
-        <v>532</v>
+        <v>479</v>
       </c>
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A131" s="2" t="s">
-        <v>161</v>
+      <c r="A131" s="1" t="s">
+        <v>476</v>
       </c>
       <c r="B131" s="2" t="s">
-        <v>162</v>
-      </c>
-      <c r="C131" s="3" t="s">
-        <v>161</v>
+        <v>488</v>
+      </c>
+      <c r="C131" s="1" t="s">
+        <v>476</v>
       </c>
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A132" s="2" t="s">
-        <v>524</v>
+      <c r="A132" s="1" t="s">
+        <v>477</v>
       </c>
       <c r="B132" s="2" t="s">
-        <v>525</v>
-      </c>
-      <c r="C132" s="2" t="s">
-        <v>524</v>
+        <v>489</v>
+      </c>
+      <c r="C132" s="1" t="s">
+        <v>477</v>
       </c>
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A133" s="2" t="s">
-        <v>523</v>
+        <v>158</v>
       </c>
       <c r="B133" s="2" t="s">
-        <v>562</v>
+        <v>159</v>
       </c>
       <c r="C133" s="2" t="s">
-        <v>523</v>
+        <v>158</v>
       </c>
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A134" s="2" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="B134" s="2" t="s">
-        <v>164</v>
+        <v>387</v>
       </c>
       <c r="C134" s="3" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A135" s="2" t="s">
-        <v>165</v>
+      <c r="A135" s="1" t="s">
+        <v>532</v>
       </c>
       <c r="B135" s="2" t="s">
-        <v>166</v>
-      </c>
-      <c r="C135" s="3" t="s">
-        <v>165</v>
+        <v>544</v>
+      </c>
+      <c r="C135" s="1" t="s">
+        <v>532</v>
       </c>
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A136" s="2" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
       <c r="B136" s="2" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
       <c r="C136" s="3" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A137" s="2" t="s">
-        <v>169</v>
+        <v>524</v>
       </c>
       <c r="B137" s="2" t="s">
-        <v>170</v>
-      </c>
-      <c r="C137" s="3" t="s">
-        <v>169</v>
+        <v>525</v>
+      </c>
+      <c r="C137" s="2" t="s">
+        <v>524</v>
       </c>
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A138" s="2" t="s">
-        <v>171</v>
+        <v>523</v>
       </c>
       <c r="B138" s="2" t="s">
-        <v>162</v>
-      </c>
-      <c r="C138" s="3" t="s">
-        <v>171</v>
+        <v>562</v>
+      </c>
+      <c r="C138" s="2" t="s">
+        <v>523</v>
       </c>
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A139" s="2" t="s">
-        <v>172</v>
-      </c>
-      <c r="B139" s="2" t="s">
-        <v>173</v>
-      </c>
-      <c r="C139" s="3" t="s">
-        <v>172</v>
+      <c r="A139" s="1" t="s">
+        <v>566</v>
+      </c>
+      <c r="B139" s="1" t="s">
+        <v>587</v>
+      </c>
+      <c r="C139" s="1" t="s">
+        <v>566</v>
       </c>
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A140" s="1" t="s">
-        <v>471</v>
+      <c r="A140" s="2" t="s">
+        <v>163</v>
       </c>
       <c r="B140" s="2" t="s">
-        <v>482</v>
-      </c>
-      <c r="C140" s="1" t="s">
-        <v>471</v>
+        <v>164</v>
+      </c>
+      <c r="C140" s="3" t="s">
+        <v>163</v>
       </c>
     </row>
     <row r="141" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A141" s="2" t="s">
-        <v>174</v>
+        <v>165</v>
       </c>
       <c r="B141" s="2" t="s">
-        <v>175</v>
+        <v>166</v>
       </c>
       <c r="C141" s="3" t="s">
-        <v>174</v>
+        <v>165</v>
       </c>
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A142" s="1" t="s">
-        <v>396</v>
+      <c r="A142" s="2" t="s">
+        <v>167</v>
       </c>
       <c r="B142" s="2" t="s">
-        <v>397</v>
-      </c>
-      <c r="C142" s="1" t="s">
-        <v>396</v>
+        <v>168</v>
+      </c>
+      <c r="C142" s="3" t="s">
+        <v>167</v>
       </c>
     </row>
     <row r="143" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A143" s="2" t="s">
-        <v>350</v>
+        <v>169</v>
       </c>
       <c r="B143" s="2" t="s">
-        <v>351</v>
+        <v>170</v>
       </c>
       <c r="C143" s="3" t="s">
-        <v>350</v>
+        <v>169</v>
       </c>
     </row>
     <row r="144" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A144" s="2" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="B144" s="2" t="s">
-        <v>177</v>
-      </c>
-      <c r="C144" s="2" t="s">
-        <v>176</v>
+        <v>162</v>
+      </c>
+      <c r="C144" s="3" t="s">
+        <v>171</v>
       </c>
     </row>
     <row r="145" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A145" s="2" t="s">
-        <v>388</v>
+        <v>172</v>
       </c>
       <c r="B145" s="2" t="s">
-        <v>391</v>
-      </c>
-      <c r="C145" s="2" t="s">
-        <v>388</v>
+        <v>173</v>
+      </c>
+      <c r="C145" s="3" t="s">
+        <v>172</v>
       </c>
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A146" s="1" t="s">
-        <v>475</v>
+        <v>471</v>
       </c>
       <c r="B146" s="2" t="s">
-        <v>487</v>
+        <v>482</v>
       </c>
       <c r="C146" s="1" t="s">
-        <v>475</v>
+        <v>471</v>
       </c>
     </row>
     <row r="147" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A147" s="2" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="B147" s="2" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="C147" s="3" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
     </row>
     <row r="148" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A148" s="2" t="s">
-        <v>180</v>
+      <c r="A148" s="1" t="s">
+        <v>396</v>
       </c>
       <c r="B148" s="2" t="s">
-        <v>181</v>
-      </c>
-      <c r="C148" s="3" t="s">
-        <v>180</v>
+        <v>397</v>
+      </c>
+      <c r="C148" s="1" t="s">
+        <v>396</v>
       </c>
     </row>
     <row r="149" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A149" s="2" t="s">
-        <v>182</v>
+        <v>350</v>
       </c>
       <c r="B149" s="2" t="s">
-        <v>183</v>
+        <v>351</v>
       </c>
       <c r="C149" s="3" t="s">
-        <v>182</v>
+        <v>350</v>
       </c>
     </row>
     <row r="150" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A150" s="2" t="s">
-        <v>338</v>
+        <v>176</v>
       </c>
       <c r="B150" s="2" t="s">
-        <v>339</v>
-      </c>
-      <c r="C150" s="3" t="s">
-        <v>338</v>
+        <v>177</v>
+      </c>
+      <c r="C150" s="2" t="s">
+        <v>176</v>
       </c>
     </row>
     <row r="151" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A151" s="2" t="s">
-        <v>354</v>
+        <v>388</v>
       </c>
       <c r="B151" s="2" t="s">
-        <v>355</v>
-      </c>
-      <c r="C151" s="3" t="s">
-        <v>354</v>
+        <v>391</v>
+      </c>
+      <c r="C151" s="2" t="s">
+        <v>388</v>
       </c>
     </row>
     <row r="152" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A152" s="2" t="s">
-        <v>352</v>
+      <c r="A152" s="1" t="s">
+        <v>475</v>
       </c>
       <c r="B152" s="2" t="s">
-        <v>353</v>
-      </c>
-      <c r="C152" s="3" t="s">
-        <v>352</v>
+        <v>487</v>
+      </c>
+      <c r="C152" s="1" t="s">
+        <v>475</v>
       </c>
     </row>
     <row r="153" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A153" s="2" t="s">
-        <v>184</v>
+        <v>178</v>
       </c>
       <c r="B153" s="2" t="s">
-        <v>185</v>
-      </c>
-      <c r="C153" s="2" t="s">
-        <v>184</v>
+        <v>179</v>
+      </c>
+      <c r="C153" s="3" t="s">
+        <v>178</v>
       </c>
     </row>
     <row r="154" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A154" s="2" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
       <c r="B154" s="2" t="s">
-        <v>187</v>
+        <v>181</v>
       </c>
       <c r="C154" s="3" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
     </row>
     <row r="155" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A155" s="2" t="s">
-        <v>528</v>
+        <v>182</v>
       </c>
       <c r="B155" s="2" t="s">
-        <v>530</v>
-      </c>
-      <c r="C155" s="2" t="s">
-        <v>528</v>
+        <v>183</v>
+      </c>
+      <c r="C155" s="3" t="s">
+        <v>182</v>
       </c>
     </row>
     <row r="156" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A156" s="2" t="s">
-        <v>188</v>
+        <v>338</v>
       </c>
       <c r="B156" s="2" t="s">
-        <v>189</v>
+        <v>339</v>
       </c>
       <c r="C156" s="3" t="s">
-        <v>188</v>
+        <v>338</v>
       </c>
     </row>
     <row r="157" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A157" s="1" t="s">
-        <v>431</v>
-      </c>
-      <c r="B157" s="1" t="s">
-        <v>432</v>
-      </c>
-      <c r="C157" s="1" t="s">
-        <v>431</v>
+      <c r="A157" s="2" t="s">
+        <v>354</v>
+      </c>
+      <c r="B157" s="2" t="s">
+        <v>355</v>
+      </c>
+      <c r="C157" s="3" t="s">
+        <v>354</v>
       </c>
     </row>
     <row r="158" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A158" s="2" t="s">
-        <v>190</v>
+        <v>352</v>
       </c>
       <c r="B158" s="2" t="s">
-        <v>191</v>
+        <v>353</v>
       </c>
       <c r="C158" s="3" t="s">
-        <v>190</v>
+        <v>352</v>
       </c>
     </row>
     <row r="159" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A159" s="2" t="s">
-        <v>340</v>
+        <v>184</v>
       </c>
       <c r="B159" s="2" t="s">
-        <v>341</v>
-      </c>
-      <c r="C159" s="3" t="s">
-        <v>340</v>
+        <v>185</v>
+      </c>
+      <c r="C159" s="2" t="s">
+        <v>184</v>
       </c>
     </row>
     <row r="160" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A160" s="2" t="s">
-        <v>454</v>
+        <v>186</v>
       </c>
       <c r="B160" s="2" t="s">
-        <v>455</v>
+        <v>187</v>
       </c>
       <c r="C160" s="3" t="s">
-        <v>454</v>
+        <v>186</v>
       </c>
     </row>
     <row r="161" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A161" s="2" t="s">
-        <v>192</v>
+        <v>528</v>
       </c>
       <c r="B161" s="2" t="s">
-        <v>193</v>
-      </c>
-      <c r="C161" s="3" t="s">
-        <v>192</v>
+        <v>530</v>
+      </c>
+      <c r="C161" s="2" t="s">
+        <v>528</v>
       </c>
     </row>
     <row r="162" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A162" s="2" t="s">
-        <v>194</v>
-      </c>
-      <c r="B162" s="2" t="s">
-        <v>195</v>
-      </c>
-      <c r="C162" s="3" t="s">
-        <v>194</v>
+      <c r="A162" s="1" t="s">
+        <v>575</v>
+      </c>
+      <c r="B162" s="1" t="s">
+        <v>578</v>
+      </c>
+      <c r="C162" s="1" t="s">
+        <v>575</v>
       </c>
     </row>
     <row r="163" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A163" s="1" t="s">
-        <v>500</v>
+      <c r="A163" s="2" t="s">
+        <v>188</v>
       </c>
       <c r="B163" s="2" t="s">
-        <v>501</v>
-      </c>
-      <c r="C163" s="1" t="s">
-        <v>500</v>
+        <v>189</v>
+      </c>
+      <c r="C163" s="3" t="s">
+        <v>188</v>
       </c>
     </row>
     <row r="164" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A164" s="2" t="s">
-        <v>196</v>
-      </c>
-      <c r="B164" s="2" t="s">
-        <v>197</v>
-      </c>
-      <c r="C164" s="3" t="s">
-        <v>196</v>
+      <c r="A164" s="1" t="s">
+        <v>431</v>
+      </c>
+      <c r="B164" s="1" t="s">
+        <v>432</v>
+      </c>
+      <c r="C164" s="1" t="s">
+        <v>431</v>
       </c>
     </row>
     <row r="165" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A165" s="2" t="s">
-        <v>198</v>
+        <v>190</v>
       </c>
       <c r="B165" s="2" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
       <c r="C165" s="3" t="s">
-        <v>198</v>
+        <v>190</v>
       </c>
     </row>
     <row r="166" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A166" s="2" t="s">
-        <v>200</v>
+        <v>340</v>
       </c>
       <c r="B166" s="2" t="s">
-        <v>201</v>
+        <v>341</v>
       </c>
       <c r="C166" s="3" t="s">
-        <v>200</v>
+        <v>340</v>
       </c>
     </row>
     <row r="167" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A167" s="2" t="s">
-        <v>202</v>
+        <v>454</v>
       </c>
       <c r="B167" s="2" t="s">
-        <v>203</v>
+        <v>455</v>
       </c>
       <c r="C167" s="3" t="s">
-        <v>202</v>
+        <v>454</v>
       </c>
     </row>
     <row r="168" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A168" s="2" t="s">
-        <v>204</v>
+        <v>192</v>
       </c>
       <c r="B168" s="2" t="s">
-        <v>205</v>
+        <v>193</v>
       </c>
       <c r="C168" s="3" t="s">
-        <v>204</v>
+        <v>192</v>
       </c>
     </row>
     <row r="169" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A169" s="2" t="s">
-        <v>206</v>
+        <v>194</v>
       </c>
       <c r="B169" s="2" t="s">
-        <v>207</v>
+        <v>195</v>
       </c>
       <c r="C169" s="3" t="s">
-        <v>206</v>
+        <v>194</v>
       </c>
     </row>
     <row r="170" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A170" s="1" t="s">
-        <v>496</v>
+        <v>500</v>
       </c>
       <c r="B170" s="2" t="s">
-        <v>497</v>
+        <v>501</v>
       </c>
       <c r="C170" s="1" t="s">
-        <v>496</v>
+        <v>500</v>
       </c>
     </row>
     <row r="171" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A171" s="2" t="s">
-        <v>529</v>
+        <v>196</v>
       </c>
       <c r="B171" s="2" t="s">
-        <v>531</v>
-      </c>
-      <c r="C171" s="2" t="s">
-        <v>529</v>
+        <v>197</v>
+      </c>
+      <c r="C171" s="3" t="s">
+        <v>196</v>
       </c>
     </row>
     <row r="172" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A172" s="2" t="s">
-        <v>208</v>
+        <v>198</v>
       </c>
       <c r="B172" s="2" t="s">
-        <v>209</v>
+        <v>199</v>
       </c>
       <c r="C172" s="3" t="s">
-        <v>208</v>
+        <v>198</v>
       </c>
     </row>
     <row r="173" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A173" s="2" t="s">
-        <v>358</v>
+        <v>200</v>
       </c>
       <c r="B173" s="2" t="s">
-        <v>359</v>
-      </c>
-      <c r="C173" s="2" t="s">
-        <v>358</v>
+        <v>201</v>
+      </c>
+      <c r="C173" s="3" t="s">
+        <v>200</v>
       </c>
     </row>
     <row r="174" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A174" s="2" t="s">
-        <v>210</v>
+        <v>202</v>
       </c>
       <c r="B174" s="2" t="s">
-        <v>211</v>
+        <v>203</v>
       </c>
       <c r="C174" s="3" t="s">
-        <v>210</v>
+        <v>202</v>
       </c>
     </row>
     <row r="175" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A175" s="2" t="s">
-        <v>212</v>
+        <v>204</v>
       </c>
       <c r="B175" s="2" t="s">
-        <v>213</v>
+        <v>205</v>
       </c>
       <c r="C175" s="3" t="s">
-        <v>212</v>
+        <v>204</v>
       </c>
     </row>
     <row r="176" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A176" s="2" t="s">
-        <v>389</v>
+        <v>206</v>
       </c>
       <c r="B176" s="2" t="s">
-        <v>392</v>
-      </c>
-      <c r="C176" s="2" t="s">
-        <v>389</v>
+        <v>207</v>
+      </c>
+      <c r="C176" s="3" t="s">
+        <v>206</v>
       </c>
     </row>
     <row r="177" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A177" s="2" t="s">
-        <v>558</v>
+      <c r="A177" s="1" t="s">
+        <v>496</v>
       </c>
       <c r="B177" s="2" t="s">
-        <v>560</v>
-      </c>
-      <c r="C177" s="2" t="s">
-        <v>558</v>
+        <v>497</v>
+      </c>
+      <c r="C177" s="1" t="s">
+        <v>496</v>
       </c>
     </row>
     <row r="178" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A178" s="1" t="s">
-        <v>410</v>
-      </c>
-      <c r="B178" s="1" t="s">
-        <v>421</v>
-      </c>
-      <c r="C178" s="1" t="s">
-        <v>410</v>
+      <c r="A178" s="2" t="s">
+        <v>529</v>
+      </c>
+      <c r="B178" s="2" t="s">
+        <v>531</v>
+      </c>
+      <c r="C178" s="2" t="s">
+        <v>529</v>
       </c>
     </row>
     <row r="179" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A179" s="2" t="s">
-        <v>214</v>
+        <v>208</v>
       </c>
       <c r="B179" s="2" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
       <c r="C179" s="3" t="s">
-        <v>214</v>
+        <v>208</v>
       </c>
     </row>
     <row r="180" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A180" s="2" t="s">
-        <v>216</v>
+        <v>358</v>
       </c>
       <c r="B180" s="2" t="s">
-        <v>217</v>
-      </c>
-      <c r="C180" s="3" t="s">
-        <v>216</v>
+        <v>359</v>
+      </c>
+      <c r="C180" s="2" t="s">
+        <v>358</v>
       </c>
     </row>
     <row r="181" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A181" s="2" t="s">
-        <v>218</v>
+        <v>210</v>
       </c>
       <c r="B181" s="2" t="s">
-        <v>219</v>
+        <v>211</v>
       </c>
       <c r="C181" s="3" t="s">
-        <v>218</v>
+        <v>210</v>
       </c>
     </row>
     <row r="182" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A182" s="2" t="s">
-        <v>220</v>
+        <v>212</v>
       </c>
       <c r="B182" s="2" t="s">
-        <v>221</v>
-      </c>
-      <c r="C182" s="2" t="s">
-        <v>220</v>
+        <v>213</v>
+      </c>
+      <c r="C182" s="3" t="s">
+        <v>212</v>
       </c>
     </row>
     <row r="183" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A183" s="1" t="s">
-        <v>444</v>
-      </c>
-      <c r="B183" s="1" t="s">
-        <v>446</v>
-      </c>
-      <c r="C183" s="1" t="s">
-        <v>444</v>
+      <c r="A183" s="2" t="s">
+        <v>389</v>
+      </c>
+      <c r="B183" s="2" t="s">
+        <v>392</v>
+      </c>
+      <c r="C183" s="2" t="s">
+        <v>389</v>
       </c>
     </row>
     <row r="184" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A184" s="2" t="s">
-        <v>376</v>
+        <v>558</v>
       </c>
       <c r="B184" s="2" t="s">
-        <v>377</v>
+        <v>560</v>
       </c>
       <c r="C184" s="2" t="s">
-        <v>376</v>
+        <v>558</v>
       </c>
     </row>
     <row r="185" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A185" s="2" t="s">
-        <v>222</v>
-      </c>
-      <c r="B185" s="2" t="s">
-        <v>223</v>
-      </c>
-      <c r="C185" s="3" t="s">
-        <v>222</v>
+      <c r="A185" s="1" t="s">
+        <v>410</v>
+      </c>
+      <c r="B185" s="1" t="s">
+        <v>421</v>
+      </c>
+      <c r="C185" s="1" t="s">
+        <v>410</v>
       </c>
     </row>
     <row r="186" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A186" s="2" t="s">
-        <v>346</v>
+        <v>214</v>
       </c>
       <c r="B186" s="2" t="s">
-        <v>347</v>
+        <v>215</v>
       </c>
       <c r="C186" s="3" t="s">
-        <v>346</v>
+        <v>214</v>
       </c>
     </row>
     <row r="187" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A187" s="1" t="s">
-        <v>448</v>
+      <c r="A187" s="2" t="s">
+        <v>216</v>
       </c>
       <c r="B187" s="2" t="s">
-        <v>449</v>
-      </c>
-      <c r="C187" s="1" t="s">
-        <v>448</v>
+        <v>217</v>
+      </c>
+      <c r="C187" s="3" t="s">
+        <v>216</v>
       </c>
     </row>
     <row r="188" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A188" s="2" t="s">
-        <v>224</v>
+        <v>218</v>
       </c>
       <c r="B188" s="2" t="s">
-        <v>225</v>
-      </c>
-      <c r="C188" s="2" t="s">
-        <v>224</v>
+        <v>219</v>
+      </c>
+      <c r="C188" s="3" t="s">
+        <v>218</v>
       </c>
     </row>
     <row r="189" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A189" s="1" t="s">
-        <v>468</v>
+      <c r="A189" s="2" t="s">
+        <v>220</v>
       </c>
       <c r="B189" s="2" t="s">
-        <v>480</v>
-      </c>
-      <c r="C189" s="1" t="s">
-        <v>468</v>
+        <v>221</v>
+      </c>
+      <c r="C189" s="2" t="s">
+        <v>220</v>
       </c>
     </row>
     <row r="190" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A190" s="2" t="s">
-        <v>226</v>
-      </c>
-      <c r="B190" s="2" t="s">
-        <v>227</v>
-      </c>
-      <c r="C190" s="2" t="s">
-        <v>226</v>
+      <c r="A190" s="1" t="s">
+        <v>444</v>
+      </c>
+      <c r="B190" s="1" t="s">
+        <v>446</v>
+      </c>
+      <c r="C190" s="1" t="s">
+        <v>444</v>
       </c>
     </row>
     <row r="191" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A191" s="2" t="s">
-        <v>228</v>
+        <v>376</v>
       </c>
       <c r="B191" s="2" t="s">
-        <v>229</v>
-      </c>
-      <c r="C191" s="3" t="s">
-        <v>228</v>
+        <v>377</v>
+      </c>
+      <c r="C191" s="2" t="s">
+        <v>376</v>
       </c>
     </row>
     <row r="192" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A192" s="2" t="s">
-        <v>230</v>
-      </c>
-      <c r="B192" s="2" t="s">
-        <v>231</v>
-      </c>
-      <c r="C192" s="2" t="s">
-        <v>230</v>
+      <c r="A192" s="1" t="s">
+        <v>573</v>
+      </c>
+      <c r="B192" s="1" t="s">
+        <v>582</v>
+      </c>
+      <c r="C192" s="1" t="s">
+        <v>573</v>
       </c>
     </row>
     <row r="193" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A193" s="2" t="s">
-        <v>232</v>
+        <v>222</v>
       </c>
       <c r="B193" s="2" t="s">
-        <v>233</v>
+        <v>223</v>
       </c>
       <c r="C193" s="3" t="s">
-        <v>232</v>
+        <v>222</v>
       </c>
     </row>
     <row r="194" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A194" s="2" t="s">
-        <v>234</v>
+        <v>346</v>
       </c>
       <c r="B194" s="2" t="s">
-        <v>235</v>
+        <v>347</v>
       </c>
       <c r="C194" s="3" t="s">
-        <v>234</v>
+        <v>346</v>
       </c>
     </row>
     <row r="195" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A195" s="2" t="s">
-        <v>494</v>
+      <c r="A195" s="1" t="s">
+        <v>448</v>
       </c>
       <c r="B195" s="2" t="s">
-        <v>495</v>
-      </c>
-      <c r="C195" s="2" t="s">
-        <v>494</v>
+        <v>449</v>
+      </c>
+      <c r="C195" s="1" t="s">
+        <v>448</v>
       </c>
     </row>
     <row r="196" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A196" s="2" t="s">
-        <v>236</v>
+        <v>224</v>
       </c>
       <c r="B196" s="2" t="s">
-        <v>237</v>
-      </c>
-      <c r="C196" s="3" t="s">
-        <v>236</v>
+        <v>225</v>
+      </c>
+      <c r="C196" s="2" t="s">
+        <v>224</v>
       </c>
     </row>
     <row r="197" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A197" s="2" t="s">
-        <v>238</v>
+      <c r="A197" s="1" t="s">
+        <v>468</v>
       </c>
       <c r="B197" s="2" t="s">
-        <v>402</v>
-      </c>
-      <c r="C197" s="2" t="s">
-        <v>238</v>
+        <v>480</v>
+      </c>
+      <c r="C197" s="1" t="s">
+        <v>468</v>
       </c>
     </row>
     <row r="198" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A198" s="2" t="s">
-        <v>394</v>
+        <v>226</v>
       </c>
       <c r="B198" s="2" t="s">
-        <v>395</v>
+        <v>227</v>
       </c>
       <c r="C198" s="2" t="s">
-        <v>394</v>
+        <v>226</v>
       </c>
     </row>
     <row r="199" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A199" s="2" t="s">
-        <v>464</v>
+        <v>228</v>
       </c>
       <c r="B199" s="2" t="s">
-        <v>466</v>
-      </c>
-      <c r="C199" s="2" t="s">
-        <v>464</v>
+        <v>229</v>
+      </c>
+      <c r="C199" s="3" t="s">
+        <v>228</v>
       </c>
     </row>
     <row r="200" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A200" s="2" t="s">
-        <v>239</v>
-      </c>
-      <c r="B200" s="2" t="s">
-        <v>398</v>
-      </c>
-      <c r="C200" s="2" t="s">
-        <v>239</v>
+      <c r="A200" s="1" t="s">
+        <v>571</v>
+      </c>
+      <c r="B200" s="1" t="s">
+        <v>584</v>
+      </c>
+      <c r="C200" s="1" t="s">
+        <v>571</v>
       </c>
     </row>
     <row r="201" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A201" s="2" t="s">
-        <v>240</v>
+        <v>230</v>
       </c>
       <c r="B201" s="2" t="s">
-        <v>241</v>
+        <v>231</v>
       </c>
       <c r="C201" s="2" t="s">
-        <v>240</v>
+        <v>230</v>
       </c>
     </row>
     <row r="202" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A202" s="2" t="s">
-        <v>242</v>
+        <v>232</v>
       </c>
       <c r="B202" s="2" t="s">
-        <v>243</v>
+        <v>233</v>
       </c>
       <c r="C202" s="3" t="s">
-        <v>242</v>
+        <v>232</v>
       </c>
     </row>
     <row r="203" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A203" s="2" t="s">
-        <v>244</v>
+        <v>234</v>
       </c>
       <c r="B203" s="2" t="s">
-        <v>245</v>
+        <v>235</v>
       </c>
       <c r="C203" s="3" t="s">
-        <v>244</v>
+        <v>234</v>
       </c>
     </row>
     <row r="204" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A204" s="2" t="s">
-        <v>246</v>
+        <v>494</v>
       </c>
       <c r="B204" s="2" t="s">
-        <v>247</v>
+        <v>495</v>
       </c>
       <c r="C204" s="2" t="s">
-        <v>246</v>
+        <v>494</v>
       </c>
     </row>
     <row r="205" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A205" s="2" t="s">
-        <v>248</v>
+        <v>236</v>
       </c>
       <c r="B205" s="2" t="s">
-        <v>429</v>
+        <v>237</v>
       </c>
       <c r="C205" s="3" t="s">
-        <v>248</v>
+        <v>236</v>
       </c>
     </row>
     <row r="206" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A206" s="2" t="s">
-        <v>249</v>
+        <v>238</v>
       </c>
       <c r="B206" s="2" t="s">
-        <v>430</v>
-      </c>
-      <c r="C206" s="3" t="s">
-        <v>249</v>
+        <v>402</v>
+      </c>
+      <c r="C206" s="2" t="s">
+        <v>238</v>
       </c>
     </row>
     <row r="207" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A207" s="2" t="s">
-        <v>462</v>
+        <v>394</v>
       </c>
       <c r="B207" s="2" t="s">
-        <v>463</v>
+        <v>395</v>
       </c>
       <c r="C207" s="2" t="s">
-        <v>462</v>
+        <v>394</v>
       </c>
     </row>
     <row r="208" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A208" s="2" t="s">
-        <v>250</v>
+        <v>464</v>
       </c>
       <c r="B208" s="2" t="s">
-        <v>251</v>
+        <v>466</v>
       </c>
       <c r="C208" s="2" t="s">
-        <v>250</v>
+        <v>464</v>
       </c>
     </row>
     <row r="209" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A209" s="2" t="s">
-        <v>252</v>
+        <v>239</v>
       </c>
       <c r="B209" s="2" t="s">
-        <v>253</v>
-      </c>
-      <c r="C209" s="3" t="s">
-        <v>252</v>
+        <v>398</v>
+      </c>
+      <c r="C209" s="2" t="s">
+        <v>239</v>
       </c>
     </row>
     <row r="210" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A210" s="2" t="s">
-        <v>254</v>
+        <v>240</v>
       </c>
       <c r="B210" s="2" t="s">
-        <v>255</v>
-      </c>
-      <c r="C210" s="3" t="s">
-        <v>254</v>
+        <v>241</v>
+      </c>
+      <c r="C210" s="2" t="s">
+        <v>240</v>
       </c>
     </row>
     <row r="211" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A211" s="2" t="s">
-        <v>256</v>
+        <v>242</v>
       </c>
       <c r="B211" s="2" t="s">
-        <v>257</v>
-      </c>
-      <c r="C211" s="2" t="s">
-        <v>256</v>
+        <v>243</v>
+      </c>
+      <c r="C211" s="3" t="s">
+        <v>242</v>
       </c>
     </row>
     <row r="212" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A212" s="2" t="s">
-        <v>258</v>
+        <v>244</v>
       </c>
       <c r="B212" s="2" t="s">
-        <v>259</v>
+        <v>245</v>
       </c>
       <c r="C212" s="3" t="s">
-        <v>258</v>
+        <v>244</v>
       </c>
     </row>
     <row r="213" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A213" s="2" t="s">
-        <v>260</v>
+        <v>246</v>
       </c>
       <c r="B213" s="2" t="s">
-        <v>261</v>
-      </c>
-      <c r="C213" s="3" t="s">
-        <v>260</v>
+        <v>247</v>
+      </c>
+      <c r="C213" s="2" t="s">
+        <v>246</v>
       </c>
     </row>
     <row r="214" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A214" s="1" t="s">
-        <v>438</v>
-      </c>
-      <c r="B214" s="1" t="s">
-        <v>440</v>
-      </c>
-      <c r="C214" s="1" t="s">
-        <v>438</v>
+      <c r="A214" s="2" t="s">
+        <v>248</v>
+      </c>
+      <c r="B214" s="2" t="s">
+        <v>429</v>
+      </c>
+      <c r="C214" s="3" t="s">
+        <v>248</v>
       </c>
     </row>
     <row r="215" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A215" s="1" t="s">
-        <v>439</v>
-      </c>
-      <c r="B215" s="1" t="s">
-        <v>441</v>
-      </c>
-      <c r="C215" s="1" t="s">
-        <v>439</v>
+      <c r="A215" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="B215" s="2" t="s">
+        <v>430</v>
+      </c>
+      <c r="C215" s="3" t="s">
+        <v>249</v>
       </c>
     </row>
     <row r="216" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A216" s="1" t="s">
-        <v>515</v>
-      </c>
-      <c r="B216" s="1" t="s">
-        <v>522</v>
-      </c>
-      <c r="C216" s="1" t="s">
-        <v>515</v>
+      <c r="A216" s="2" t="s">
+        <v>462</v>
+      </c>
+      <c r="B216" s="2" t="s">
+        <v>463</v>
+      </c>
+      <c r="C216" s="2" t="s">
+        <v>462</v>
       </c>
     </row>
     <row r="217" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A217" s="2" t="s">
-        <v>262</v>
+        <v>250</v>
       </c>
       <c r="B217" s="2" t="s">
-        <v>263</v>
-      </c>
-      <c r="C217" s="3" t="s">
-        <v>262</v>
+        <v>251</v>
+      </c>
+      <c r="C217" s="2" t="s">
+        <v>250</v>
       </c>
     </row>
     <row r="218" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A218" s="2" t="s">
-        <v>400</v>
+        <v>252</v>
       </c>
       <c r="B218" s="2" t="s">
-        <v>401</v>
-      </c>
-      <c r="C218" s="2" t="s">
-        <v>400</v>
+        <v>253</v>
+      </c>
+      <c r="C218" s="3" t="s">
+        <v>252</v>
       </c>
     </row>
     <row r="219" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A219" s="2" t="s">
-        <v>374</v>
+        <v>254</v>
       </c>
       <c r="B219" s="2" t="s">
-        <v>375</v>
-      </c>
-      <c r="C219" s="2" t="s">
-        <v>374</v>
+        <v>255</v>
+      </c>
+      <c r="C219" s="3" t="s">
+        <v>254</v>
       </c>
     </row>
     <row r="220" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A220" s="2" t="s">
-        <v>264</v>
+        <v>256</v>
       </c>
       <c r="B220" s="2" t="s">
-        <v>399</v>
+        <v>257</v>
       </c>
       <c r="C220" s="2" t="s">
-        <v>264</v>
+        <v>256</v>
       </c>
     </row>
     <row r="221" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A221" s="1" t="s">
-        <v>533</v>
+      <c r="A221" s="2" t="s">
+        <v>258</v>
       </c>
       <c r="B221" s="2" t="s">
-        <v>545</v>
-      </c>
-      <c r="C221" s="1" t="s">
-        <v>533</v>
+        <v>259</v>
+      </c>
+      <c r="C221" s="3" t="s">
+        <v>258</v>
       </c>
     </row>
     <row r="222" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A222" s="2" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
       <c r="B222" s="2" t="s">
-        <v>266</v>
+        <v>261</v>
       </c>
       <c r="C222" s="3" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
     </row>
     <row r="223" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A223" s="2" t="s">
-        <v>267</v>
-      </c>
-      <c r="B223" s="2" t="s">
-        <v>268</v>
-      </c>
-      <c r="C223" s="2" t="s">
-        <v>267</v>
+      <c r="A223" s="1" t="s">
+        <v>438</v>
+      </c>
+      <c r="B223" s="1" t="s">
+        <v>440</v>
+      </c>
+      <c r="C223" s="1" t="s">
+        <v>438</v>
       </c>
     </row>
     <row r="224" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A224" s="2" t="s">
-        <v>556</v>
-      </c>
-      <c r="B224" s="2" t="s">
-        <v>557</v>
-      </c>
-      <c r="C224" s="2" t="s">
-        <v>556</v>
+      <c r="A224" s="1" t="s">
+        <v>439</v>
+      </c>
+      <c r="B224" s="1" t="s">
+        <v>441</v>
+      </c>
+      <c r="C224" s="1" t="s">
+        <v>439</v>
       </c>
     </row>
     <row r="225" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A225" s="1" t="s">
-        <v>403</v>
-      </c>
-      <c r="B225" s="2" t="s">
-        <v>414</v>
+        <v>515</v>
+      </c>
+      <c r="B225" s="1" t="s">
+        <v>522</v>
       </c>
       <c r="C225" s="1" t="s">
-        <v>403</v>
+        <v>515</v>
       </c>
     </row>
     <row r="226" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A226" s="2" t="s">
-        <v>269</v>
+        <v>262</v>
       </c>
       <c r="B226" s="2" t="s">
-        <v>270</v>
+        <v>263</v>
       </c>
       <c r="C226" s="3" t="s">
-        <v>269</v>
+        <v>262</v>
       </c>
     </row>
     <row r="227" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A227" s="2" t="s">
-        <v>271</v>
+        <v>400</v>
       </c>
       <c r="B227" s="2" t="s">
-        <v>272</v>
+        <v>401</v>
       </c>
       <c r="C227" s="2" t="s">
-        <v>271</v>
+        <v>400</v>
       </c>
     </row>
     <row r="228" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A228" s="2" t="s">
-        <v>273</v>
+        <v>374</v>
       </c>
       <c r="B228" s="2" t="s">
-        <v>274</v>
-      </c>
-      <c r="C228" s="3" t="s">
-        <v>273</v>
+        <v>375</v>
+      </c>
+      <c r="C228" s="2" t="s">
+        <v>374</v>
       </c>
     </row>
     <row r="229" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A229" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B229" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C229" s="3" t="s">
-        <v>9</v>
+      <c r="A229" s="1" t="s">
+        <v>567</v>
+      </c>
+      <c r="B229" s="1" t="s">
+        <v>586</v>
+      </c>
+      <c r="C229" s="1" t="s">
+        <v>567</v>
       </c>
     </row>
     <row r="230" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A230" s="2" t="s">
-        <v>506</v>
+        <v>264</v>
       </c>
       <c r="B230" s="2" t="s">
-        <v>1</v>
+        <v>399</v>
       </c>
       <c r="C230" s="2" t="s">
-        <v>506</v>
+        <v>264</v>
       </c>
     </row>
     <row r="231" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A231" s="2" t="s">
-        <v>275</v>
+      <c r="A231" s="1" t="s">
+        <v>533</v>
       </c>
       <c r="B231" s="2" t="s">
-        <v>276</v>
-      </c>
-      <c r="C231" s="3" t="s">
-        <v>275</v>
+        <v>545</v>
+      </c>
+      <c r="C231" s="1" t="s">
+        <v>533</v>
       </c>
     </row>
     <row r="232" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A232" s="1" t="s">
-        <v>473</v>
-      </c>
-      <c r="B232" s="2" t="s">
-        <v>484</v>
+        <v>576</v>
+      </c>
+      <c r="B232" s="1" t="s">
+        <v>580</v>
       </c>
       <c r="C232" s="1" t="s">
-        <v>473</v>
+        <v>576</v>
       </c>
     </row>
     <row r="233" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A233" s="2" t="s">
-        <v>378</v>
+        <v>265</v>
       </c>
       <c r="B233" s="2" t="s">
-        <v>379</v>
-      </c>
-      <c r="C233" s="2" t="s">
-        <v>378</v>
+        <v>266</v>
+      </c>
+      <c r="C233" s="3" t="s">
+        <v>265</v>
       </c>
     </row>
     <row r="234" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A234" s="2" t="s">
-        <v>277</v>
+        <v>267</v>
       </c>
       <c r="B234" s="2" t="s">
-        <v>278</v>
-      </c>
-      <c r="C234" s="3" t="s">
-        <v>277</v>
+        <v>268</v>
+      </c>
+      <c r="C234" s="2" t="s">
+        <v>267</v>
       </c>
     </row>
     <row r="235" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A235" s="1" t="s">
-        <v>478</v>
+      <c r="A235" s="2" t="s">
+        <v>556</v>
       </c>
       <c r="B235" s="2" t="s">
-        <v>490</v>
-      </c>
-      <c r="C235" s="1" t="s">
-        <v>478</v>
+        <v>557</v>
+      </c>
+      <c r="C235" s="2" t="s">
+        <v>556</v>
       </c>
     </row>
     <row r="236" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A236" s="1" t="s">
-        <v>502</v>
+        <v>403</v>
       </c>
       <c r="B236" s="2" t="s">
-        <v>503</v>
+        <v>414</v>
       </c>
       <c r="C236" s="1" t="s">
-        <v>502</v>
+        <v>403</v>
       </c>
     </row>
     <row r="237" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A237" s="2" t="s">
-        <v>279</v>
+        <v>269</v>
       </c>
       <c r="B237" s="2" t="s">
-        <v>280</v>
+        <v>270</v>
       </c>
       <c r="C237" s="3" t="s">
-        <v>279</v>
+        <v>269</v>
       </c>
     </row>
     <row r="238" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A238" s="2" t="s">
-        <v>5</v>
+        <v>271</v>
       </c>
       <c r="B238" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C238" s="3" t="s">
-        <v>5</v>
+        <v>272</v>
+      </c>
+      <c r="C238" s="2" t="s">
+        <v>271</v>
       </c>
     </row>
     <row r="239" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A239" s="2" t="s">
-        <v>281</v>
+        <v>273</v>
       </c>
       <c r="B239" s="2" t="s">
-        <v>282</v>
-      </c>
-      <c r="C239" s="2" t="s">
-        <v>281</v>
+        <v>274</v>
+      </c>
+      <c r="C239" s="3" t="s">
+        <v>273</v>
       </c>
     </row>
     <row r="240" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A240" s="2" t="s">
-        <v>283</v>
+        <v>9</v>
       </c>
       <c r="B240" s="2" t="s">
-        <v>284</v>
+        <v>10</v>
       </c>
       <c r="C240" s="3" t="s">
-        <v>283</v>
+        <v>9</v>
       </c>
     </row>
     <row r="241" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A241" s="2" t="s">
-        <v>285</v>
+        <v>506</v>
       </c>
       <c r="B241" s="2" t="s">
-        <v>284</v>
-      </c>
-      <c r="C241" s="3" t="s">
-        <v>285</v>
+        <v>1</v>
+      </c>
+      <c r="C241" s="2" t="s">
+        <v>506</v>
       </c>
     </row>
     <row r="242" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A242" s="2" t="s">
-        <v>286</v>
+        <v>275</v>
       </c>
       <c r="B242" s="2" t="s">
-        <v>287</v>
+        <v>276</v>
       </c>
       <c r="C242" s="3" t="s">
-        <v>286</v>
+        <v>275</v>
       </c>
     </row>
     <row r="243" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A243" s="2" t="s">
-        <v>288</v>
+      <c r="A243" s="1" t="s">
+        <v>473</v>
       </c>
       <c r="B243" s="2" t="s">
-        <v>289</v>
-      </c>
-      <c r="C243" s="3" t="s">
-        <v>288</v>
+        <v>484</v>
+      </c>
+      <c r="C243" s="1" t="s">
+        <v>473</v>
       </c>
     </row>
     <row r="244" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A244" s="2" t="s">
-        <v>290</v>
+        <v>378</v>
       </c>
       <c r="B244" s="2" t="s">
-        <v>291</v>
-      </c>
-      <c r="C244" s="3" t="s">
-        <v>290</v>
+        <v>379</v>
+      </c>
+      <c r="C244" s="2" t="s">
+        <v>378</v>
       </c>
     </row>
     <row r="245" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A245" s="2" t="s">
-        <v>292</v>
+        <v>277</v>
       </c>
       <c r="B245" s="2" t="s">
-        <v>293</v>
+        <v>278</v>
       </c>
       <c r="C245" s="3" t="s">
-        <v>292</v>
+        <v>277</v>
       </c>
     </row>
     <row r="246" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A246" s="2" t="s">
-        <v>294</v>
+      <c r="A246" s="1" t="s">
+        <v>478</v>
       </c>
       <c r="B246" s="2" t="s">
-        <v>295</v>
-      </c>
-      <c r="C246" s="3" t="s">
-        <v>294</v>
+        <v>490</v>
+      </c>
+      <c r="C246" s="1" t="s">
+        <v>478</v>
       </c>
     </row>
     <row r="247" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A247" s="2" t="s">
-        <v>296</v>
+      <c r="A247" s="1" t="s">
+        <v>502</v>
       </c>
       <c r="B247" s="2" t="s">
-        <v>297</v>
-      </c>
-      <c r="C247" s="3" t="s">
-        <v>296</v>
+        <v>503</v>
+      </c>
+      <c r="C247" s="1" t="s">
+        <v>502</v>
       </c>
     </row>
     <row r="248" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A248" s="2" t="s">
-        <v>298</v>
+        <v>279</v>
       </c>
       <c r="B248" s="2" t="s">
-        <v>299</v>
-      </c>
-      <c r="C248" s="2" t="s">
-        <v>298</v>
+        <v>280</v>
+      </c>
+      <c r="C248" s="3" t="s">
+        <v>279</v>
       </c>
     </row>
     <row r="249" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A249" s="1" t="s">
-        <v>551</v>
-      </c>
-      <c r="B249" s="1" t="s">
-        <v>550</v>
-      </c>
-      <c r="C249" s="1" t="s">
-        <v>551</v>
+      <c r="A249" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B249" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C249" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="250" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A250" s="1" t="s">
-        <v>409</v>
+      <c r="A250" s="2" t="s">
+        <v>281</v>
       </c>
       <c r="B250" s="2" t="s">
-        <v>418</v>
-      </c>
-      <c r="C250" s="1" t="s">
-        <v>409</v>
+        <v>282</v>
+      </c>
+      <c r="C250" s="2" t="s">
+        <v>281</v>
       </c>
     </row>
     <row r="251" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A251" s="2" t="s">
-        <v>300</v>
+        <v>283</v>
       </c>
       <c r="B251" s="2" t="s">
-        <v>301</v>
+        <v>284</v>
       </c>
       <c r="C251" s="3" t="s">
-        <v>300</v>
+        <v>283</v>
       </c>
     </row>
     <row r="252" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A252" s="1" t="s">
-        <v>472</v>
+      <c r="A252" s="2" t="s">
+        <v>285</v>
       </c>
       <c r="B252" s="2" t="s">
-        <v>483</v>
-      </c>
-      <c r="C252" s="1" t="s">
-        <v>472</v>
+        <v>284</v>
+      </c>
+      <c r="C252" s="3" t="s">
+        <v>285</v>
       </c>
     </row>
     <row r="253" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A253" s="2" t="s">
-        <v>302</v>
+        <v>286</v>
       </c>
       <c r="B253" s="2" t="s">
-        <v>303</v>
+        <v>287</v>
       </c>
       <c r="C253" s="3" t="s">
-        <v>302</v>
+        <v>286</v>
       </c>
     </row>
     <row r="254" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A254" s="1" t="s">
-        <v>470</v>
+      <c r="A254" s="2" t="s">
+        <v>288</v>
       </c>
       <c r="B254" s="2" t="s">
-        <v>486</v>
-      </c>
-      <c r="C254" s="1" t="s">
-        <v>470</v>
+        <v>289</v>
+      </c>
+      <c r="C254" s="3" t="s">
+        <v>288</v>
       </c>
     </row>
     <row r="255" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A255" s="1" t="s">
-        <v>413</v>
-      </c>
-      <c r="B255" s="1" t="s">
-        <v>420</v>
-      </c>
-      <c r="C255" s="1" t="s">
-        <v>413</v>
+      <c r="A255" s="2" t="s">
+        <v>290</v>
+      </c>
+      <c r="B255" s="2" t="s">
+        <v>291</v>
+      </c>
+      <c r="C255" s="3" t="s">
+        <v>290</v>
       </c>
     </row>
     <row r="256" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A256" s="1" t="s">
-        <v>474</v>
+      <c r="A256" s="2" t="s">
+        <v>292</v>
       </c>
       <c r="B256" s="2" t="s">
-        <v>485</v>
-      </c>
-      <c r="C256" s="1" t="s">
-        <v>474</v>
+        <v>293</v>
+      </c>
+      <c r="C256" s="3" t="s">
+        <v>292</v>
       </c>
     </row>
     <row r="257" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A257" s="1" t="s">
-        <v>534</v>
+      <c r="A257" s="2" t="s">
+        <v>294</v>
       </c>
       <c r="B257" s="2" t="s">
-        <v>549</v>
-      </c>
-      <c r="C257" s="1" t="s">
-        <v>534</v>
+        <v>295</v>
+      </c>
+      <c r="C257" s="3" t="s">
+        <v>294</v>
       </c>
     </row>
     <row r="258" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A258" s="2" t="s">
-        <v>304</v>
+        <v>296</v>
       </c>
       <c r="B258" s="2" t="s">
-        <v>305</v>
+        <v>297</v>
       </c>
       <c r="C258" s="3" t="s">
-        <v>304</v>
+        <v>296</v>
       </c>
     </row>
     <row r="259" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A259" s="1" t="s">
-        <v>492</v>
+      <c r="A259" s="2" t="s">
+        <v>298</v>
       </c>
       <c r="B259" s="2" t="s">
-        <v>493</v>
-      </c>
-      <c r="C259" s="1" t="s">
-        <v>492</v>
+        <v>299</v>
+      </c>
+      <c r="C259" s="2" t="s">
+        <v>298</v>
       </c>
     </row>
     <row r="260" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A260" s="2" t="s">
-        <v>306</v>
-      </c>
-      <c r="B260" s="2" t="s">
-        <v>307</v>
-      </c>
-      <c r="C260" s="3" t="s">
-        <v>306</v>
+      <c r="A260" s="1" t="s">
+        <v>551</v>
+      </c>
+      <c r="B260" s="1" t="s">
+        <v>550</v>
+      </c>
+      <c r="C260" s="1" t="s">
+        <v>551</v>
       </c>
     </row>
     <row r="261" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A261" s="2" t="s">
-        <v>308</v>
+      <c r="A261" s="1" t="s">
+        <v>409</v>
       </c>
       <c r="B261" s="2" t="s">
-        <v>309</v>
-      </c>
-      <c r="C261" s="3" t="s">
-        <v>308</v>
+        <v>418</v>
+      </c>
+      <c r="C261" s="1" t="s">
+        <v>409</v>
       </c>
     </row>
     <row r="262" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A262" s="2" t="s">
-        <v>310</v>
+        <v>300</v>
       </c>
       <c r="B262" s="2" t="s">
-        <v>311</v>
+        <v>301</v>
       </c>
       <c r="C262" s="3" t="s">
-        <v>310</v>
+        <v>300</v>
       </c>
     </row>
     <row r="263" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A263" s="1" t="s">
-        <v>408</v>
+        <v>472</v>
       </c>
       <c r="B263" s="2" t="s">
-        <v>423</v>
+        <v>483</v>
       </c>
       <c r="C263" s="1" t="s">
-        <v>408</v>
+        <v>472</v>
       </c>
     </row>
     <row r="264" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A264" s="2" t="s">
-        <v>364</v>
+        <v>302</v>
       </c>
       <c r="B264" s="2" t="s">
-        <v>365</v>
-      </c>
-      <c r="C264" s="2" t="s">
-        <v>364</v>
+        <v>303</v>
+      </c>
+      <c r="C264" s="3" t="s">
+        <v>302</v>
       </c>
     </row>
     <row r="265" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A265" s="2" t="s">
-        <v>370</v>
+      <c r="A265" s="1" t="s">
+        <v>470</v>
       </c>
       <c r="B265" s="2" t="s">
-        <v>371</v>
-      </c>
-      <c r="C265" s="2" t="s">
-        <v>370</v>
+        <v>486</v>
+      </c>
+      <c r="C265" s="1" t="s">
+        <v>470</v>
       </c>
     </row>
     <row r="266" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A266" s="2" t="s">
-        <v>312</v>
-      </c>
-      <c r="B266" s="2" t="s">
-        <v>313</v>
-      </c>
-      <c r="C266" s="3" t="s">
-        <v>312</v>
+      <c r="A266" s="1" t="s">
+        <v>413</v>
+      </c>
+      <c r="B266" s="1" t="s">
+        <v>420</v>
+      </c>
+      <c r="C266" s="1" t="s">
+        <v>413</v>
       </c>
     </row>
     <row r="267" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A267" s="2" t="s">
-        <v>11</v>
+      <c r="A267" s="1" t="s">
+        <v>474</v>
       </c>
       <c r="B267" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C267" s="3" t="s">
-        <v>11</v>
+        <v>485</v>
+      </c>
+      <c r="C267" s="1" t="s">
+        <v>474</v>
       </c>
     </row>
     <row r="268" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A268" s="2" t="s">
-        <v>314</v>
+      <c r="A268" s="1" t="s">
+        <v>534</v>
       </c>
       <c r="B268" s="2" t="s">
-        <v>315</v>
-      </c>
-      <c r="C268" s="2" t="s">
-        <v>314</v>
+        <v>549</v>
+      </c>
+      <c r="C268" s="1" t="s">
+        <v>534</v>
       </c>
     </row>
     <row r="269" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A269" s="2" t="s">
-        <v>316</v>
+        <v>304</v>
       </c>
       <c r="B269" s="2" t="s">
-        <v>317</v>
+        <v>305</v>
       </c>
       <c r="C269" s="3" t="s">
-        <v>316</v>
+        <v>304</v>
       </c>
     </row>
     <row r="270" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A270" s="2" t="s">
-        <v>318</v>
+      <c r="A270" s="1" t="s">
+        <v>492</v>
       </c>
       <c r="B270" s="2" t="s">
-        <v>319</v>
-      </c>
-      <c r="C270" s="3" t="s">
-        <v>318</v>
+        <v>493</v>
+      </c>
+      <c r="C270" s="1" t="s">
+        <v>492</v>
       </c>
     </row>
     <row r="271" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A271" s="2" t="s">
-        <v>320</v>
+        <v>306</v>
       </c>
       <c r="B271" s="2" t="s">
-        <v>321</v>
-      </c>
-      <c r="C271" s="2" t="s">
-        <v>320</v>
+        <v>307</v>
+      </c>
+      <c r="C271" s="3" t="s">
+        <v>306</v>
       </c>
     </row>
     <row r="272" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A272" s="1" t="s">
-        <v>445</v>
-      </c>
-      <c r="B272" s="1" t="s">
-        <v>447</v>
-      </c>
-      <c r="C272" s="1" t="s">
-        <v>445</v>
+      <c r="A272" s="2" t="s">
+        <v>308</v>
+      </c>
+      <c r="B272" s="2" t="s">
+        <v>309</v>
+      </c>
+      <c r="C272" s="3" t="s">
+        <v>308</v>
       </c>
     </row>
     <row r="273" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A273" s="2" t="s">
-        <v>322</v>
+        <v>310</v>
       </c>
       <c r="B273" s="2" t="s">
-        <v>323</v>
+        <v>311</v>
       </c>
       <c r="C273" s="3" t="s">
-        <v>322</v>
+        <v>310</v>
       </c>
     </row>
     <row r="274" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A274" s="2" t="s">
-        <v>324</v>
+      <c r="A274" s="1" t="s">
+        <v>408</v>
       </c>
       <c r="B274" s="2" t="s">
-        <v>325</v>
-      </c>
-      <c r="C274" s="2" t="s">
-        <v>324</v>
+        <v>423</v>
+      </c>
+      <c r="C274" s="1" t="s">
+        <v>408</v>
       </c>
     </row>
     <row r="275" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A275" s="2" t="s">
-        <v>326</v>
+        <v>364</v>
       </c>
       <c r="B275" s="2" t="s">
-        <v>327</v>
+        <v>365</v>
       </c>
       <c r="C275" s="2" t="s">
-        <v>326</v>
+        <v>364</v>
       </c>
     </row>
     <row r="276" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A276" s="2" t="s">
-        <v>328</v>
+        <v>370</v>
       </c>
       <c r="B276" s="2" t="s">
-        <v>329</v>
-      </c>
-      <c r="C276" s="3" t="s">
-        <v>328</v>
+        <v>371</v>
+      </c>
+      <c r="C276" s="2" t="s">
+        <v>370</v>
       </c>
     </row>
     <row r="277" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A277" s="2" t="s">
-        <v>425</v>
+        <v>312</v>
       </c>
       <c r="B277" s="2" t="s">
-        <v>428</v>
-      </c>
-      <c r="C277" s="2" t="s">
-        <v>425</v>
+        <v>313</v>
+      </c>
+      <c r="C277" s="3" t="s">
+        <v>312</v>
       </c>
     </row>
     <row r="278" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A278" s="2" t="s">
-        <v>330</v>
+        <v>11</v>
       </c>
       <c r="B278" s="2" t="s">
-        <v>331</v>
-      </c>
-      <c r="C278" s="2" t="s">
-        <v>330</v>
+        <v>12</v>
+      </c>
+      <c r="C278" s="3" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="279" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A279" s="1" t="s">
-        <v>509</v>
+        <v>565</v>
       </c>
       <c r="B279" s="2" t="s">
-        <v>516</v>
+        <v>589</v>
       </c>
       <c r="C279" s="1" t="s">
-        <v>509</v>
+        <v>565</v>
       </c>
     </row>
     <row r="280" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A280" s="1" t="s">
-        <v>511</v>
+        <v>564</v>
       </c>
       <c r="B280" s="2" t="s">
-        <v>518</v>
+        <v>588</v>
       </c>
       <c r="C280" s="1" t="s">
-        <v>511</v>
+        <v>564</v>
       </c>
     </row>
     <row r="281" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A281" s="1" t="s">
-        <v>510</v>
-      </c>
-      <c r="B281" s="2" t="s">
-        <v>517</v>
+        <v>574</v>
+      </c>
+      <c r="B281" s="1" t="s">
+        <v>581</v>
       </c>
       <c r="C281" s="1" t="s">
-        <v>510</v>
+        <v>574</v>
       </c>
     </row>
     <row r="282" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A282" s="2" t="s">
-        <v>554</v>
+        <v>314</v>
       </c>
       <c r="B282" s="2" t="s">
-        <v>555</v>
-      </c>
-      <c r="C282" s="3" t="s">
-        <v>554</v>
+        <v>315</v>
+      </c>
+      <c r="C282" s="2" t="s">
+        <v>314</v>
       </c>
     </row>
     <row r="283" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A283" s="2" t="s">
-        <v>332</v>
+        <v>316</v>
       </c>
       <c r="B283" s="2" t="s">
-        <v>333</v>
+        <v>317</v>
       </c>
       <c r="C283" s="3" t="s">
-        <v>332</v>
+        <v>316</v>
       </c>
     </row>
     <row r="284" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A284" s="2" t="s">
-        <v>334</v>
+        <v>318</v>
       </c>
       <c r="B284" s="2" t="s">
-        <v>335</v>
+        <v>319</v>
       </c>
       <c r="C284" s="3" t="s">
-        <v>334</v>
+        <v>318</v>
       </c>
     </row>
     <row r="285" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A285" s="2" t="s">
-        <v>366</v>
+        <v>320</v>
       </c>
       <c r="B285" s="2" t="s">
-        <v>367</v>
+        <v>321</v>
       </c>
       <c r="C285" s="2" t="s">
-        <v>366</v>
+        <v>320</v>
       </c>
     </row>
     <row r="286" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A286" s="1" t="s">
-        <v>540</v>
+        <v>445</v>
       </c>
       <c r="B286" s="1" t="s">
-        <v>552</v>
+        <v>447</v>
       </c>
       <c r="C286" s="1" t="s">
-        <v>540</v>
+        <v>445</v>
       </c>
     </row>
     <row r="287" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A287" s="2" t="s">
+        <v>322</v>
+      </c>
+      <c r="B287" s="2" t="s">
+        <v>323</v>
+      </c>
+      <c r="C287" s="3" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="288" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A288" s="2" t="s">
+        <v>324</v>
+      </c>
+      <c r="B288" s="2" t="s">
+        <v>325</v>
+      </c>
+      <c r="C288" s="2" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="289" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A289" s="2" t="s">
+        <v>326</v>
+      </c>
+      <c r="B289" s="2" t="s">
+        <v>327</v>
+      </c>
+      <c r="C289" s="2" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="290" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A290" s="2" t="s">
+        <v>328</v>
+      </c>
+      <c r="B290" s="2" t="s">
+        <v>329</v>
+      </c>
+      <c r="C290" s="3" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="291" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A291" s="2" t="s">
+        <v>425</v>
+      </c>
+      <c r="B291" s="2" t="s">
+        <v>428</v>
+      </c>
+      <c r="C291" s="2" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="292" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A292" s="2" t="s">
+        <v>330</v>
+      </c>
+      <c r="B292" s="2" t="s">
+        <v>331</v>
+      </c>
+      <c r="C292" s="2" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="293" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A293" s="1" t="s">
+        <v>572</v>
+      </c>
+      <c r="B293" s="1" t="s">
+        <v>583</v>
+      </c>
+      <c r="C293" s="1" t="s">
+        <v>572</v>
+      </c>
+    </row>
+    <row r="294" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A294" s="1" t="s">
+        <v>509</v>
+      </c>
+      <c r="B294" s="2" t="s">
+        <v>516</v>
+      </c>
+      <c r="C294" s="1" t="s">
+        <v>509</v>
+      </c>
+    </row>
+    <row r="295" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A295" s="1" t="s">
+        <v>511</v>
+      </c>
+      <c r="B295" s="2" t="s">
+        <v>518</v>
+      </c>
+      <c r="C295" s="1" t="s">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="296" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A296" s="1" t="s">
+        <v>510</v>
+      </c>
+      <c r="B296" s="2" t="s">
+        <v>517</v>
+      </c>
+      <c r="C296" s="1" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="297" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A297" s="2" t="s">
+        <v>554</v>
+      </c>
+      <c r="B297" s="2" t="s">
+        <v>555</v>
+      </c>
+      <c r="C297" s="3" t="s">
+        <v>554</v>
+      </c>
+    </row>
+    <row r="298" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A298" s="2" t="s">
+        <v>332</v>
+      </c>
+      <c r="B298" s="2" t="s">
+        <v>333</v>
+      </c>
+      <c r="C298" s="3" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="299" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A299" s="2" t="s">
+        <v>334</v>
+      </c>
+      <c r="B299" s="2" t="s">
+        <v>335</v>
+      </c>
+      <c r="C299" s="3" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="300" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A300" s="2" t="s">
+        <v>366</v>
+      </c>
+      <c r="B300" s="2" t="s">
+        <v>367</v>
+      </c>
+      <c r="C300" s="2" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="301" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A301" s="1" t="s">
+        <v>540</v>
+      </c>
+      <c r="B301" s="1" t="s">
+        <v>552</v>
+      </c>
+      <c r="C301" s="1" t="s">
+        <v>540</v>
+      </c>
+    </row>
+    <row r="302" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A302" s="2" t="s">
         <v>342</v>
       </c>
-      <c r="B287" s="2" t="s">
+      <c r="B302" s="2" t="s">
         <v>343</v>
       </c>
-      <c r="C287" s="3" t="s">
+      <c r="C302" s="3" t="s">
         <v>342</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:C1" xr:uid="{56EE5BC3-7B0A-4577-92C7-56F73F7DDC8B}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C287">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C302">
       <sortCondition ref="A1"/>
     </sortState>
   </autoFilter>

</xml_diff>

<commit_message>
Removed renv, mode fix, by_group fix, package update, sidebar update
</commit_message>
<xml_diff>
--- a/translations/source.xlsx
+++ b/translations/source.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/e6c7874704bc5dfb/Documents/R Studio/DataSuite/translations/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="300" documentId="8_{D77EC384-F39F-4BA6-8963-4B8AF986F7DE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{602C5BE0-599F-4AB8-8383-B39F0D99F1B3}"/>
+  <xr:revisionPtr revIDLastSave="303" documentId="8_{D77EC384-F39F-4BA6-8963-4B8AF986F7DE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{3A1A4535-44B3-4F32-9E24-3F2FA57285C6}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="16395" xr2:uid="{BD840C99-A56D-4EBC-B1B7-A6018ADC22A6}"/>
+    <workbookView xWindow="8145" yWindow="270" windowWidth="15345" windowHeight="15930" xr2:uid="{BD840C99-A56D-4EBC-B1B7-A6018ADC22A6}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -243,12 +243,6 @@
     <t>NbClust::NbClust conclusions:</t>
   </si>
   <si>
-    <t>Выводы psycho::n_factors:</t>
-  </si>
-  <si>
-    <t>psycho::n_factors conclusions:</t>
-  </si>
-  <si>
     <t>График нагрузок</t>
   </si>
   <si>
@@ -1810,6 +1804,12 @@
   </si>
   <si>
     <t>(different sample sizes)</t>
+  </si>
+  <si>
+    <t>Выводы parameters::n_factors:</t>
+  </si>
+  <si>
+    <t>parameters::n_factors conclusions:</t>
   </si>
 </sst>
 </file>
@@ -2169,8 +2169,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C853ECA4-158B-4D85-A448-9ECE56776B5F}">
   <dimension ref="A1:C302"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+    <sheetView tabSelected="1" topLeftCell="B34" workbookViewId="0">
+      <selection activeCell="B41" sqref="B41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -2194,24 +2194,24 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A2" s="1" t="s">
-        <v>569</v>
+        <v>567</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>590</v>
+        <v>588</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>569</v>
+        <v>567</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A3" s="1" t="s">
-        <v>570</v>
+        <v>568</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>591</v>
+        <v>589</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>570</v>
+        <v>568</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.45">
@@ -2227,13 +2227,13 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A5" s="2" t="s">
-        <v>526</v>
+        <v>524</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>527</v>
+        <v>525</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>526</v>
+        <v>524</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.45">
@@ -2271,13 +2271,13 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A9" s="1" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>17</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.45">
@@ -2293,13 +2293,13 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A11" s="1" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>19</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.45">
@@ -2315,35 +2315,35 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A13" s="2" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A14" s="2" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A15" s="2" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.45">
@@ -2458,35 +2458,35 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A26" s="2" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A27" s="1" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A28" s="2" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.45">
@@ -2516,7 +2516,7 @@
         <v>40</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="C31" s="3" t="s">
         <v>40</v>
@@ -2524,13 +2524,13 @@
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A32" s="1" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>578</v>
+        <v>576</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.45">
@@ -2557,57 +2557,57 @@
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A35" s="1" t="s">
-        <v>541</v>
+        <v>539</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>541</v>
+        <v>539</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A36" s="1" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>520</v>
+        <v>518</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A37" s="1" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>521</v>
+        <v>519</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A38" s="2" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A39" s="1" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.45">
@@ -2623,13 +2623,13 @@
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A41" s="2" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>505</v>
+        <v>503</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.45">
@@ -2656,24 +2656,24 @@
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A44" s="2" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A45" s="2" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.45">
@@ -2689,46 +2689,46 @@
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A47" s="1" t="s">
+        <v>575</v>
+      </c>
+      <c r="B47" s="1" t="s">
         <v>577</v>
       </c>
-      <c r="B47" s="1" t="s">
-        <v>579</v>
-      </c>
       <c r="C47" s="1" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A48" s="2" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A49" s="2" t="s">
+        <v>557</v>
+      </c>
+      <c r="B49" s="2" t="s">
         <v>559</v>
       </c>
-      <c r="B49" s="2" t="s">
-        <v>561</v>
-      </c>
       <c r="C49" s="2" t="s">
-        <v>559</v>
+        <v>557</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A50" s="1" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.45">
@@ -2744,13 +2744,13 @@
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A52" s="2" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="C52" s="3" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.45">
@@ -2766,13 +2766,13 @@
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A54" s="1" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.45">
@@ -2821,13 +2821,13 @@
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A59" s="1" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.45">
@@ -2854,1960 +2854,1960 @@
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A62" s="2" t="s">
-        <v>69</v>
+        <v>590</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="C62" s="3" t="s">
-        <v>69</v>
+        <v>591</v>
+      </c>
+      <c r="C62" s="2" t="s">
+        <v>590</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A63" s="2" t="s">
+        <v>463</v>
+      </c>
+      <c r="B63" s="2" t="s">
         <v>465</v>
       </c>
-      <c r="B63" s="2" t="s">
-        <v>467</v>
-      </c>
       <c r="C63" s="2" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A64" s="2" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="C64" s="3" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A65" s="2" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A66" s="1" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A67" s="2" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C67" s="3" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A68" s="2" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C68" s="3" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A69" s="2" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C69" s="3" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A70" s="2" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C70" s="3" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A71" s="2" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C71" s="3" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A72" s="2" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C72" s="3" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A73" s="2" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A74" s="2" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C74" s="3" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A75" s="2" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C75" s="3" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A76" s="2" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C76" s="3" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A77" s="1" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A78" s="1" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A79" s="2" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C79" s="2" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A80" s="1" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>585</v>
+        <v>583</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A81" s="2" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="C81" s="2" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A82" s="2" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C82" s="3" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A83" s="2" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B83" s="2" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="C83" s="3" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A84" s="2" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B84" s="2" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C84" s="3" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A85" s="1" t="s">
-        <v>535</v>
+        <v>533</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>546</v>
+        <v>544</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>535</v>
+        <v>533</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A86" s="1" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>547</v>
+        <v>545</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A87" s="2" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B87" s="2" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C87" s="3" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A88" s="2" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B88" s="2" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C88" s="3" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A89" s="2" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B89" s="2" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C89" s="3" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A90" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B90" s="2" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C90" s="3" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A91" s="2" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B91" s="2" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C91" s="3" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A92" s="2" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="B92" s="2" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="C92" s="2" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A93" s="2" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B93" s="2" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C93" s="3" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A94" s="2" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B94" s="2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C94" s="2" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A95" s="2" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B95" s="2" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C95" s="2" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A96" s="2" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B96" s="2" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C96" s="2" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A97" s="1" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="B97" s="2" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="C97" s="1" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A98" s="2" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B98" s="2" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C98" s="2" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A99" s="2" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="B99" s="2" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
       <c r="C99" s="3" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A100" s="2" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B100" s="2" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C100" s="3" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A101" s="2" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B101" s="2" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C101" s="3" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A102" s="2" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B102" s="2" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C102" s="3" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A103" s="2" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B103" s="2" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C103" s="3" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A104" s="2" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B104" s="2" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C104" s="2" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A105" s="1" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
       <c r="B105" s="1" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="C105" s="1" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A106" s="1" t="s">
-        <v>539</v>
+        <v>537</v>
       </c>
       <c r="B106" s="1" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="C106" s="1" t="s">
-        <v>539</v>
+        <v>537</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A107" s="2" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="B107" s="2" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="C107" s="2" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A108" s="2" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B108" s="2" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="C108" s="2" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A109" s="2" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="B109" s="2" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="C109" s="2" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A110" s="2" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B110" s="2" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="C110" s="3" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A111" s="2" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B111" s="2" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C111" s="3" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A112" s="2" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B112" s="2" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C112" s="2" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A113" s="2" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B113" s="2" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C113" s="3" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A114" s="1" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="B114" s="2" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="C114" s="1" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A115" s="2" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B115" s="2" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="C115" s="3" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A116" s="2" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B116" s="2" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C116" s="3" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A117" s="2" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B117" s="2" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="C117" s="3" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A118" s="2" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B118" s="2" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C118" s="3" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A119" s="2" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="B119" s="2" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C119" s="3" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A120" s="2" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B120" s="2" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="C120" s="3" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A121" s="2" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B121" s="2" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="C121" s="3" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A122" s="2" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B122" s="2" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="C122" s="2" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A123" s="2" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="B123" s="2" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="C123" s="2" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A124" s="2" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B124" s="2" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C124" s="2" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A125" s="2" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="B125" s="2" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
       <c r="C125" s="3" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A126" s="2" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="B126" s="2" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="C126" s="3" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A127" s="1" t="s">
-        <v>536</v>
+        <v>534</v>
       </c>
       <c r="B127" s="1" t="s">
-        <v>548</v>
+        <v>546</v>
       </c>
       <c r="C127" s="1" t="s">
-        <v>536</v>
+        <v>534</v>
       </c>
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A128" s="1" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="B128" s="1" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="C128" s="1" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A129" s="2" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B129" s="2" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="C129" s="3" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A130" s="1" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="B130" s="2" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
       <c r="C130" s="1" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A131" s="1" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="B131" s="2" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="C131" s="1" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A132" s="1" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
       <c r="B132" s="2" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
       <c r="C132" s="1" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A133" s="2" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="B133" s="2" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C133" s="2" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A134" s="2" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="B134" s="2" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="C134" s="3" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A135" s="1" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
       <c r="B135" s="2" t="s">
-        <v>544</v>
+        <v>542</v>
       </c>
       <c r="C135" s="1" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A136" s="2" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="B136" s="2" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="C136" s="3" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A137" s="2" t="s">
-        <v>524</v>
+        <v>522</v>
       </c>
       <c r="B137" s="2" t="s">
-        <v>525</v>
+        <v>523</v>
       </c>
       <c r="C137" s="2" t="s">
-        <v>524</v>
+        <v>522</v>
       </c>
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A138" s="2" t="s">
-        <v>523</v>
+        <v>521</v>
       </c>
       <c r="B138" s="2" t="s">
-        <v>562</v>
+        <v>560</v>
       </c>
       <c r="C138" s="2" t="s">
-        <v>523</v>
+        <v>521</v>
       </c>
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A139" s="1" t="s">
-        <v>566</v>
+        <v>564</v>
       </c>
       <c r="B139" s="1" t="s">
-        <v>587</v>
+        <v>585</v>
       </c>
       <c r="C139" s="1" t="s">
-        <v>566</v>
+        <v>564</v>
       </c>
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A140" s="2" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="B140" s="2" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C140" s="3" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="141" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A141" s="2" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="B141" s="2" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="C141" s="3" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A142" s="2" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="B142" s="2" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="C142" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="143" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A143" s="2" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B143" s="2" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="C143" s="3" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
     </row>
     <row r="144" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A144" s="2" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B144" s="2" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="C144" s="3" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
     </row>
     <row r="145" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A145" s="2" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B145" s="2" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="C145" s="3" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A146" s="1" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
       <c r="B146" s="2" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
       <c r="C146" s="1" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
     </row>
     <row r="147" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A147" s="2" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B147" s="2" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="C147" s="3" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="148" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A148" s="1" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="B148" s="2" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="C148" s="1" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
     </row>
     <row r="149" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A149" s="2" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="B149" s="2" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="C149" s="3" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
     </row>
     <row r="150" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A150" s="2" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="B150" s="2" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="C150" s="2" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="151" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A151" s="2" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="B151" s="2" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="C151" s="2" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
     </row>
     <row r="152" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A152" s="1" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="B152" s="2" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
       <c r="C152" s="1" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
     </row>
     <row r="153" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A153" s="2" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="B153" s="2" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="C153" s="3" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="154" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A154" s="2" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="B154" s="2" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="C154" s="3" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
     <row r="155" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A155" s="2" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="B155" s="2" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="C155" s="3" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="156" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A156" s="2" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="B156" s="2" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="C156" s="3" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
     </row>
     <row r="157" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A157" s="2" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="B157" s="2" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="C157" s="3" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
     </row>
     <row r="158" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A158" s="2" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="B158" s="2" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="C158" s="3" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
     </row>
     <row r="159" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A159" s="2" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="B159" s="2" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="C159" s="2" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
     </row>
     <row r="160" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A160" s="2" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="B160" s="2" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="C160" s="3" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
     </row>
     <row r="161" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A161" s="2" t="s">
+        <v>526</v>
+      </c>
+      <c r="B161" s="2" t="s">
         <v>528</v>
       </c>
-      <c r="B161" s="2" t="s">
-        <v>530</v>
-      </c>
       <c r="C161" s="2" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
     </row>
     <row r="162" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A162" s="1" t="s">
-        <v>575</v>
+        <v>573</v>
       </c>
       <c r="B162" s="1" t="s">
-        <v>578</v>
+        <v>576</v>
       </c>
       <c r="C162" s="1" t="s">
-        <v>575</v>
+        <v>573</v>
       </c>
     </row>
     <row r="163" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A163" s="2" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="B163" s="2" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="C163" s="3" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="164" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A164" s="1" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="B164" s="1" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="C164" s="1" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
     </row>
     <row r="165" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A165" s="2" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="B165" s="2" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="C165" s="3" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
     </row>
     <row r="166" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A166" s="2" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="B166" s="2" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="C166" s="3" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
     </row>
     <row r="167" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A167" s="2" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="B167" s="2" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="C167" s="3" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
     </row>
     <row r="168" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A168" s="2" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="B168" s="2" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="C168" s="3" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
     </row>
     <row r="169" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A169" s="2" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="B169" s="2" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C169" s="3" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
     </row>
     <row r="170" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A170" s="1" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="B170" s="2" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="C170" s="1" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
     </row>
     <row r="171" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A171" s="2" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="B171" s="2" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="C171" s="3" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
     </row>
     <row r="172" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A172" s="2" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="B172" s="2" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="C172" s="3" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
     <row r="173" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A173" s="2" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="B173" s="2" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="C173" s="3" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
     </row>
     <row r="174" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A174" s="2" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="B174" s="2" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="C174" s="3" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
     </row>
     <row r="175" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A175" s="2" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="B175" s="2" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="C175" s="3" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
     </row>
     <row r="176" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A176" s="2" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="B176" s="2" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="C176" s="3" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
     </row>
     <row r="177" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A177" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="B177" s="2" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="C177" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
     </row>
     <row r="178" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A178" s="2" t="s">
+        <v>527</v>
+      </c>
+      <c r="B178" s="2" t="s">
         <v>529</v>
       </c>
-      <c r="B178" s="2" t="s">
-        <v>531</v>
-      </c>
       <c r="C178" s="2" t="s">
-        <v>529</v>
+        <v>527</v>
       </c>
     </row>
     <row r="179" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A179" s="2" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="B179" s="2" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="C179" s="3" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
     </row>
     <row r="180" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A180" s="2" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="B180" s="2" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="C180" s="2" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
     </row>
     <row r="181" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A181" s="2" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="B181" s="2" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="C181" s="3" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
     </row>
     <row r="182" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A182" s="2" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="B182" s="2" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="C182" s="3" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="183" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A183" s="2" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="B183" s="2" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="C183" s="2" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
     </row>
     <row r="184" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A184" s="2" t="s">
+        <v>556</v>
+      </c>
+      <c r="B184" s="2" t="s">
         <v>558</v>
       </c>
-      <c r="B184" s="2" t="s">
-        <v>560</v>
-      </c>
       <c r="C184" s="2" t="s">
-        <v>558</v>
+        <v>556</v>
       </c>
     </row>
     <row r="185" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A185" s="1" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="B185" s="1" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="C185" s="1" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
     </row>
     <row r="186" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A186" s="2" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="B186" s="2" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="C186" s="3" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
     </row>
     <row r="187" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A187" s="2" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="B187" s="2" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C187" s="3" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="188" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A188" s="2" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="B188" s="2" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="C188" s="3" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="189" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A189" s="2" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="B189" s="2" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="C189" s="2" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="190" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A190" s="1" t="s">
+        <v>442</v>
+      </c>
+      <c r="B190" s="1" t="s">
         <v>444</v>
       </c>
-      <c r="B190" s="1" t="s">
-        <v>446</v>
-      </c>
       <c r="C190" s="1" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
     </row>
     <row r="191" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A191" s="2" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="B191" s="2" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="C191" s="2" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
     </row>
     <row r="192" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A192" s="1" t="s">
-        <v>573</v>
+        <v>571</v>
       </c>
       <c r="B192" s="1" t="s">
-        <v>582</v>
+        <v>580</v>
       </c>
       <c r="C192" s="1" t="s">
-        <v>573</v>
+        <v>571</v>
       </c>
     </row>
     <row r="193" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A193" s="2" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="B193" s="2" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="C193" s="3" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
     </row>
     <row r="194" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A194" s="2" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="B194" s="2" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="C194" s="3" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
     </row>
     <row r="195" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A195" s="1" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="B195" s="2" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="C195" s="1" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
     </row>
     <row r="196" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A196" s="2" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="B196" s="2" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="C196" s="2" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
     </row>
     <row r="197" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A197" s="1" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="B197" s="2" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
       <c r="C197" s="1" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
     </row>
     <row r="198" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A198" s="2" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="B198" s="2" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="C198" s="2" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
     </row>
     <row r="199" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A199" s="2" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="B199" s="2" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="C199" s="3" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
     </row>
     <row r="200" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A200" s="1" t="s">
-        <v>571</v>
+        <v>569</v>
       </c>
       <c r="B200" s="1" t="s">
-        <v>584</v>
+        <v>582</v>
       </c>
       <c r="C200" s="1" t="s">
-        <v>571</v>
+        <v>569</v>
       </c>
     </row>
     <row r="201" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A201" s="2" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="B201" s="2" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="C201" s="2" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="202" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A202" s="2" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="B202" s="2" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="C202" s="3" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
     </row>
     <row r="203" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A203" s="2" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="B203" s="2" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="C203" s="3" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
     </row>
     <row r="204" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A204" s="2" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
       <c r="B204" s="2" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
       <c r="C204" s="2" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
     </row>
     <row r="205" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A205" s="2" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="B205" s="2" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="C205" s="3" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
     </row>
     <row r="206" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A206" s="2" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="B206" s="2" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="C206" s="2" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
     </row>
     <row r="207" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A207" s="2" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="B207" s="2" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="C207" s="2" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
     </row>
     <row r="208" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A208" s="2" t="s">
+        <v>462</v>
+      </c>
+      <c r="B208" s="2" t="s">
         <v>464</v>
       </c>
-      <c r="B208" s="2" t="s">
-        <v>466</v>
-      </c>
       <c r="C208" s="2" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
     </row>
     <row r="209" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A209" s="2" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="B209" s="2" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="C209" s="2" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
     </row>
     <row r="210" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A210" s="2" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="B210" s="2" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="C210" s="2" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
     </row>
     <row r="211" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A211" s="2" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="B211" s="2" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="C211" s="3" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
     </row>
     <row r="212" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A212" s="2" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="B212" s="2" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="C212" s="3" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
     </row>
     <row r="213" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A213" s="2" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="B213" s="2" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="C213" s="2" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
     </row>
     <row r="214" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A214" s="2" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="B214" s="2" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="C214" s="3" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
     </row>
     <row r="215" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A215" s="2" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="B215" s="2" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="C215" s="3" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
     </row>
     <row r="216" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A216" s="2" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
       <c r="B216" s="2" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="C216" s="2" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
     </row>
     <row r="217" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A217" s="2" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="B217" s="2" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="C217" s="2" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
     </row>
     <row r="218" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A218" s="2" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="B218" s="2" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="C218" s="3" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
     </row>
     <row r="219" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A219" s="2" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="B219" s="2" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="C219" s="3" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
     </row>
     <row r="220" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A220" s="2" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="B220" s="2" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="C220" s="2" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
     </row>
     <row r="221" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A221" s="2" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="B221" s="2" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="C221" s="3" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
     </row>
     <row r="222" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A222" s="2" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="B222" s="2" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="C222" s="3" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
     </row>
     <row r="223" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A223" s="1" t="s">
+        <v>436</v>
+      </c>
+      <c r="B223" s="1" t="s">
         <v>438</v>
       </c>
-      <c r="B223" s="1" t="s">
-        <v>440</v>
-      </c>
       <c r="C223" s="1" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
     </row>
     <row r="224" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A224" s="1" t="s">
+        <v>437</v>
+      </c>
+      <c r="B224" s="1" t="s">
         <v>439</v>
       </c>
-      <c r="B224" s="1" t="s">
-        <v>441</v>
-      </c>
       <c r="C224" s="1" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
     </row>
     <row r="225" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A225" s="1" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
       <c r="B225" s="1" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
       <c r="C225" s="1" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
     </row>
     <row r="226" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A226" s="2" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="B226" s="2" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="C226" s="3" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
     </row>
     <row r="227" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A227" s="2" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="B227" s="2" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="C227" s="2" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
     </row>
     <row r="228" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A228" s="2" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="B228" s="2" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="C228" s="2" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
     </row>
     <row r="229" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A229" s="1" t="s">
-        <v>567</v>
+        <v>565</v>
       </c>
       <c r="B229" s="1" t="s">
-        <v>586</v>
+        <v>584</v>
       </c>
       <c r="C229" s="1" t="s">
-        <v>567</v>
+        <v>565</v>
       </c>
     </row>
     <row r="230" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A230" s="2" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="B230" s="2" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="C230" s="2" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
     </row>
     <row r="231" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A231" s="1" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
       <c r="B231" s="2" t="s">
-        <v>545</v>
+        <v>543</v>
       </c>
       <c r="C231" s="1" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
     </row>
     <row r="232" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A232" s="1" t="s">
-        <v>576</v>
+        <v>574</v>
       </c>
       <c r="B232" s="1" t="s">
-        <v>580</v>
+        <v>578</v>
       </c>
       <c r="C232" s="1" t="s">
-        <v>576</v>
+        <v>574</v>
       </c>
     </row>
     <row r="233" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A233" s="2" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="B233" s="2" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="C233" s="3" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
     </row>
     <row r="234" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A234" s="2" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="B234" s="2" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="C234" s="2" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
     </row>
     <row r="235" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A235" s="2" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="B235" s="2" t="s">
-        <v>557</v>
+        <v>555</v>
       </c>
       <c r="C235" s="2" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
     </row>
     <row r="236" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A236" s="1" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="B236" s="2" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="C236" s="1" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
     </row>
     <row r="237" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A237" s="2" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="B237" s="2" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="C237" s="3" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
     </row>
     <row r="238" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A238" s="2" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="B238" s="2" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="C238" s="2" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
     </row>
     <row r="239" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A239" s="2" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="B239" s="2" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="C239" s="3" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
     </row>
     <row r="240" spans="1:3" x14ac:dyDescent="0.45">
@@ -4823,90 +4823,90 @@
     </row>
     <row r="241" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A241" s="2" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
       <c r="B241" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C241" s="2" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
     </row>
     <row r="242" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A242" s="2" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="B242" s="2" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="C242" s="3" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
     </row>
     <row r="243" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A243" s="1" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
       <c r="B243" s="2" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
       <c r="C243" s="1" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
     </row>
     <row r="244" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A244" s="2" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="B244" s="2" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="C244" s="2" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
     </row>
     <row r="245" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A245" s="2" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="B245" s="2" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="C245" s="3" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
     </row>
     <row r="246" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A246" s="1" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
       <c r="B246" s="2" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
       <c r="C246" s="1" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
     </row>
     <row r="247" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A247" s="1" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="B247" s="2" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="C247" s="1" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
     </row>
     <row r="248" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A248" s="2" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="B248" s="2" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="C248" s="3" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
     </row>
     <row r="249" spans="1:3" x14ac:dyDescent="0.45">
@@ -4922,310 +4922,310 @@
     </row>
     <row r="250" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A250" s="2" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="B250" s="2" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="C250" s="2" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
     </row>
     <row r="251" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A251" s="2" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="B251" s="2" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="C251" s="3" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
     </row>
     <row r="252" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A252" s="2" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="B252" s="2" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="C252" s="3" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
     </row>
     <row r="253" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A253" s="2" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="B253" s="2" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="C253" s="3" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
     </row>
     <row r="254" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A254" s="2" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="B254" s="2" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="C254" s="3" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
     </row>
     <row r="255" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A255" s="2" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="B255" s="2" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="C255" s="3" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
     </row>
     <row r="256" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A256" s="2" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="B256" s="2" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="C256" s="3" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
     </row>
     <row r="257" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A257" s="2" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="B257" s="2" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="C257" s="3" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
     </row>
     <row r="258" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A258" s="2" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="B258" s="2" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="C258" s="3" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
     </row>
     <row r="259" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A259" s="2" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="B259" s="2" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="C259" s="2" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
     </row>
     <row r="260" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A260" s="1" t="s">
-        <v>551</v>
+        <v>549</v>
       </c>
       <c r="B260" s="1" t="s">
-        <v>550</v>
+        <v>548</v>
       </c>
       <c r="C260" s="1" t="s">
-        <v>551</v>
+        <v>549</v>
       </c>
     </row>
     <row r="261" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A261" s="1" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="B261" s="2" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="C261" s="1" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
     </row>
     <row r="262" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A262" s="2" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="B262" s="2" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="C262" s="3" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
     </row>
     <row r="263" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A263" s="1" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
       <c r="B263" s="2" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
       <c r="C263" s="1" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
     </row>
     <row r="264" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A264" s="2" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="B264" s="2" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="C264" s="3" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
     </row>
     <row r="265" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A265" s="1" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
       <c r="B265" s="2" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
       <c r="C265" s="1" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
     </row>
     <row r="266" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A266" s="1" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="B266" s="1" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="C266" s="1" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
     </row>
     <row r="267" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A267" s="1" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="B267" s="2" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="C267" s="1" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
     </row>
     <row r="268" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A268" s="1" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
       <c r="B268" s="2" t="s">
-        <v>549</v>
+        <v>547</v>
       </c>
       <c r="C268" s="1" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
     </row>
     <row r="269" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A269" s="2" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="B269" s="2" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="C269" s="3" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
     </row>
     <row r="270" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A270" s="1" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
       <c r="B270" s="2" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
       <c r="C270" s="1" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
     </row>
     <row r="271" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A271" s="2" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="B271" s="2" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="C271" s="3" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
     </row>
     <row r="272" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A272" s="2" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="B272" s="2" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="C272" s="3" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
     </row>
     <row r="273" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A273" s="2" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="B273" s="2" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="C273" s="3" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
     </row>
     <row r="274" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A274" s="1" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="B274" s="2" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="C274" s="1" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
     </row>
     <row r="275" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A275" s="2" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="B275" s="2" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="C275" s="2" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
     </row>
     <row r="276" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A276" s="2" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="B276" s="2" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="C276" s="2" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
     </row>
     <row r="277" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A277" s="2" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="B277" s="2" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="C277" s="3" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
     </row>
     <row r="278" spans="1:3" x14ac:dyDescent="0.45">
@@ -5241,266 +5241,266 @@
     </row>
     <row r="279" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A279" s="1" t="s">
-        <v>565</v>
+        <v>563</v>
       </c>
       <c r="B279" s="2" t="s">
-        <v>589</v>
+        <v>587</v>
       </c>
       <c r="C279" s="1" t="s">
-        <v>565</v>
+        <v>563</v>
       </c>
     </row>
     <row r="280" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A280" s="1" t="s">
-        <v>564</v>
+        <v>562</v>
       </c>
       <c r="B280" s="2" t="s">
-        <v>588</v>
+        <v>586</v>
       </c>
       <c r="C280" s="1" t="s">
-        <v>564</v>
+        <v>562</v>
       </c>
     </row>
     <row r="281" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A281" s="1" t="s">
-        <v>574</v>
+        <v>572</v>
       </c>
       <c r="B281" s="1" t="s">
-        <v>581</v>
+        <v>579</v>
       </c>
       <c r="C281" s="1" t="s">
-        <v>574</v>
+        <v>572</v>
       </c>
     </row>
     <row r="282" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A282" s="2" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="B282" s="2" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="C282" s="2" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
     </row>
     <row r="283" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A283" s="2" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="B283" s="2" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="C283" s="3" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
     </row>
     <row r="284" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A284" s="2" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="B284" s="2" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="C284" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="285" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A285" s="2" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="B285" s="2" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="C285" s="2" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
     </row>
     <row r="286" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A286" s="1" t="s">
+        <v>443</v>
+      </c>
+      <c r="B286" s="1" t="s">
         <v>445</v>
       </c>
-      <c r="B286" s="1" t="s">
-        <v>447</v>
-      </c>
       <c r="C286" s="1" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
     </row>
     <row r="287" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A287" s="2" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="B287" s="2" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="C287" s="3" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
     </row>
     <row r="288" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A288" s="2" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="B288" s="2" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="C288" s="2" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
     </row>
     <row r="289" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A289" s="2" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="B289" s="2" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="C289" s="2" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
     </row>
     <row r="290" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A290" s="2" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="B290" s="2" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="C290" s="3" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
     </row>
     <row r="291" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A291" s="2" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="B291" s="2" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="C291" s="2" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
     </row>
     <row r="292" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A292" s="2" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="B292" s="2" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="C292" s="2" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
     </row>
     <row r="293" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A293" s="1" t="s">
-        <v>572</v>
+        <v>570</v>
       </c>
       <c r="B293" s="1" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="C293" s="1" t="s">
-        <v>572</v>
+        <v>570</v>
       </c>
     </row>
     <row r="294" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A294" s="1" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="B294" s="2" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
       <c r="C294" s="1" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
     </row>
     <row r="295" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A295" s="1" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="B295" s="2" t="s">
-        <v>518</v>
+        <v>516</v>
       </c>
       <c r="C295" s="1" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
     </row>
     <row r="296" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A296" s="1" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
       <c r="B296" s="2" t="s">
-        <v>517</v>
+        <v>515</v>
       </c>
       <c r="C296" s="1" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
     </row>
     <row r="297" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A297" s="2" t="s">
-        <v>554</v>
+        <v>552</v>
       </c>
       <c r="B297" s="2" t="s">
-        <v>555</v>
+        <v>553</v>
       </c>
       <c r="C297" s="3" t="s">
-        <v>554</v>
+        <v>552</v>
       </c>
     </row>
     <row r="298" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A298" s="2" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="B298" s="2" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="C298" s="3" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
     </row>
     <row r="299" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A299" s="2" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="B299" s="2" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="C299" s="3" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
     </row>
     <row r="300" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A300" s="2" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="B300" s="2" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="C300" s="2" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
     </row>
     <row r="301" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A301" s="1" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
       <c r="B301" s="1" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
       <c r="C301" s="1" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
     </row>
     <row r="302" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A302" s="2" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="B302" s="2" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="C302" s="3" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update for translation, locale for plotly
</commit_message>
<xml_diff>
--- a/translations/source.xlsx
+++ b/translations/source.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/e6c7874704bc5dfb/Documents/R Studio/DataSuite/translations/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="307" documentId="8_{D77EC384-F39F-4BA6-8963-4B8AF986F7DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{30483F88-0505-4FC6-9117-702E1F25928B}"/>
+  <xr:revisionPtr revIDLastSave="311" documentId="8_{D77EC384-F39F-4BA6-8963-4B8AF986F7DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{408B36C7-CFA6-44D5-91EB-6FC5401CED67}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="16395" xr2:uid="{BD840C99-A56D-4EBC-B1B7-A6018ADC22A6}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="604" uniqueCount="592">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="610" uniqueCount="598">
   <si>
     <t>English</t>
   </si>
@@ -1810,6 +1810,24 @@
   </si>
   <si>
     <t>en</t>
+  </si>
+  <si>
+    <t>Таблицы частот</t>
+  </si>
+  <si>
+    <t>Проверка нормальности</t>
+  </si>
+  <si>
+    <t>Графики разброса</t>
+  </si>
+  <si>
+    <t>Frequency tables</t>
+  </si>
+  <si>
+    <t>Normality testing</t>
+  </si>
+  <si>
+    <t>Scatterplots</t>
   </si>
 </sst>
 </file>
@@ -1863,6 +1881,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2162,10 +2184,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C853ECA4-158B-4D85-A448-9ECE56776B5F}">
-  <dimension ref="A1:B302"/>
+  <dimension ref="A1:B305"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" topLeftCell="A277" workbookViewId="0">
+      <selection activeCell="B303" sqref="B303"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -4590,6 +4612,30 @@
         <v>339</v>
       </c>
     </row>
+    <row r="303" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A303" t="s">
+        <v>592</v>
+      </c>
+      <c r="B303" t="s">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="304" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A304" t="s">
+        <v>593</v>
+      </c>
+      <c r="B304" t="s">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="305" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A305" t="s">
+        <v>594</v>
+      </c>
+      <c r="B305" t="s">
+        <v>597</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:B1" xr:uid="{56EE5BC3-7B0A-4577-92C7-56F73F7DDC8B}">
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B302">

</xml_diff>